<commit_message>
fix local condition expiration, fix bind and silence, and null reference when setting condition cooldown
</commit_message>
<xml_diff>
--- a/Dictionaries/store.xlsx
+++ b/Dictionaries/store.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="299">
   <si>
     <t>id</t>
   </si>
@@ -29,12 +29,57 @@
     <t>bundle_abondiasBest</t>
   </si>
   <si>
+    <t>silver1</t>
+  </si>
+  <si>
+    <t>silver2</t>
+  </si>
+  <si>
     <t>bundle_sapphosChoice</t>
   </si>
   <si>
+    <t>silver3</t>
+  </si>
+  <si>
+    <t>silver4</t>
+  </si>
+  <si>
     <t>bundle_hermeticCollection</t>
   </si>
   <si>
+    <t>consumable_alignmentBoosterSmaller</t>
+  </si>
+  <si>
+    <t>silver5</t>
+  </si>
+  <si>
+    <t>consumable_alignmentBoosterMedium</t>
+  </si>
+  <si>
+    <t>silver6</t>
+  </si>
+  <si>
+    <t>consumable_alignmentBoosterGreater</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterSmaller</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterMedium</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterGreater</t>
+  </si>
+  <si>
+    <t>consumable_invisible</t>
+  </si>
+  <si>
+    <t>consumable_truesight</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_HHO</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_WENDIGO</t>
   </si>
   <si>
@@ -47,69 +92,45 @@
     <t>shop_locked_barg</t>
   </si>
   <si>
-    <t>consumable_alignmentBoosterSmaller</t>
-  </si>
-  <si>
-    <t>silver1</t>
-  </si>
-  <si>
-    <t>consumable_alignmentBoosterMedium</t>
-  </si>
-  <si>
-    <t>silver2</t>
-  </si>
-  <si>
-    <t>consumable_alignmentBoosterGreater</t>
-  </si>
-  <si>
-    <t>silver3</t>
-  </si>
-  <si>
-    <t>consumable_xpBoosterSmaller</t>
-  </si>
-  <si>
-    <t>silver4</t>
-  </si>
-  <si>
-    <t>silver5</t>
-  </si>
-  <si>
-    <t>consumable_xpBoosterMedium</t>
-  </si>
-  <si>
-    <t>silver6</t>
-  </si>
-  <si>
-    <t>consumable_xpBoosterGreater</t>
-  </si>
-  <si>
-    <t>consumable_invisible</t>
-  </si>
-  <si>
-    <t>consumable_truesight</t>
-  </si>
-  <si>
     <t>cosmetic_f_PF_CATSIDHE</t>
   </si>
   <si>
+    <t>cosmetic_f_S_HKO</t>
+  </si>
+  <si>
     <t>shop_locked_sidh</t>
   </si>
   <si>
     <t>cosmetic_f_PF_GRINDYLOW</t>
   </si>
   <si>
+    <t>cosmetic_f_S_HLO</t>
+  </si>
+  <si>
     <t>shop_locked_grdlw</t>
   </si>
   <si>
+    <t>cosmetic_f_S_SNOWQUEEN</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_SENTINALOWL</t>
   </si>
   <si>
     <t>shop_locked_owl</t>
   </si>
   <si>
+    <t>cosmetic_f_S_LILYOV</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_MIDSUMMER</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_DWO</t>
   </si>
   <si>
+    <t>cosmetic_f_S_THUNDERMOON</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_HDWO</t>
   </si>
   <si>
@@ -119,57 +140,87 @@
     <t>cosmetic_f_HE_HBO</t>
   </si>
   <si>
+    <t>cosmetic_f_S_ECLIPSE</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_HHO</t>
   </si>
   <si>
     <t>cosmetic_f_HE_HNO</t>
   </si>
   <si>
+    <t>cosmetic_f_S_CORNMOON</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_CEH</t>
   </si>
   <si>
+    <t>cosmetic_f_S_BRNNGWTCH</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_CES</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HHO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_HKO</t>
+    <t>cosmetic_f_S_CALYPSO</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_HKO</t>
   </si>
   <si>
     <t>cosmetic_f_HE_FLOWER</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HLO</t>
+    <t>cosmetic_m_S_HHO</t>
   </si>
   <si>
     <t>cosmetic_f_HE_BDH</t>
   </si>
   <si>
+    <t>cosmetic_m_S_HLO</t>
+  </si>
+  <si>
     <t>shop_locked_rrc</t>
   </si>
   <si>
-    <t>cosmetic_f_S_SNOWQUEEN</t>
+    <t>cosmetic_m_S_JACKFROST</t>
   </si>
   <si>
     <t>cosmetic_f_HA_DWO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_LILYOV</t>
+    <t>cosmetic_m_S_MIDSUMMER</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_CORNMOON</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_CALYPSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_FIREDANCER</t>
   </si>
   <si>
     <t>cosmetic_f_HA_FKFO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_MIDSUMMER</t>
+    <t>cosmetic_m_S_BRNNGWTCH</t>
   </si>
   <si>
     <t>cosmetic_f_HA_KSO</t>
   </si>
   <si>
+    <t>cosmetic_m_S_ECLIPSE</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_CGH</t>
   </si>
   <si>
+    <t>cosmetic_m_S_THUNDERMOON</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_PNY</t>
   </si>
   <si>
@@ -248,42 +299,27 @@
     <t>cosmetic_f_C_WBYE</t>
   </si>
   <si>
-    <t>cosmetic_f_S_THUNDERMOON</t>
-  </si>
-  <si>
     <t>cosmetic_f_C_WITCHCO</t>
   </si>
   <si>
     <t>cosmetic_f_C_MAGICINK</t>
   </si>
   <si>
-    <t>cosmetic_f_S_ECLIPSE</t>
-  </si>
-  <si>
     <t>cosmetic_f_WL_DWO</t>
   </si>
   <si>
     <t>cosmetic_f_WL_KFO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_CORNMOON</t>
-  </si>
-  <si>
     <t>cosmetic_f_WR_DWO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_BRNNGWTCH</t>
-  </si>
-  <si>
     <t>cosmetic_f_WR_KFO</t>
   </si>
   <si>
     <t>cosmetic_f_H_DWO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_CALYPSO</t>
-  </si>
-  <si>
     <t>cosmetic_f_H_BH</t>
   </si>
   <si>
@@ -513,6 +549,369 @@
   </si>
   <si>
     <t>cosmetic_f_SC_SUN</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_CES</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_DTO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_F_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_HSS</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_HST</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SA_TRIBE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_HBH</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_GLSS</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_HDWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_CGH</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_CEH</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_DSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_N_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_FR_HSR</t>
+  </si>
+  <si>
+    <t>cosmetic_m_WR_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_FR_HGR</t>
+  </si>
+  <si>
+    <t>cosmetic_m_WL_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_F_DSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_F_CHFO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_F_DTO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_DBB</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_HST</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_HBT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_DBM</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_HAT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_F_HFO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_HFT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_JET</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SA_JDT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_JSET</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_HSF</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SA_HWT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_HRT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SA_JWT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SA_FLWR</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_HMT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_JBT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SA_JGT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_F_SANDALS</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_CROWN</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_HOOD</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_GOATEE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_GLSS</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_WITCHCO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_SSBUTTON</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_MAGICINK</t>
+  </si>
+  <si>
+    <t>cosmetic_m_L_TRAVEL</t>
+  </si>
+  <si>
+    <t>cosmetic_m_L_SHORTS</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_HNO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_DSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_OPEN</t>
+  </si>
+  <si>
+    <t>cosmetic_m_WR_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_L_DSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_L_PUFF</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_SPARSEMUSTACHE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_DTO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_WBYE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_H_BH</t>
+  </si>
+  <si>
+    <t>cosmetic_m_L_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_L_DTO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_L_LOOSE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_BRDPNY</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_BKSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_HFO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_ANCHORBEARD</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_SPARSEBEARD</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_ZEFRON</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_WL_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_TUNIC</t>
+  </si>
+  <si>
+    <t>cosmetic_m_FL_HFR</t>
+  </si>
+  <si>
+    <t>cosmetic_m_L_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_L_HFO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_BUTTERFLY</t>
+  </si>
+  <si>
+    <t>cosmetic_m_PF_SENTINALOWL</t>
+  </si>
+  <si>
+    <t>cosmetic_m_PF_WENDIGO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_LT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_N_WOLFAMULET</t>
+  </si>
+  <si>
+    <t>cosmetic_m_PF_BARGHEST</t>
+  </si>
+  <si>
+    <t>cosmetic_m_PF_GRINDYLOW</t>
+  </si>
+  <si>
+    <t>cosmetic_m_PF_CATSIDHE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_BIRDSKULL</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HE_BDH</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_LNG</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_BUN</t>
+  </si>
+  <si>
+    <t>cosmetic_m_CL_KIM</t>
+  </si>
+  <si>
+    <t>cosmetic_m_HA_AFRO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_N_CROWAMULET</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_PC</t>
+  </si>
+  <si>
+    <t>cosmetic_m_C_TT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_PYRAMIDS</t>
+  </si>
+  <si>
+    <t>cosmetic_m_CL_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_CL_SMMRSOL</t>
+  </si>
+  <si>
+    <t>cosmetic_m_CL_DTO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_CL_GRAY</t>
+  </si>
+  <si>
+    <t>cosmetic_m_F_STRAPPEDSHOES</t>
+  </si>
+  <si>
+    <t>cosmetic_m_CL_DSO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_CL_PRIMAVERA</t>
+  </si>
+  <si>
+    <t>cosmetic_m_CL_SHADOW</t>
+  </si>
+  <si>
+    <t>cosmetic_m_CL_WHITE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_BALLET</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SF_SUNGLASSES</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_CROWSKULL</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_BIRDCAGE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_UNICORN</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_SPIDER</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_MOLOTOV</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_COFFIN</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SA_LEOPARD</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_ELEPHANT</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_JOKER</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_COUPLE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_SUN</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SS_PUPPET</t>
+  </si>
+  <si>
+    <t>cosmetic_m_SC_ASTRONAUT</t>
   </si>
 </sst>
 </file>
@@ -641,7 +1040,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -651,7 +1050,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -817,7 +1216,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -827,7 +1226,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -837,7 +1236,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -847,7 +1246,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -857,7 +1256,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -953,7 +1352,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -963,7 +1362,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -973,7 +1372,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -983,7 +1382,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -993,7 +1392,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1003,7 +1402,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1115,13 +1514,13 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="3"/>
@@ -1129,13 +1528,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="3"/>
@@ -1143,13 +1542,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="3"/>
@@ -1157,13 +1556,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="3"/>
@@ -1171,13 +1570,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="3"/>
@@ -1185,7 +1584,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1195,7 +1594,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1205,7 +1604,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1215,7 +1614,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1225,7 +1624,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1235,7 +1634,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1245,7 +1644,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1255,7 +1654,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1265,7 +1664,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1275,11 +1674,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
@@ -1287,7 +1686,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1297,7 +1696,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1307,7 +1706,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1317,7 +1716,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1327,7 +1726,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1337,7 +1736,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1347,7 +1746,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1357,7 +1756,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1367,7 +1766,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1377,7 +1776,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1387,7 +1786,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1397,7 +1796,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1407,7 +1806,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1417,7 +1816,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1427,7 +1826,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1437,7 +1836,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1447,7 +1846,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1457,7 +1856,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1467,7 +1866,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1477,7 +1876,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1487,7 +1886,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1497,7 +1896,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1507,7 +1906,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1517,7 +1916,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1527,7 +1926,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1537,7 +1936,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1547,7 +1946,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1557,7 +1956,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1567,7 +1966,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1577,7 +1976,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1587,7 +1986,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1597,7 +1996,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1607,7 +2006,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1617,7 +2016,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1627,7 +2026,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1637,7 +2036,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1647,7 +2046,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1657,7 +2056,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1667,7 +2066,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1677,7 +2076,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1687,7 +2086,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1697,7 +2096,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1707,7 +2106,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1717,7 +2116,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1727,7 +2126,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1737,7 +2136,7 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1747,7 +2146,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1757,7 +2156,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1767,7 +2166,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1777,7 +2176,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1787,7 +2186,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1797,7 +2196,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1807,7 +2206,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1817,7 +2216,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1827,7 +2226,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1837,7 +2236,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1847,7 +2246,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1857,7 +2256,7 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1867,7 +2266,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1877,7 +2276,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1887,11 +2286,11 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="3"/>
@@ -1899,11 +2298,11 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="3"/>
@@ -1911,11 +2310,11 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="3"/>
@@ -1923,7 +2322,7 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1933,13 +2332,13 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B81" s="1">
         <v>1.5646176E12</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="3"/>
@@ -1947,7 +2346,7 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1957,11 +2356,11 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="3"/>
@@ -1969,11 +2368,11 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="3"/>
@@ -1981,11 +2380,11 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="3"/>
@@ -1993,7 +2392,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2003,7 +2402,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2013,7 +2412,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2023,7 +2422,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2033,7 +2432,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2043,7 +2442,7 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2053,7 +2452,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2063,7 +2462,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2073,7 +2472,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2083,7 +2482,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2093,7 +2492,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2103,7 +2502,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2113,7 +2512,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2123,7 +2522,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2133,7 +2532,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2143,7 +2542,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2153,7 +2552,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2163,7 +2562,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2173,7 +2572,7 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2183,7 +2582,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2193,7 +2592,7 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2203,7 +2602,7 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2213,7 +2612,7 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2223,7 +2622,7 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2233,7 +2632,7 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2243,7 +2642,7 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2253,7 +2652,7 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2263,7 +2662,7 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2273,7 +2672,7 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2283,7 +2682,7 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2293,13 +2692,13 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="B116" s="1">
         <v>1.5667056E12</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="3"/>
@@ -2307,13 +2706,13 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="B117" s="1">
         <v>1.5667056E12</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="3"/>
@@ -2321,13 +2720,13 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="B118" s="1">
         <v>1.5667056E12</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="3"/>
@@ -2335,13 +2734,13 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="B119" s="1">
         <v>1.5667056E12</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="3"/>
@@ -2349,13 +2748,13 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="B120" s="1">
         <v>1.5667056E12</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="3"/>
@@ -2363,13 +2762,13 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="B121" s="1">
         <v>1.5667056E12</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="3"/>
@@ -2377,13 +2776,13 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="B122" s="1">
         <v>1.5667056E12</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="3"/>
@@ -2391,13 +2790,13 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="B123" s="1">
         <v>1.5667056E12</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="3"/>
@@ -2405,20 +2804,1256 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="B124" s="1">
         <v>1.5667056E12</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="3"/>
       <c r="F124" s="1"/>
     </row>
+    <row r="125">
+      <c r="A125" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="1"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="1"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="1"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="1"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="1"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="1"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="1"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="1"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="1"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="1"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="1"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="1"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="1"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="1"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="3"/>
+      <c r="F139" s="1"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="1"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="1"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B142" s="1"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="1"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+      <c r="E143" s="3"/>
+      <c r="F143" s="1"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="1"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B145" s="1"/>
+      <c r="C145" s="1"/>
+      <c r="D145" s="1"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="1"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="1"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="3"/>
+      <c r="F147" s="1"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B148" s="1"/>
+      <c r="C148" s="1"/>
+      <c r="D148" s="1"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="1"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="1"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="1"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="3"/>
+      <c r="F151" s="1"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="1"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B153" s="1"/>
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+      <c r="E153" s="3"/>
+      <c r="F153" s="1"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B154" s="1"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="1"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="1"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="3"/>
+      <c r="F156" s="1"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="1"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="1"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1"/>
+      <c r="E159" s="3"/>
+      <c r="F159" s="1"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="1"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+      <c r="E161" s="3"/>
+      <c r="F161" s="1"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="1"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="3"/>
+      <c r="F163" s="1"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="3"/>
+      <c r="F164" s="1"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="3"/>
+      <c r="F165" s="1"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="3"/>
+      <c r="F166" s="1"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="3"/>
+      <c r="F167" s="1"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="3"/>
+      <c r="F168" s="1"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="3"/>
+      <c r="F169" s="1"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="1"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="3"/>
+      <c r="F171" s="1"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="3"/>
+      <c r="F172" s="1"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="3"/>
+      <c r="F173" s="1"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="3"/>
+      <c r="F174" s="1"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="3"/>
+      <c r="F175" s="1"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="3"/>
+      <c r="F176" s="1"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="3"/>
+      <c r="F177" s="1"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="3"/>
+      <c r="F178" s="1"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="3"/>
+      <c r="F179" s="1"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="1"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="3"/>
+      <c r="F181" s="1"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B182" s="1"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="1"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="1"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+      <c r="D183" s="1"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="1"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
+      <c r="D184" s="1"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="1"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+      <c r="D185" s="1"/>
+      <c r="E185" s="3"/>
+      <c r="F185" s="1"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B186" s="1"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="1"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B187" s="1"/>
+      <c r="C187" s="1"/>
+      <c r="D187" s="1"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="1"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B188" s="1"/>
+      <c r="C188" s="1"/>
+      <c r="D188" s="1"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="1"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B189" s="1"/>
+      <c r="C189" s="1"/>
+      <c r="D189" s="1"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="1"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B190" s="1"/>
+      <c r="C190" s="1"/>
+      <c r="D190" s="1"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="1"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B191" s="1"/>
+      <c r="C191" s="1"/>
+      <c r="D191" s="1"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="1"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B192" s="1"/>
+      <c r="C192" s="1"/>
+      <c r="D192" s="1"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="1"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
+      <c r="D193" s="1"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="1"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B194" s="1"/>
+      <c r="C194" s="1"/>
+      <c r="D194" s="1"/>
+      <c r="E194" s="3"/>
+      <c r="F194" s="1"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B195" s="1"/>
+      <c r="C195" s="1"/>
+      <c r="D195" s="1"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="1"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B196" s="1"/>
+      <c r="C196" s="1"/>
+      <c r="D196" s="1"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="1"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B197" s="1"/>
+      <c r="C197" s="1"/>
+      <c r="D197" s="1"/>
+      <c r="E197" s="3"/>
+      <c r="F197" s="1"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B198" s="1"/>
+      <c r="C198" s="1"/>
+      <c r="D198" s="1"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="1"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B199" s="1"/>
+      <c r="C199" s="1"/>
+      <c r="D199" s="1"/>
+      <c r="E199" s="3"/>
+      <c r="F199" s="1"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B200" s="1"/>
+      <c r="C200" s="1"/>
+      <c r="D200" s="1"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="1"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B201" s="1"/>
+      <c r="C201" s="1"/>
+      <c r="D201" s="1"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="1"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B202" s="1"/>
+      <c r="C202" s="1"/>
+      <c r="D202" s="1"/>
+      <c r="E202" s="3"/>
+      <c r="F202" s="1"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B203" s="1"/>
+      <c r="C203" s="1"/>
+      <c r="D203" s="1"/>
+      <c r="E203" s="3"/>
+      <c r="F203" s="1"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B204" s="1"/>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+      <c r="E204" s="3"/>
+      <c r="F204" s="1"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+      <c r="D205" s="1"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="1"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B206" s="1"/>
+      <c r="C206" s="1"/>
+      <c r="D206" s="1"/>
+      <c r="E206" s="3"/>
+      <c r="F206" s="1"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B207" s="1"/>
+      <c r="C207" s="1"/>
+      <c r="D207" s="1"/>
+      <c r="E207" s="3"/>
+      <c r="F207" s="1"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B208" s="1"/>
+      <c r="C208" s="1"/>
+      <c r="D208" s="1"/>
+      <c r="E208" s="3"/>
+      <c r="F208" s="1"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B209" s="1"/>
+      <c r="C209" s="1"/>
+      <c r="D209" s="1"/>
+      <c r="E209" s="3"/>
+      <c r="F209" s="1"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B210" s="1"/>
+      <c r="C210" s="1"/>
+      <c r="D210" s="1"/>
+      <c r="E210" s="3"/>
+      <c r="F210" s="1"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B211" s="1"/>
+      <c r="C211" s="1"/>
+      <c r="D211" s="1"/>
+      <c r="E211" s="3"/>
+      <c r="F211" s="1"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B212" s="1"/>
+      <c r="C212" s="1"/>
+      <c r="D212" s="1"/>
+      <c r="E212" s="3"/>
+      <c r="F212" s="1"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B213" s="1"/>
+      <c r="C213" s="1"/>
+      <c r="D213" s="1"/>
+      <c r="E213" s="3"/>
+      <c r="F213" s="1"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B214" s="1"/>
+      <c r="C214" s="1"/>
+      <c r="D214" s="1"/>
+      <c r="E214" s="3"/>
+      <c r="F214" s="1"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B215" s="1"/>
+      <c r="C215" s="1"/>
+      <c r="D215" s="1"/>
+      <c r="E215" s="3"/>
+      <c r="F215" s="1"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B216" s="1"/>
+      <c r="C216" s="1"/>
+      <c r="D216" s="1"/>
+      <c r="E216" s="3"/>
+      <c r="F216" s="1"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B217" s="1"/>
+      <c r="C217" s="1"/>
+      <c r="D217" s="1"/>
+      <c r="E217" s="3"/>
+      <c r="F217" s="1"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B218" s="1"/>
+      <c r="C218" s="1"/>
+      <c r="D218" s="1"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="1"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B219" s="1"/>
+      <c r="C219" s="1"/>
+      <c r="D219" s="1"/>
+      <c r="E219" s="3"/>
+      <c r="F219" s="1"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B220" s="1"/>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="1"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B221" s="1"/>
+      <c r="C221" s="1"/>
+      <c r="D221" s="1"/>
+      <c r="E221" s="3"/>
+      <c r="F221" s="1"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B222" s="1"/>
+      <c r="C222" s="1"/>
+      <c r="D222" s="1"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="1"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
+      <c r="D223" s="1"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="1"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B224" s="1"/>
+      <c r="C224" s="1"/>
+      <c r="D224" s="1"/>
+      <c r="E224" s="3"/>
+      <c r="F224" s="1"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B225" s="1"/>
+      <c r="C225" s="1"/>
+      <c r="D225" s="1"/>
+      <c r="E225" s="3"/>
+      <c r="F225" s="1"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B226" s="1"/>
+      <c r="C226" s="1"/>
+      <c r="D226" s="1"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="1"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B227" s="1"/>
+      <c r="C227" s="1"/>
+      <c r="D227" s="1"/>
+      <c r="E227" s="3"/>
+      <c r="F227" s="1"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B228" s="1"/>
+      <c r="C228" s="1"/>
+      <c r="D228" s="1"/>
+      <c r="E228" s="3"/>
+      <c r="F228" s="1"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B229" s="1"/>
+      <c r="C229" s="1"/>
+      <c r="D229" s="1"/>
+      <c r="E229" s="3"/>
+      <c r="F229" s="1"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B230" s="1"/>
+      <c r="C230" s="1"/>
+      <c r="D230" s="1"/>
+      <c r="E230" s="3"/>
+      <c r="F230" s="1"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B231" s="1"/>
+      <c r="C231" s="1"/>
+      <c r="D231" s="1"/>
+      <c r="E231" s="3"/>
+      <c r="F231" s="1"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B232" s="1"/>
+      <c r="C232" s="1"/>
+      <c r="D232" s="1"/>
+      <c r="E232" s="3"/>
+      <c r="F232" s="1"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B233" s="1"/>
+      <c r="C233" s="1"/>
+      <c r="D233" s="1"/>
+      <c r="E233" s="3"/>
+      <c r="F233" s="1"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B234" s="1"/>
+      <c r="C234" s="1"/>
+      <c r="D234" s="1"/>
+      <c r="E234" s="3"/>
+      <c r="F234" s="1"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B235" s="1"/>
+      <c r="C235" s="1"/>
+      <c r="D235" s="1"/>
+      <c r="E235" s="3"/>
+      <c r="F235" s="1"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B236" s="1"/>
+      <c r="C236" s="1"/>
+      <c r="D236" s="1"/>
+      <c r="E236" s="3"/>
+      <c r="F236" s="1"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B237" s="1"/>
+      <c r="C237" s="1"/>
+      <c r="D237" s="1"/>
+      <c r="E237" s="3"/>
+      <c r="F237" s="1"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B238" s="1"/>
+      <c r="C238" s="1"/>
+      <c r="D238" s="1"/>
+      <c r="E238" s="3"/>
+      <c r="F238" s="1"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B239" s="1"/>
+      <c r="C239" s="1"/>
+      <c r="D239" s="1"/>
+      <c r="E239" s="3"/>
+      <c r="F239" s="1"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B240" s="1"/>
+      <c r="C240" s="1"/>
+      <c r="D240" s="1"/>
+      <c r="E240" s="3"/>
+      <c r="F240" s="1"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B241" s="1"/>
+      <c r="C241" s="1"/>
+      <c r="D241" s="1"/>
+      <c r="E241" s="3"/>
+      <c r="F241" s="1"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B242" s="1"/>
+      <c r="C242" s="1"/>
+      <c r="D242" s="1"/>
+      <c r="E242" s="3"/>
+      <c r="F242" s="1"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B243" s="1"/>
+      <c r="C243" s="1"/>
+      <c r="D243" s="1"/>
+      <c r="E243" s="3"/>
+      <c r="F243" s="1"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B244" s="1"/>
+      <c r="C244" s="1"/>
+      <c r="D244" s="1"/>
+      <c r="E244" s="3"/>
+      <c r="F244" s="1"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
+      <c r="D245" s="1"/>
+      <c r="E245" s="3"/>
+      <c r="F245" s="1"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B246" s="1"/>
+      <c r="C246" s="1"/>
+      <c r="D246" s="1"/>
+      <c r="E246" s="3"/>
+      <c r="F246" s="1"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="1"/>
+      <c r="B247" s="1"/>
+      <c r="C247" s="1"/>
+      <c r="D247" s="1"/>
+      <c r="E247" s="3"/>
+      <c r="F247" s="1"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="1"/>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="1"/>
+      <c r="E248" s="3"/>
+      <c r="F248" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C124 D2:F124">
+  <conditionalFormatting sqref="A1:C248 D2:F248">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
@@ -2465,7 +4100,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2475,7 +4110,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2485,7 +4120,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2495,7 +4130,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2505,7 +4140,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2515,7 +4150,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2525,7 +4160,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1">
         <v>1.5632496E12</v>
@@ -2537,7 +4172,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1">
         <v>1.56204E12</v>
@@ -2549,7 +4184,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1">
         <v>1.5658416E12</v>
@@ -2561,7 +4196,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1">
         <v>1.5667056E12</v>
@@ -2573,7 +4208,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1">
         <v>1.5649776E12</v>
@@ -2584,7 +4219,9 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2592,15 +4229,125 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="3"/>
       <c r="F14" s="1"/>
     </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C14 D2:F14">
+  <conditionalFormatting sqref="A1:C25 D2:F25">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>

</xml_diff>

<commit_message>
added spell efficiency to moonmanager ui, and fix moonrise timer
</commit_message>
<xml_diff>
--- a/Dictionaries/store.xlsx
+++ b/Dictionaries/store.xlsx
@@ -32,13 +32,31 @@
     <t>gold</t>
   </si>
   <si>
+    <t>bundle_abondiasBest</t>
+  </si>
+  <si>
     <t>silver1</t>
   </si>
   <si>
     <t>consumable_alignmentBoosterSmaller</t>
   </si>
   <si>
-    <t>bundle_abondiasBest</t>
+    <t>consumable_alignmentBoosterMedium</t>
+  </si>
+  <si>
+    <t>bundle_sapphosChoice</t>
+  </si>
+  <si>
+    <t>consumable_alignmentBoosterGreater</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterSmaller</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterMedium</t>
+  </si>
+  <si>
+    <t>bundle_hermeticCollection</t>
   </si>
   <si>
     <t>silver2</t>
@@ -50,48 +68,348 @@
     <t>silver4</t>
   </si>
   <si>
+    <t>consumable_xpBoosterGreater</t>
+  </si>
+  <si>
     <t>silver5</t>
   </si>
   <si>
+    <t>consumable_invisible</t>
+  </si>
+  <si>
     <t>silver6</t>
   </si>
   <si>
-    <t>bundle_sapphosChoice</t>
-  </si>
-  <si>
-    <t>consumable_alignmentBoosterMedium</t>
-  </si>
-  <si>
-    <t>consumable_alignmentBoosterGreater</t>
-  </si>
-  <si>
-    <t>consumable_xpBoosterSmaller</t>
-  </si>
-  <si>
-    <t>bundle_hermeticCollection</t>
-  </si>
-  <si>
-    <t>consumable_xpBoosterMedium</t>
-  </si>
-  <si>
-    <t>consumable_xpBoosterGreater</t>
-  </si>
-  <si>
-    <t>consumable_invisible</t>
-  </si>
-  <si>
     <t>consumable_truesight</t>
   </si>
   <si>
     <t>cosmetic_f_PF_WENDIGO</t>
   </si>
   <si>
+    <t>shop_locked_wndg</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_BARGHEST</t>
+  </si>
+  <si>
+    <t>shop_locked_barg</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_CATSIDHE</t>
+  </si>
+  <si>
+    <t>shop_locked_sidh</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_GRINDYLOW</t>
+  </si>
+  <si>
+    <t>shop_locked_grdlw</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_SENTINALOWL</t>
+  </si>
+  <si>
+    <t>shop_locked_owl</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HDWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HBH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HBO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HHO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HNO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_CEH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_CES</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_FLOWER</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_BDH</t>
+  </si>
+  <si>
+    <t>shop_locked_rrc</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_FKFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_CGH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_PNY</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_SNWDRP</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_BUN</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_BRD</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_SPK</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_BZZ</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_CURL</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_WAVE</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_BOB</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_FANCYCHOKER</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_MOONNECKLACE</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_BOW</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_KFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_PPS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_SCT</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_MESHDRESS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_TN</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_MESHTOP</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_WRAP</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_ROMP</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_BUTTON</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_WBYE</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_WITCHCO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_MAGICINK</t>
+  </si>
+  <si>
+    <t>cosmetic_f_WL_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_WL_KFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_WR_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_WR_KFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_H_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_H_BH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_FL_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_FL_HFR</t>
+  </si>
+  <si>
+    <t>cosmetic_f_FR_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_KFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_PPS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_LS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_SS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_TIGHT</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_HEAVYSKIRT</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_SHORTS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_ROMPER</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_LACELEG</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_BDWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_SBDWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_SDWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_KFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_TIED</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_BOW</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_FUR</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_DWO</t>
+  </si>
+  <si>
+    <t>shop_locked_beta</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_DSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_DTO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_PRIMAVERA</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_KIM</t>
+  </si>
+  <si>
+    <t>shop_locked_top</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_SMMRSOL</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_SHADOW</t>
+  </si>
+  <si>
+    <t>shop_locked_shadow</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_GRAY</t>
+  </si>
+  <si>
+    <t>shop_locked_gray</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_WHITE</t>
+  </si>
+  <si>
+    <t>shop_locked_white</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SF_HSF</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SF_HSS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SF_HST</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SF_GLSS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SF_HOOPS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SS_CROWSKULL</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SS_HAT</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SS_HBT</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SS_HFT</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SS_HMT</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SS_HST</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SS_JET</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SS_DWO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_HHO</t>
   </si>
   <si>
-    <t>shop_locked_wndg</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -128,12 +446,6 @@
     <t>_</t>
   </si>
   <si>
-    <t>cosmetic_f_PF_BARGHEST</t>
-  </si>
-  <si>
-    <t>shop_locked_barg</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_HKO</t>
   </si>
   <si>
@@ -143,42 +455,21 @@
     <t>cosmetic_m_S_HLO</t>
   </si>
   <si>
-    <t>cosmetic_f_PF_CATSIDHE</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_JACKFROST</t>
   </si>
   <si>
-    <t>shop_locked_sidh</t>
-  </si>
-  <si>
-    <t>cosmetic_f_PF_GRINDYLOW</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_MIDSUMMER</t>
   </si>
   <si>
-    <t>shop_locked_grdlw</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_CORNMOON</t>
   </si>
   <si>
-    <t>cosmetic_f_PF_SENTINALOWL</t>
-  </si>
-  <si>
-    <t>shop_locked_owl</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_CALYPSO</t>
   </si>
   <si>
     <t>cosmetic_m_S_FIREDANCER</t>
   </si>
   <si>
-    <t>cosmetic_f_HE_DWO</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_BRNNGWTCH</t>
   </si>
   <si>
@@ -186,297 +477,6 @@
   </si>
   <si>
     <t>cosmetic_m_S_THUNDERMOON</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HDWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HBH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HBO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HHO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HNO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_CEH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_CES</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_FLOWER</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_BDH</t>
-  </si>
-  <si>
-    <t>shop_locked_rrc</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_FKFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_CGH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_PNY</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_SNWDRP</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_BUN</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_BRD</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_SPK</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_BZZ</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_CURL</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_WAVE</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_BOB</t>
-  </si>
-  <si>
-    <t>cosmetic_f_N_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_N_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_N_FANCYCHOKER</t>
-  </si>
-  <si>
-    <t>cosmetic_f_N_MOONNECKLACE</t>
-  </si>
-  <si>
-    <t>cosmetic_f_N_BOW</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_PPS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_SCT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_MESHDRESS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_TN</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_MESHTOP</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_WRAP</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_ROMP</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_BUTTON</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_WBYE</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_WITCHCO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_MAGICINK</t>
-  </si>
-  <si>
-    <t>cosmetic_f_WL_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_WL_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_WR_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_WR_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_H_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_H_BH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_FL_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_FL_HFR</t>
-  </si>
-  <si>
-    <t>cosmetic_f_FR_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_PPS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_LS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_SS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_TIGHT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_HEAVYSKIRT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_SHORTS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_ROMPER</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_LACELEG</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_BDWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_SBDWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_SDWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_TIED</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_BOW</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_FUR</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_DWO</t>
-  </si>
-  <si>
-    <t>shop_locked_beta</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_DSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_DTO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_PRIMAVERA</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_KIM</t>
-  </si>
-  <si>
-    <t>shop_locked_top</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_SMMRSOL</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_SHADOW</t>
-  </si>
-  <si>
-    <t>shop_locked_shadow</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_GRAY</t>
-  </si>
-  <si>
-    <t>shop_locked_gray</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_WHITE</t>
-  </si>
-  <si>
-    <t>shop_locked_white</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_HSF</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_HSS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_HST</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_GLSS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_HOOPS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SS_CROWSKULL</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SS_HAT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SS_HBT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SS_HFT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SS_HMT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SS_HST</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SS_JET</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SS_DWO</t>
   </si>
   <si>
     <t>cosmetic_f_SS_MOLOTOV</t>
@@ -987,23 +987,23 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="top"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1120,20 +1120,20 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>300.0</v>
       </c>
       <c r="E2" s="8"/>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1153,11 +1153,11 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>300.0</v>
       </c>
       <c r="E4" s="8"/>
@@ -1168,7 +1168,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
@@ -1176,7 +1176,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="6"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
@@ -1184,7 +1184,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1192,7 +1192,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1200,7 +1200,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1208,7 +1208,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1216,7 +1216,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1224,7 +1224,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1232,7 +1232,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1240,7 +1240,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1287,95 +1287,95 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>100.0</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="9">
         <v>300.0</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>500.0</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="9">
         <v>100.0</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>300.0</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="9">
         <v>500.0</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>200.0</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1387,7 +1387,7 @@
       <c r="D9" s="11">
         <v>200.0</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1395,15 +1395,15 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="6"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1411,15 +1411,15 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="6"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1427,7 +1427,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1474,71 +1474,71 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="6"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="6"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="6"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="6"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1546,7 +1546,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1554,7 +1554,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1562,7 +1562,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1570,7 +1570,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1578,7 +1578,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1586,7 +1586,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1594,7 +1594,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1641,10 +1641,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
         <v>1.56168E12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="13">
         <v>1000.0</v>
@@ -1668,13 +1668,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D3" s="13">
         <v>1000.0</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D4" s="13">
         <v>1000.0</v>
@@ -1704,13 +1704,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D5" s="13">
         <v>1000.0</v>
@@ -1722,13 +1722,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D6" s="13">
         <v>1000.0</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1866,11 +1866,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D16" s="13">
         <v>900.0</v>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2232,7 +2232,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2288,7 +2288,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2568,7 +2568,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2596,7 +2596,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2638,7 +2638,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2680,7 +2680,7 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2694,7 +2694,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2708,7 +2708,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2722,43 +2722,43 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D77" s="1"/>
-      <c r="E77" s="6"/>
+      <c r="E77" s="7"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D78" s="1"/>
-      <c r="E78" s="6"/>
+      <c r="E78" s="7"/>
       <c r="F78" s="1"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D79" s="1"/>
-      <c r="E79" s="6"/>
+      <c r="E79" s="7"/>
       <c r="F79" s="1"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2772,13 +2772,13 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="B81" s="1">
         <v>1.5646176E12</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="D81" s="13">
         <v>1200.0</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2804,11 +2804,11 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="D83" s="13">
         <v>1200.0</v>
@@ -2820,11 +2820,11 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D84" s="13">
         <v>1200.0</v>
@@ -2836,11 +2836,11 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="D85" s="13">
         <v>1200.0</v>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2880,7 +2880,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2908,7 +2908,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2964,7 +2964,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3434,12 +3434,12 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
-      <c r="E125" s="6"/>
+      <c r="E125" s="7"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126">
@@ -3575,7 +3575,7 @@
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
-      <c r="E135" s="6"/>
+      <c r="E135" s="7"/>
       <c r="F135" s="1"/>
     </row>
     <row r="136">
@@ -4803,7 +4803,7 @@
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
-      <c r="E223" s="6"/>
+      <c r="E223" s="7"/>
       <c r="F223" s="1"/>
     </row>
     <row r="224">
@@ -4827,7 +4827,7 @@
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
-      <c r="E225" s="6"/>
+      <c r="E225" s="7"/>
       <c r="F225" s="1"/>
     </row>
     <row r="226">
@@ -4865,7 +4865,7 @@
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
-      <c r="E228" s="6"/>
+      <c r="E228" s="7"/>
       <c r="F228" s="1"/>
     </row>
     <row r="229">
@@ -5125,7 +5125,7 @@
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
-      <c r="E247" s="6"/>
+      <c r="E247" s="7"/>
       <c r="F247" s="1"/>
     </row>
     <row r="248">
@@ -5133,7 +5133,7 @@
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
-      <c r="E248" s="6"/>
+      <c r="E248" s="7"/>
       <c r="F248" s="1"/>
     </row>
   </sheetData>
@@ -5175,100 +5175,100 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>25</v>
+      <c r="E2" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>25</v>
+      <c r="E3" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>25</v>
+      <c r="E4" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>25</v>
+      <c r="E5" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
+      <c r="E6" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
+      <c r="E7" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="B8" s="1">
         <v>1.5632496E12</v>
@@ -5277,14 +5277,14 @@
       <c r="D8" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>25</v>
+      <c r="E8" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="B9" s="1">
         <v>1.56204E12</v>
@@ -5293,14 +5293,14 @@
       <c r="D9" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>25</v>
+      <c r="E9" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="B10" s="1">
         <v>1.5658416E12</v>
@@ -5309,14 +5309,14 @@
       <c r="D10" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>25</v>
+      <c r="E10" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="B11" s="1">
         <v>1.5667056E12</v>
@@ -5325,14 +5325,14 @@
       <c r="D11" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>25</v>
+      <c r="E11" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
       <c r="B12" s="1">
         <v>1.5649776E12</v>
@@ -5341,176 +5341,176 @@
       <c r="D12" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>25</v>
+      <c r="E12" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>25</v>
+      <c r="E13" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>25</v>
+      <c r="E14" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>25</v>
+      <c r="E15" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>145</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>25</v>
+      <c r="E16" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>25</v>
+      <c r="E17" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>25</v>
+      <c r="E18" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>148</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>25</v>
+      <c r="E19" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>25</v>
+      <c r="E20" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>25</v>
+      <c r="E21" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>25</v>
+      <c r="E22" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>25</v>
+      <c r="E23" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>153</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>25</v>
+      <c r="E24" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -5519,7 +5519,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="6"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip nearby pops UI
</commit_message>
<xml_diff>
--- a/Dictionaries/store.xlsx
+++ b/Dictionaries/store.xlsx
@@ -35,30 +35,39 @@
     <t>bundle_abondiasBest</t>
   </si>
   <si>
+    <t>bundle_sapphosChoice</t>
+  </si>
+  <si>
+    <t>bundle_hermeticCollection</t>
+  </si>
+  <si>
+    <t>consumable_alignmentBoosterSmaller</t>
+  </si>
+  <si>
+    <t>consumable_alignmentBoosterMedium</t>
+  </si>
+  <si>
+    <t>consumable_alignmentBoosterGreater</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterSmaller</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterMedium</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterGreater</t>
+  </si>
+  <si>
+    <t>consumable_invisible</t>
+  </si>
+  <si>
+    <t>consumable_truesight</t>
+  </si>
+  <si>
     <t>silver1</t>
   </si>
   <si>
-    <t>consumable_alignmentBoosterSmaller</t>
-  </si>
-  <si>
-    <t>consumable_alignmentBoosterMedium</t>
-  </si>
-  <si>
-    <t>bundle_sapphosChoice</t>
-  </si>
-  <si>
-    <t>consumable_alignmentBoosterGreater</t>
-  </si>
-  <si>
-    <t>consumable_xpBoosterSmaller</t>
-  </si>
-  <si>
-    <t>consumable_xpBoosterMedium</t>
-  </si>
-  <si>
-    <t>bundle_hermeticCollection</t>
-  </si>
-  <si>
     <t>silver2</t>
   </si>
   <si>
@@ -68,21 +77,12 @@
     <t>silver4</t>
   </si>
   <si>
-    <t>consumable_xpBoosterGreater</t>
-  </si>
-  <si>
     <t>silver5</t>
   </si>
   <si>
-    <t>consumable_invisible</t>
-  </si>
-  <si>
     <t>silver6</t>
   </si>
   <si>
-    <t>consumable_truesight</t>
-  </si>
-  <si>
     <t>cosmetic_f_PF_WENDIGO</t>
   </si>
   <si>
@@ -164,30 +164,87 @@
     <t>cosmetic_f_HA_SNWDRP</t>
   </si>
   <si>
+    <t>cosmetic_f_S_HHO</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_BUN</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_HKO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_HLO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_SNOWQUEEN</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_LILYOV</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_MIDSUMMER</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_THUNDERMOON</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_ECLIPSE</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_CORNMOON</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_BRNNGWTCH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_CALYPSO</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_BRD</t>
   </si>
   <si>
+    <t>cosmetic_m_S_HKO</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_SPK</t>
   </si>
   <si>
+    <t>cosmetic_m_S_HHO</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_BZZ</t>
   </si>
   <si>
+    <t>cosmetic_m_S_HLO</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_CURL</t>
   </si>
   <si>
+    <t>cosmetic_m_S_JACKFROST</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_WAVE</t>
   </si>
   <si>
+    <t>cosmetic_m_S_MIDSUMMER</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_BOB</t>
   </si>
   <si>
     <t>cosmetic_f_N_DWO</t>
   </si>
   <si>
+    <t>cosmetic_m_S_CORNMOON</t>
+  </si>
+  <si>
     <t>cosmetic_f_N_KSO</t>
   </si>
   <si>
@@ -212,21 +269,36 @@
     <t>cosmetic_f_C_PPS</t>
   </si>
   <si>
+    <t>cosmetic_m_S_CALYPSO</t>
+  </si>
+  <si>
     <t>cosmetic_f_C_SCT</t>
   </si>
   <si>
     <t>cosmetic_f_C_MESHDRESS</t>
   </si>
   <si>
+    <t>cosmetic_m_S_FIREDANCER</t>
+  </si>
+  <si>
     <t>cosmetic_f_C_TN</t>
   </si>
   <si>
+    <t>cosmetic_m_S_BRNNGWTCH</t>
+  </si>
+  <si>
     <t>cosmetic_f_C_MESHTOP</t>
   </si>
   <si>
+    <t>cosmetic_m_S_ECLIPSE</t>
+  </si>
+  <si>
     <t>cosmetic_f_C_WRAP</t>
   </si>
   <si>
+    <t>cosmetic_m_S_THUNDERMOON</t>
+  </si>
+  <si>
     <t>cosmetic_f_C_ROMP</t>
   </si>
   <si>
@@ -405,78 +477,6 @@
   </si>
   <si>
     <t>cosmetic_f_SS_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_HHO</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_HKO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_HLO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_SNOWQUEEN</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_LILYOV</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_MIDSUMMER</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_THUNDERMOON</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_ECLIPSE</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_CORNMOON</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_BRNNGWTCH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_CALYPSO</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_HKO</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_HHO</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_HLO</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_JACKFROST</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_MIDSUMMER</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_CORNMOON</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_CALYPSO</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_FIREDANCER</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_BRNNGWTCH</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_ECLIPSE</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_THUNDERMOON</t>
   </si>
   <si>
     <t>cosmetic_f_SS_MOLOTOV</t>
@@ -987,23 +987,14 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1014,11 +1005,20 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -1120,10 +1120,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1133,34 +1133,34 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="6">
+      <c r="D2" s="4">
         <v>300.0</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="9">
+      <c r="D3" s="6">
         <v>300.0</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>300.0</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
@@ -1168,7 +1168,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
@@ -1176,7 +1176,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
@@ -1184,7 +1184,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1192,7 +1192,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1200,7 +1200,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1208,7 +1208,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1216,7 +1216,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1224,7 +1224,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1232,7 +1232,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1240,7 +1240,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1287,35 +1287,35 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="6">
+      <c r="D2" s="4">
         <v>100.0</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="9">
+      <c r="D3" s="6">
         <v>300.0</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
@@ -1324,10 +1324,10 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>500.0</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
@@ -1336,10 +1336,10 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>100.0</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
@@ -1348,86 +1348,86 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>300.0</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>500.0</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>200.0</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>200.0</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="7"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1474,71 +1474,71 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1546,7 +1546,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1554,7 +1554,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1562,7 +1562,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1570,7 +1570,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1578,7 +1578,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1586,7 +1586,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1594,7 +1594,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1641,10 +1641,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2232,7 +2232,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2288,7 +2288,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2568,7 +2568,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2596,7 +2596,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2638,7 +2638,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2680,7 +2680,7 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2694,7 +2694,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2708,7 +2708,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2722,43 +2722,43 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="D77" s="1"/>
-      <c r="E77" s="7"/>
+      <c r="E77" s="8"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="D78" s="1"/>
-      <c r="E78" s="7"/>
+      <c r="E78" s="8"/>
       <c r="F78" s="1"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="D79" s="1"/>
-      <c r="E79" s="7"/>
+      <c r="E79" s="8"/>
       <c r="F79" s="1"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2772,13 +2772,13 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="B81" s="1">
         <v>1.5646176E12</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="D81" s="13">
         <v>1200.0</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2804,11 +2804,11 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="D83" s="13">
         <v>1200.0</v>
@@ -2820,11 +2820,11 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="D84" s="13">
         <v>1200.0</v>
@@ -2836,11 +2836,11 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="D85" s="13">
         <v>1200.0</v>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2880,7 +2880,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2908,7 +2908,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2964,7 +2964,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3434,12 +3434,12 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>142</v>
+        <v>62</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
-      <c r="E125" s="7"/>
+      <c r="E125" s="8"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126">
@@ -3575,7 +3575,7 @@
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
-      <c r="E135" s="7"/>
+      <c r="E135" s="8"/>
       <c r="F135" s="1"/>
     </row>
     <row r="136">
@@ -4803,7 +4803,7 @@
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
-      <c r="E223" s="7"/>
+      <c r="E223" s="8"/>
       <c r="F223" s="1"/>
     </row>
     <row r="224">
@@ -4827,7 +4827,7 @@
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
-      <c r="E225" s="7"/>
+      <c r="E225" s="8"/>
       <c r="F225" s="1"/>
     </row>
     <row r="226">
@@ -4865,7 +4865,7 @@
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
-      <c r="E228" s="7"/>
+      <c r="E228" s="8"/>
       <c r="F228" s="1"/>
     </row>
     <row r="229">
@@ -5125,7 +5125,7 @@
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
-      <c r="E247" s="7"/>
+      <c r="E247" s="8"/>
       <c r="F247" s="1"/>
     </row>
     <row r="248">
@@ -5133,7 +5133,7 @@
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
-      <c r="E248" s="7"/>
+      <c r="E248" s="8"/>
       <c r="F248" s="1"/>
     </row>
   </sheetData>
@@ -5175,100 +5175,100 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>131</v>
+      <c r="E2" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>131</v>
+      <c r="E3" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>131</v>
+      <c r="E4" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>131</v>
+      <c r="E5" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>131</v>
+      <c r="E6" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>136</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>131</v>
+      <c r="E7" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1">
         <v>1.5632496E12</v>
@@ -5277,14 +5277,14 @@
       <c r="D8" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>131</v>
+      <c r="E8" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>138</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1">
         <v>1.56204E12</v>
@@ -5293,14 +5293,14 @@
       <c r="D9" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>131</v>
+      <c r="E9" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>139</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1">
         <v>1.5658416E12</v>
@@ -5309,14 +5309,14 @@
       <c r="D10" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>131</v>
+      <c r="E10" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1">
         <v>1.5667056E12</v>
@@ -5325,14 +5325,14 @@
       <c r="D11" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>131</v>
+      <c r="E11" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1">
         <v>1.5649776E12</v>
@@ -5341,176 +5341,176 @@
       <c r="D12" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>131</v>
+      <c r="E12" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>142</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>131</v>
+      <c r="E13" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>143</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>131</v>
+      <c r="E14" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>144</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>131</v>
+      <c r="E15" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>145</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>131</v>
+      <c r="E16" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>131</v>
+      <c r="E17" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>131</v>
+      <c r="E18" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>148</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>131</v>
+      <c r="E19" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>149</v>
+        <v>84</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>131</v>
+      <c r="E20" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>131</v>
+      <c r="E21" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>151</v>
+        <v>89</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>131</v>
+      <c r="E22" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>131</v>
+      <c r="E23" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>131</v>
+      <c r="E24" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -5519,7 +5519,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="7"/>
+      <c r="E25" s="8"/>
       <c r="F25" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add helper to extract spell templates data into spreadsheet format
</commit_message>
<xml_diff>
--- a/Dictionaries/store.xlsx
+++ b/Dictionaries/store.xlsx
@@ -41,6 +41,60 @@
     <t>bundle_hermeticCollection</t>
   </si>
   <si>
+    <t>silver1</t>
+  </si>
+  <si>
+    <t>silver2</t>
+  </si>
+  <si>
+    <t>silver3</t>
+  </si>
+  <si>
+    <t>silver4</t>
+  </si>
+  <si>
+    <t>silver5</t>
+  </si>
+  <si>
+    <t>silver6</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_WENDIGO</t>
+  </si>
+  <si>
+    <t>shop_locked_wndg</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_BARGHEST</t>
+  </si>
+  <si>
+    <t>shop_locked_barg</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_CATSIDHE</t>
+  </si>
+  <si>
+    <t>shop_locked_sidh</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_GRINDYLOW</t>
+  </si>
+  <si>
+    <t>shop_locked_grdlw</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_SENTINALOWL</t>
+  </si>
+  <si>
+    <t>shop_locked_owl</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HDWO</t>
+  </si>
+  <si>
     <t>consumable_alignmentBoosterSmaller</t>
   </si>
   <si>
@@ -53,102 +107,48 @@
     <t>consumable_xpBoosterSmaller</t>
   </si>
   <si>
+    <t>cosmetic_f_HE_HBH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HBO</t>
+  </si>
+  <si>
     <t>consumable_xpBoosterMedium</t>
   </si>
   <si>
+    <t>cosmetic_f_HE_HHO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HNO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_CEH</t>
+  </si>
+  <si>
     <t>consumable_xpBoosterGreater</t>
   </si>
   <si>
+    <t>cosmetic_f_HE_CES</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_FLOWER</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_BDH</t>
+  </si>
+  <si>
+    <t>shop_locked_rrc</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_DWO</t>
+  </si>
+  <si>
     <t>consumable_invisible</t>
   </si>
   <si>
     <t>consumable_truesight</t>
   </si>
   <si>
-    <t>silver1</t>
-  </si>
-  <si>
-    <t>silver2</t>
-  </si>
-  <si>
-    <t>silver3</t>
-  </si>
-  <si>
-    <t>silver4</t>
-  </si>
-  <si>
-    <t>silver5</t>
-  </si>
-  <si>
-    <t>silver6</t>
-  </si>
-  <si>
-    <t>cosmetic_f_PF_WENDIGO</t>
-  </si>
-  <si>
-    <t>shop_locked_wndg</t>
-  </si>
-  <si>
-    <t>cosmetic_f_PF_BARGHEST</t>
-  </si>
-  <si>
-    <t>shop_locked_barg</t>
-  </si>
-  <si>
-    <t>cosmetic_f_PF_CATSIDHE</t>
-  </si>
-  <si>
-    <t>shop_locked_sidh</t>
-  </si>
-  <si>
-    <t>cosmetic_f_PF_GRINDYLOW</t>
-  </si>
-  <si>
-    <t>shop_locked_grdlw</t>
-  </si>
-  <si>
-    <t>cosmetic_f_PF_SENTINALOWL</t>
-  </si>
-  <si>
-    <t>shop_locked_owl</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HDWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HBH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HBO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HHO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HNO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_CEH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_CES</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_FLOWER</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_BDH</t>
-  </si>
-  <si>
-    <t>shop_locked_rrc</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_DWO</t>
-  </si>
-  <si>
     <t>cosmetic_f_HA_FKFO</t>
   </si>
   <si>
@@ -164,298 +164,298 @@
     <t>cosmetic_f_HA_SNWDRP</t>
   </si>
   <si>
+    <t>cosmetic_f_HA_BUN</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_BRD</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_SPK</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_BZZ</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_CURL</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_WAVE</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_BOB</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_FANCYCHOKER</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_MOONNECKLACE</t>
+  </si>
+  <si>
+    <t>cosmetic_f_N_BOW</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_KFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_PPS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_SCT</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_MESHDRESS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_TN</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_MESHTOP</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_WRAP</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_ROMP</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_BUTTON</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_WBYE</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_WITCHCO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_C_MAGICINK</t>
+  </si>
+  <si>
+    <t>cosmetic_f_WL_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_WL_KFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_WR_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_WR_KFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_H_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_H_BH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_FL_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_FL_HFR</t>
+  </si>
+  <si>
+    <t>cosmetic_f_FR_KSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_KFO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_KSO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_HHO</t>
   </si>
   <si>
-    <t>cosmetic_f_HA_BUN</t>
+    <t>cosmetic_f_L_PPS</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
+    <t>cosmetic_f_L_LS</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_HKO</t>
   </si>
   <si>
+    <t>cosmetic_f_L_SS</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_HLO</t>
   </si>
   <si>
+    <t>cosmetic_f_L_TIGHT</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_HEAVYSKIRT</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_SNOWQUEEN</t>
   </si>
   <si>
+    <t>cosmetic_f_L_SHORTS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_L_ROMPER</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_LILYOV</t>
   </si>
   <si>
+    <t>cosmetic_f_L_LACELEG</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_MIDSUMMER</t>
   </si>
   <si>
+    <t>cosmetic_f_F_BDWO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_THUNDERMOON</t>
   </si>
   <si>
+    <t>cosmetic_f_F_SBDWO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_ECLIPSE</t>
   </si>
   <si>
+    <t>cosmetic_f_F_SDWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_KFO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_CORNMOON</t>
   </si>
   <si>
+    <t>cosmetic_f_F_KSO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_BRNNGWTCH</t>
   </si>
   <si>
+    <t>cosmetic_f_F_TIED</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_CALYPSO</t>
   </si>
   <si>
+    <t>cosmetic_f_F_BOW</t>
+  </si>
+  <si>
+    <t>cosmetic_f_F_FUR</t>
+  </si>
+  <si>
     <t>_</t>
   </si>
   <si>
-    <t>cosmetic_f_HA_BRD</t>
+    <t>cosmetic_f_CR_DWO</t>
+  </si>
+  <si>
+    <t>shop_locked_beta</t>
   </si>
   <si>
     <t>cosmetic_m_S_HKO</t>
   </si>
   <si>
-    <t>cosmetic_f_HA_SPK</t>
+    <t>cosmetic_f_CR_DSO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_DTO</t>
   </si>
   <si>
     <t>cosmetic_m_S_HHO</t>
   </si>
   <si>
-    <t>cosmetic_f_HA_BZZ</t>
+    <t>cosmetic_f_CR_PRIMAVERA</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_KIM</t>
   </si>
   <si>
     <t>cosmetic_m_S_HLO</t>
   </si>
   <si>
-    <t>cosmetic_f_HA_CURL</t>
+    <t>shop_locked_top</t>
+  </si>
+  <si>
+    <t>cosmetic_f_CR_SMMRSOL</t>
   </si>
   <si>
     <t>cosmetic_m_S_JACKFROST</t>
   </si>
   <si>
-    <t>cosmetic_f_HA_WAVE</t>
+    <t>cosmetic_f_CR_SHADOW</t>
+  </si>
+  <si>
+    <t>shop_locked_shadow</t>
   </si>
   <si>
     <t>cosmetic_m_S_MIDSUMMER</t>
   </si>
   <si>
-    <t>cosmetic_f_HA_BOB</t>
-  </si>
-  <si>
-    <t>cosmetic_f_N_DWO</t>
+    <t>cosmetic_f_CR_GRAY</t>
+  </si>
+  <si>
+    <t>shop_locked_gray</t>
   </si>
   <si>
     <t>cosmetic_m_S_CORNMOON</t>
   </si>
   <si>
-    <t>cosmetic_f_N_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_N_FANCYCHOKER</t>
-  </si>
-  <si>
-    <t>cosmetic_f_N_MOONNECKLACE</t>
-  </si>
-  <si>
-    <t>cosmetic_f_N_BOW</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_PPS</t>
+    <t>cosmetic_f_CR_WHITE</t>
+  </si>
+  <si>
+    <t>shop_locked_white</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SF_HSF</t>
   </si>
   <si>
     <t>cosmetic_m_S_CALYPSO</t>
   </si>
   <si>
-    <t>cosmetic_f_C_SCT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_MESHDRESS</t>
+    <t>cosmetic_f_SF_HSS</t>
   </si>
   <si>
     <t>cosmetic_m_S_FIREDANCER</t>
   </si>
   <si>
-    <t>cosmetic_f_C_TN</t>
+    <t>cosmetic_f_SF_HST</t>
   </si>
   <si>
     <t>cosmetic_m_S_BRNNGWTCH</t>
   </si>
   <si>
-    <t>cosmetic_f_C_MESHTOP</t>
+    <t>cosmetic_f_SF_GLSS</t>
   </si>
   <si>
     <t>cosmetic_m_S_ECLIPSE</t>
   </si>
   <si>
-    <t>cosmetic_f_C_WRAP</t>
+    <t>cosmetic_f_SF_HOOPS</t>
+  </si>
+  <si>
+    <t>cosmetic_f_SS_CROWSKULL</t>
   </si>
   <si>
     <t>cosmetic_m_S_THUNDERMOON</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_ROMP</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_BUTTON</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_WBYE</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_WITCHCO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_C_MAGICINK</t>
-  </si>
-  <si>
-    <t>cosmetic_f_WL_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_WL_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_WR_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_WR_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_H_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_H_BH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_FL_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_FL_HFR</t>
-  </si>
-  <si>
-    <t>cosmetic_f_FR_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_PPS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_LS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_SS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_TIGHT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_HEAVYSKIRT</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_SHORTS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_ROMPER</t>
-  </si>
-  <si>
-    <t>cosmetic_f_L_LACELEG</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_BDWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_SBDWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_SDWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_KFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_TIED</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_BOW</t>
-  </si>
-  <si>
-    <t>cosmetic_f_F_FUR</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_DWO</t>
-  </si>
-  <si>
-    <t>shop_locked_beta</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_DSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_DTO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_PRIMAVERA</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_KIM</t>
-  </si>
-  <si>
-    <t>shop_locked_top</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_SMMRSOL</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_SHADOW</t>
-  </si>
-  <si>
-    <t>shop_locked_shadow</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_GRAY</t>
-  </si>
-  <si>
-    <t>shop_locked_gray</t>
-  </si>
-  <si>
-    <t>cosmetic_f_CR_WHITE</t>
-  </si>
-  <si>
-    <t>shop_locked_white</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_HSF</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_HSS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_HST</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_GLSS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SF_HOOPS</t>
-  </si>
-  <si>
-    <t>cosmetic_f_SS_CROWSKULL</t>
   </si>
   <si>
     <t>cosmetic_f_SS_HAT</t>
@@ -1008,16 +1008,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1034,6 +1028,12 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -1290,13 +1290,13 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1332,7 +1332,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1380,11 +1380,11 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="10">
+      <c r="D9" s="16">
         <v>200.0</v>
       </c>
       <c r="E9" s="8"/>
@@ -1394,7 +1394,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="8"/>
       <c r="F10" s="1"/>
     </row>
@@ -1410,7 +1410,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="11"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="8"/>
       <c r="F12" s="1"/>
     </row>
@@ -1426,7 +1426,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="11"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="8"/>
       <c r="F14" s="1"/>
     </row>
@@ -1474,16 +1474,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1641,255 +1641,255 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="13">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="12">
         <v>10.0</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="13">
+        <v>17</v>
+      </c>
+      <c r="D3" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="13">
         <v>10.0</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="13">
+        <v>19</v>
+      </c>
+      <c r="D4" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="13">
         <v>10.0</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="13">
+        <v>21</v>
+      </c>
+      <c r="D5" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="13">
         <v>10.0</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="13">
+        <v>23</v>
+      </c>
+      <c r="D6" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="14">
         <v>10.0</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="13">
+      <c r="D7" s="11">
         <v>800.0</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>8.0</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="13">
+      <c r="D8" s="11">
         <v>900.0</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="13">
         <v>9.0</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="13">
+      <c r="D9" s="11">
         <v>850.0</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="13">
         <v>8.0</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="13">
+      <c r="D10" s="11">
         <v>500.0</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="13">
         <v>5.0</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="13">
+      <c r="D11" s="11">
         <v>600.0</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="13">
         <v>6.0</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="13">
+      <c r="D12" s="11">
         <v>800.0</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="13">
         <v>8.0</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="13">
+      <c r="D13" s="11">
         <v>850.0</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="13">
         <v>8.0</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="13">
+      <c r="D14" s="11">
         <v>850.0</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="13">
         <v>8.0</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="13">
+      <c r="D15" s="11">
         <v>500.0</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="13">
         <v>5.0</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="13">
+        <v>40</v>
+      </c>
+      <c r="D16" s="11">
         <v>900.0</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="13">
         <v>9.0</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="17">
+      <c r="D17" s="15">
         <v>300.0</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="12">
         <v>3.0</v>
       </c>
       <c r="F17" s="1"/>
@@ -1900,10 +1900,10 @@
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="13">
+      <c r="D18" s="11">
         <v>450.0</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="13">
         <v>4.0</v>
       </c>
       <c r="F18" s="1"/>
@@ -1914,10 +1914,10 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="13">
+      <c r="D19" s="11">
         <v>450.0</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="13">
         <v>4.0</v>
       </c>
       <c r="F19" s="1"/>
@@ -1928,10 +1928,10 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="13">
+      <c r="D20" s="11">
         <v>300.0</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="13">
         <v>3.0</v>
       </c>
       <c r="F20" s="1"/>
@@ -1942,10 +1942,10 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="13">
+      <c r="D21" s="11">
         <v>500.0</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="13">
         <v>5.0</v>
       </c>
       <c r="F21" s="1"/>
@@ -1956,17 +1956,17 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="13">
+      <c r="D22" s="11">
         <v>550.0</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="13">
         <v>5.0</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1980,753 +1980,753 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="13">
+      <c r="D24" s="11">
         <v>450.0</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="13">
         <v>4.0</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="13">
+      <c r="D25" s="11">
         <v>400.0</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="13">
         <v>4.0</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="13">
+      <c r="D26" s="11">
         <v>300.0</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="13">
         <v>3.0</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="13">
+      <c r="D27" s="11">
         <v>500.0</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="13">
         <v>5.0</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="13">
+      <c r="D28" s="11">
         <v>350.0</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="13">
         <v>3.0</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="13">
+      <c r="D29" s="11">
         <v>300.0</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="13">
         <v>3.0</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="13">
+      <c r="D30" s="11">
         <v>250.0</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="13">
         <v>2.0</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="13">
+      <c r="D31" s="11">
         <v>250.0</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="13">
         <v>2.0</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="13">
+      <c r="D32" s="11">
         <v>250.0</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="13">
         <v>2.0</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="13">
+      <c r="D33" s="11">
         <v>250.0</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="13">
         <v>2.0</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="13">
+      <c r="D34" s="11">
         <v>250.0</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="13">
         <v>2.0</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="13">
+      <c r="D35" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="13">
         <v>12.0</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="13">
+      <c r="D36" s="11">
         <v>950.0</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="13">
         <v>9.0</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="13">
+      <c r="D37" s="11">
         <v>950.0</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="13">
         <v>9.0</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="13">
+      <c r="D38" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="13">
         <v>12.0</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="13">
+      <c r="D39" s="11">
         <v>950.0</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="13">
         <v>9.0</v>
       </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="13">
+      <c r="D40" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="13">
         <v>12.0</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="13">
+      <c r="D41" s="11">
         <v>900.0</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="13">
         <v>9.0</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="13">
+      <c r="D42" s="11">
         <v>950.0</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="13">
         <v>9.0</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="13">
+      <c r="D43" s="11">
         <v>900.0</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="13">
         <v>9.0</v>
       </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="13">
+      <c r="D44" s="11">
         <v>950.0</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="13">
         <v>9.0</v>
       </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="13">
+      <c r="D45" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="13">
         <v>12.0</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="13">
+      <c r="D46" s="11">
         <v>900.0</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="13">
         <v>9.0</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="13">
+      <c r="D47" s="11">
         <v>900.0</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="13">
         <v>9.0</v>
       </c>
       <c r="F47" s="1"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="13">
+      <c r="D48" s="11">
         <v>900.0</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="13">
         <v>9.0</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="13">
+      <c r="D49" s="11">
         <v>150.0</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="13">
         <v>1.0</v>
       </c>
       <c r="F49" s="1"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="13">
+      <c r="D50" s="11">
         <v>150.0</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="13">
         <v>1.0</v>
       </c>
       <c r="F50" s="1"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="13">
+      <c r="D51" s="11">
         <v>150.0</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="13">
         <v>1.0</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="13">
+      <c r="D52" s="11">
         <v>150.0</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="13">
         <v>1.0</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="13">
+      <c r="D53" s="11">
         <v>300.0</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="13">
         <v>3.0</v>
       </c>
       <c r="F53" s="1"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="13">
+      <c r="D54" s="11">
         <v>300.0</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="13">
         <v>3.0</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="13">
+      <c r="D55" s="11">
         <v>150.0</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E55" s="13">
         <v>1.0</v>
       </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="13">
+      <c r="D56" s="11">
         <v>150.0</v>
       </c>
-      <c r="E56" s="15">
+      <c r="E56" s="13">
         <v>1.0</v>
       </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="13">
+      <c r="D57" s="11">
         <v>150.0</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E57" s="13">
         <v>1.0</v>
       </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="13">
+      <c r="D58" s="11">
         <v>550.0</v>
       </c>
-      <c r="E58" s="15">
+      <c r="E58" s="13">
         <v>5.0</v>
       </c>
       <c r="F58" s="1"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="13">
+      <c r="D59" s="11">
         <v>600.0</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="13">
         <v>6.0</v>
       </c>
       <c r="F59" s="1"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="13">
+      <c r="D60" s="11">
         <v>550.0</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="13">
         <v>5.0</v>
       </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="13">
+      <c r="D61" s="11">
         <v>600.0</v>
       </c>
-      <c r="E61" s="15">
+      <c r="E61" s="13">
         <v>6.0</v>
       </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="13">
+      <c r="D62" s="11">
         <v>600.0</v>
       </c>
-      <c r="E62" s="15">
+      <c r="E62" s="13">
         <v>6.0</v>
       </c>
       <c r="F62" s="1"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="13">
+      <c r="D63" s="11">
         <v>600.0</v>
       </c>
-      <c r="E63" s="15">
+      <c r="E63" s="13">
         <v>6.0</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="13">
+      <c r="D64" s="11">
         <v>500.0</v>
       </c>
-      <c r="E64" s="15">
+      <c r="E64" s="13">
         <v>5.0</v>
       </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="13">
+      <c r="D65" s="11">
         <v>600.0</v>
       </c>
-      <c r="E65" s="15">
+      <c r="E65" s="13">
         <v>6.0</v>
       </c>
       <c r="F65" s="1"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="13">
+      <c r="D66" s="11">
         <v>550.0</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E66" s="13">
         <v>5.0</v>
       </c>
       <c r="F66" s="1"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="13">
+      <c r="D67" s="11">
         <v>550.0</v>
       </c>
-      <c r="E67" s="15">
+      <c r="E67" s="13">
         <v>5.0</v>
       </c>
       <c r="F67" s="1"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="13">
+      <c r="D68" s="11">
         <v>600.0</v>
       </c>
-      <c r="E68" s="15">
+      <c r="E68" s="13">
         <v>6.0</v>
       </c>
       <c r="F68" s="1"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="13">
+      <c r="D69" s="11">
         <v>450.0</v>
       </c>
-      <c r="E69" s="15">
+      <c r="E69" s="13">
         <v>4.0</v>
       </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="13">
+      <c r="D70" s="11">
         <v>450.0</v>
       </c>
-      <c r="E70" s="15">
+      <c r="E70" s="13">
         <v>4.0</v>
       </c>
       <c r="F70" s="1"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="13">
+      <c r="D71" s="11">
         <v>400.0</v>
       </c>
-      <c r="E71" s="15">
+      <c r="E71" s="13">
         <v>4.0</v>
       </c>
       <c r="F71" s="1"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="13">
+      <c r="D72" s="11">
         <v>450.0</v>
       </c>
-      <c r="E72" s="15">
+      <c r="E72" s="13">
         <v>4.0</v>
       </c>
       <c r="F72" s="1"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="13">
+      <c r="D73" s="11">
         <v>450.0</v>
       </c>
-      <c r="E73" s="15">
+      <c r="E73" s="13">
         <v>4.0</v>
       </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="13">
+      <c r="D74" s="11">
         <v>450.0</v>
       </c>
-      <c r="E74" s="15">
+      <c r="E74" s="13">
         <v>4.0</v>
       </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="13">
+      <c r="D75" s="11">
         <v>450.0</v>
       </c>
-      <c r="E75" s="15">
+      <c r="E75" s="13">
         <v>4.0</v>
       </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="13">
+      <c r="D76" s="11">
         <v>450.0</v>
       </c>
-      <c r="E76" s="15">
+      <c r="E76" s="13">
         <v>4.0</v>
       </c>
       <c r="F76" s="1"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="8"/>
@@ -2734,11 +2734,11 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="8"/>
@@ -2746,11 +2746,11 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="8"/>
@@ -2758,178 +2758,178 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="13">
+      <c r="D80" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E80" s="15">
+      <c r="E80" s="13">
         <v>12.0</v>
       </c>
       <c r="F80" s="1"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B81" s="1">
         <v>1.5646176E12</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D81" s="13">
+        <v>125</v>
+      </c>
+      <c r="D81" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E81" s="15">
+      <c r="E81" s="13">
         <v>12.0</v>
       </c>
       <c r="F81" s="1"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="13">
+      <c r="D82" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E82" s="15">
+      <c r="E82" s="13">
         <v>12.0</v>
       </c>
       <c r="F82" s="1"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D83" s="13">
+        <v>129</v>
+      </c>
+      <c r="D83" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E83" s="15">
+      <c r="E83" s="13">
         <v>12.0</v>
       </c>
       <c r="F83" s="1"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D84" s="13">
+        <v>132</v>
+      </c>
+      <c r="D84" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E84" s="15">
+      <c r="E84" s="13">
         <v>12.0</v>
       </c>
       <c r="F84" s="1"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D85" s="13">
+        <v>135</v>
+      </c>
+      <c r="D85" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E85" s="15">
+      <c r="E85" s="13">
         <v>12.0</v>
       </c>
       <c r="F85" s="1"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="13">
+      <c r="D86" s="11">
         <v>800.0</v>
       </c>
-      <c r="E86" s="15">
+      <c r="E86" s="13">
         <v>8.0</v>
       </c>
       <c r="F86" s="1"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="13">
+      <c r="D87" s="11">
         <v>800.0</v>
       </c>
-      <c r="E87" s="15">
+      <c r="E87" s="13">
         <v>8.0</v>
       </c>
       <c r="F87" s="1"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="13">
+      <c r="D88" s="11">
         <v>800.0</v>
       </c>
-      <c r="E88" s="15">
+      <c r="E88" s="13">
         <v>8.0</v>
       </c>
       <c r="F88" s="1"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="13">
+      <c r="D89" s="11">
         <v>600.0</v>
       </c>
-      <c r="E89" s="15">
+      <c r="E89" s="13">
         <v>6.0</v>
       </c>
       <c r="F89" s="1"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="13">
+      <c r="D90" s="11">
         <v>600.0</v>
       </c>
-      <c r="E90" s="15">
+      <c r="E90" s="13">
         <v>6.0</v>
       </c>
       <c r="F90" s="1"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="13">
+      <c r="D91" s="11">
         <v>850.0</v>
       </c>
-      <c r="E91" s="15">
+      <c r="E91" s="13">
         <v>8.0</v>
       </c>
       <c r="F91" s="1"/>
@@ -2940,10 +2940,10 @@
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="13">
+      <c r="D92" s="11">
         <v>550.0</v>
       </c>
-      <c r="E92" s="15">
+      <c r="E92" s="13">
         <v>5.0</v>
       </c>
       <c r="F92" s="1"/>
@@ -2954,10 +2954,10 @@
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="13">
+      <c r="D93" s="11">
         <v>850.0</v>
       </c>
-      <c r="E93" s="15">
+      <c r="E93" s="13">
         <v>8.0</v>
       </c>
       <c r="F93" s="1"/>
@@ -2968,10 +2968,10 @@
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="13">
+      <c r="D94" s="11">
         <v>650.0</v>
       </c>
-      <c r="E94" s="15">
+      <c r="E94" s="13">
         <v>6.0</v>
       </c>
       <c r="F94" s="1"/>
@@ -2982,10 +2982,10 @@
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="13">
+      <c r="D95" s="11">
         <v>550.0</v>
       </c>
-      <c r="E95" s="15">
+      <c r="E95" s="13">
         <v>5.0</v>
       </c>
       <c r="F95" s="1"/>
@@ -2996,10 +2996,10 @@
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="13">
+      <c r="D96" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E96" s="15">
+      <c r="E96" s="13">
         <v>12.0</v>
       </c>
       <c r="F96" s="1"/>
@@ -3010,10 +3010,10 @@
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="13">
+      <c r="D97" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E97" s="15">
+      <c r="E97" s="13">
         <v>10.0</v>
       </c>
       <c r="F97" s="1"/>
@@ -3024,10 +3024,10 @@
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="13">
+      <c r="D98" s="11">
         <v>500.0</v>
       </c>
-      <c r="E98" s="15">
+      <c r="E98" s="13">
         <v>5.0</v>
       </c>
       <c r="F98" s="1"/>
@@ -3038,10 +3038,10 @@
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="13">
+      <c r="D99" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E99" s="15">
+      <c r="E99" s="13">
         <v>12.0</v>
       </c>
       <c r="F99" s="1"/>
@@ -3052,10 +3052,10 @@
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="13">
+      <c r="D100" s="11">
         <v>700.0</v>
       </c>
-      <c r="E100" s="15">
+      <c r="E100" s="13">
         <v>7.0</v>
       </c>
       <c r="F100" s="1"/>
@@ -3066,10 +3066,10 @@
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
-      <c r="D101" s="13">
+      <c r="D101" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E101" s="15">
+      <c r="E101" s="13">
         <v>12.0</v>
       </c>
       <c r="F101" s="1"/>
@@ -3080,10 +3080,10 @@
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
-      <c r="D102" s="13">
+      <c r="D102" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E102" s="15">
+      <c r="E102" s="13">
         <v>12.0</v>
       </c>
       <c r="F102" s="1"/>
@@ -3094,10 +3094,10 @@
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
-      <c r="D103" s="13">
+      <c r="D103" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E103" s="15">
+      <c r="E103" s="13">
         <v>12.0</v>
       </c>
       <c r="F103" s="1"/>
@@ -3108,10 +3108,10 @@
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
-      <c r="D104" s="13">
+      <c r="D104" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E104" s="15">
+      <c r="E104" s="13">
         <v>12.0</v>
       </c>
       <c r="F104" s="1"/>
@@ -3122,10 +3122,10 @@
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
-      <c r="D105" s="13">
+      <c r="D105" s="11">
         <v>900.0</v>
       </c>
-      <c r="E105" s="15">
+      <c r="E105" s="13">
         <v>9.0</v>
       </c>
       <c r="F105" s="1"/>
@@ -3136,10 +3136,10 @@
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
-      <c r="D106" s="13">
+      <c r="D106" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E106" s="15">
+      <c r="E106" s="13">
         <v>11.0</v>
       </c>
       <c r="F106" s="1"/>
@@ -3150,10 +3150,10 @@
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
-      <c r="D107" s="13">
+      <c r="D107" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E107" s="15">
+      <c r="E107" s="13">
         <v>12.0</v>
       </c>
       <c r="F107" s="1"/>
@@ -3164,10 +3164,10 @@
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
-      <c r="D108" s="13">
+      <c r="D108" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E108" s="15">
+      <c r="E108" s="13">
         <v>11.0</v>
       </c>
       <c r="F108" s="1"/>
@@ -3178,10 +3178,10 @@
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
-      <c r="D109" s="13">
+      <c r="D109" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E109" s="15">
+      <c r="E109" s="13">
         <v>12.0</v>
       </c>
       <c r="F109" s="1"/>
@@ -3192,10 +3192,10 @@
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
-      <c r="D110" s="13">
+      <c r="D110" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E110" s="15">
+      <c r="E110" s="13">
         <v>12.0</v>
       </c>
       <c r="F110" s="1"/>
@@ -3206,10 +3206,10 @@
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
-      <c r="D111" s="13">
+      <c r="D111" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E111" s="15">
+      <c r="E111" s="13">
         <v>11.0</v>
       </c>
       <c r="F111" s="1"/>
@@ -3220,10 +3220,10 @@
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
-      <c r="D112" s="13">
+      <c r="D112" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E112" s="15">
+      <c r="E112" s="13">
         <v>11.0</v>
       </c>
       <c r="F112" s="1"/>
@@ -3234,10 +3234,10 @@
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
-      <c r="D113" s="13">
+      <c r="D113" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E113" s="15">
+      <c r="E113" s="13">
         <v>11.0</v>
       </c>
       <c r="F113" s="1"/>
@@ -3248,10 +3248,10 @@
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
-      <c r="D114" s="13">
+      <c r="D114" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E114" s="15">
+      <c r="E114" s="13">
         <v>11.0</v>
       </c>
       <c r="F114" s="1"/>
@@ -3262,10 +3262,10 @@
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
-      <c r="D115" s="13">
+      <c r="D115" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E115" s="15">
+      <c r="E115" s="13">
         <v>12.0</v>
       </c>
       <c r="F115" s="1"/>
@@ -3280,10 +3280,10 @@
       <c r="C116" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D116" s="17">
+      <c r="D116" s="15">
         <v>550.0</v>
       </c>
-      <c r="E116" s="14">
+      <c r="E116" s="12">
         <v>5.0</v>
       </c>
       <c r="F116" s="1"/>
@@ -3298,10 +3298,10 @@
       <c r="C117" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D117" s="13">
+      <c r="D117" s="11">
         <v>700.0</v>
       </c>
-      <c r="E117" s="15">
+      <c r="E117" s="13">
         <v>7.0</v>
       </c>
       <c r="F117" s="1"/>
@@ -3316,10 +3316,10 @@
       <c r="C118" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D118" s="13">
+      <c r="D118" s="11">
         <v>800.0</v>
       </c>
-      <c r="E118" s="15">
+      <c r="E118" s="13">
         <v>8.0</v>
       </c>
       <c r="F118" s="1"/>
@@ -3334,10 +3334,10 @@
       <c r="C119" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D119" s="13">
+      <c r="D119" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E119" s="15">
+      <c r="E119" s="13">
         <v>12.0</v>
       </c>
       <c r="F119" s="1"/>
@@ -3352,10 +3352,10 @@
       <c r="C120" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D120" s="13">
+      <c r="D120" s="11">
         <v>700.0</v>
       </c>
-      <c r="E120" s="15">
+      <c r="E120" s="13">
         <v>7.0</v>
       </c>
       <c r="F120" s="1"/>
@@ -3370,10 +3370,10 @@
       <c r="C121" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D121" s="17">
+      <c r="D121" s="15">
         <v>1100.0</v>
       </c>
-      <c r="E121" s="14">
+      <c r="E121" s="12">
         <v>11.0</v>
       </c>
       <c r="F121" s="1"/>
@@ -3388,10 +3388,10 @@
       <c r="C122" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D122" s="13">
+      <c r="D122" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E122" s="15">
+      <c r="E122" s="13">
         <v>11.0</v>
       </c>
       <c r="F122" s="1"/>
@@ -3406,10 +3406,10 @@
       <c r="C123" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D123" s="13">
+      <c r="D123" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E123" s="15">
+      <c r="E123" s="13">
         <v>12.0</v>
       </c>
       <c r="F123" s="1"/>
@@ -3424,17 +3424,17 @@
       <c r="C124" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D124" s="13">
+      <c r="D124" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E124" s="15">
+      <c r="E124" s="13">
         <v>12.0</v>
       </c>
       <c r="F124" s="1"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3448,10 +3448,10 @@
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
-      <c r="D126" s="13">
+      <c r="D126" s="11">
         <v>850.0</v>
       </c>
-      <c r="E126" s="15">
+      <c r="E126" s="13">
         <v>8.0</v>
       </c>
       <c r="F126" s="1"/>
@@ -3462,10 +3462,10 @@
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
-      <c r="D127" s="13">
+      <c r="D127" s="11">
         <v>450.0</v>
       </c>
-      <c r="E127" s="15">
+      <c r="E127" s="13">
         <v>4.0</v>
       </c>
       <c r="F127" s="1"/>
@@ -3476,10 +3476,10 @@
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
-      <c r="D128" s="13">
+      <c r="D128" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E128" s="15">
+      <c r="E128" s="13">
         <v>12.0</v>
       </c>
       <c r="F128" s="1"/>
@@ -3490,10 +3490,10 @@
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
-      <c r="D129" s="13">
+      <c r="D129" s="11">
         <v>450.0</v>
       </c>
-      <c r="E129" s="15">
+      <c r="E129" s="13">
         <v>4.0</v>
       </c>
       <c r="F129" s="1"/>
@@ -3504,10 +3504,10 @@
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
-      <c r="D130" s="13">
+      <c r="D130" s="11">
         <v>800.0</v>
       </c>
-      <c r="E130" s="15">
+      <c r="E130" s="13">
         <v>8.0</v>
       </c>
       <c r="F130" s="1"/>
@@ -3518,10 +3518,10 @@
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
-      <c r="D131" s="13">
+      <c r="D131" s="11">
         <v>500.0</v>
       </c>
-      <c r="E131" s="15">
+      <c r="E131" s="13">
         <v>5.0</v>
       </c>
       <c r="F131" s="1"/>
@@ -3532,10 +3532,10 @@
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
-      <c r="D132" s="13">
+      <c r="D132" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E132" s="15">
+      <c r="E132" s="13">
         <v>12.0</v>
       </c>
       <c r="F132" s="1"/>
@@ -3546,10 +3546,10 @@
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
-      <c r="D133" s="13">
+      <c r="D133" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E133" s="15">
+      <c r="E133" s="13">
         <v>11.0</v>
       </c>
       <c r="F133" s="1"/>
@@ -3560,10 +3560,10 @@
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
-      <c r="D134" s="13">
+      <c r="D134" s="11">
         <v>850.0</v>
       </c>
-      <c r="E134" s="15">
+      <c r="E134" s="13">
         <v>8.0</v>
       </c>
       <c r="F134" s="1"/>
@@ -3584,10 +3584,10 @@
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
-      <c r="D136" s="13">
+      <c r="D136" s="11">
         <v>900.0</v>
       </c>
-      <c r="E136" s="15">
+      <c r="E136" s="13">
         <v>9.0</v>
       </c>
       <c r="F136" s="1"/>
@@ -3598,10 +3598,10 @@
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
-      <c r="D137" s="13">
+      <c r="D137" s="11">
         <v>300.0</v>
       </c>
-      <c r="E137" s="15">
+      <c r="E137" s="13">
         <v>3.0</v>
       </c>
       <c r="F137" s="1"/>
@@ -3612,10 +3612,10 @@
       </c>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
-      <c r="D138" s="13">
+      <c r="D138" s="11">
         <v>300.0</v>
       </c>
-      <c r="E138" s="15">
+      <c r="E138" s="13">
         <v>3.0</v>
       </c>
       <c r="F138" s="1"/>
@@ -3626,10 +3626,10 @@
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
-      <c r="D139" s="13">
+      <c r="D139" s="11">
         <v>850.0</v>
       </c>
-      <c r="E139" s="15">
+      <c r="E139" s="13">
         <v>8.0</v>
       </c>
       <c r="F139" s="1"/>
@@ -3640,10 +3640,10 @@
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
-      <c r="D140" s="13">
+      <c r="D140" s="11">
         <v>450.0</v>
       </c>
-      <c r="E140" s="15">
+      <c r="E140" s="13">
         <v>4.0</v>
       </c>
       <c r="F140" s="1"/>
@@ -3654,10 +3654,10 @@
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
-      <c r="D141" s="13">
+      <c r="D141" s="11">
         <v>250.0</v>
       </c>
-      <c r="E141" s="15">
+      <c r="E141" s="13">
         <v>2.0</v>
       </c>
       <c r="F141" s="1"/>
@@ -3668,10 +3668,10 @@
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
-      <c r="D142" s="13">
+      <c r="D142" s="11">
         <v>150.0</v>
       </c>
-      <c r="E142" s="15">
+      <c r="E142" s="13">
         <v>1.0</v>
       </c>
       <c r="F142" s="1"/>
@@ -3682,10 +3682,10 @@
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
-      <c r="D143" s="13">
+      <c r="D143" s="11">
         <v>150.0</v>
       </c>
-      <c r="E143" s="15">
+      <c r="E143" s="13">
         <v>1.0</v>
       </c>
       <c r="F143" s="1"/>
@@ -3696,10 +3696,10 @@
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
-      <c r="D144" s="13">
+      <c r="D144" s="11">
         <v>150.0</v>
       </c>
-      <c r="E144" s="15">
+      <c r="E144" s="13">
         <v>1.0</v>
       </c>
       <c r="F144" s="1"/>
@@ -3710,10 +3710,10 @@
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
-      <c r="D145" s="13">
+      <c r="D145" s="11">
         <v>150.0</v>
       </c>
-      <c r="E145" s="15">
+      <c r="E145" s="13">
         <v>1.0</v>
       </c>
       <c r="F145" s="1"/>
@@ -3724,10 +3724,10 @@
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
-      <c r="D146" s="13">
+      <c r="D146" s="11">
         <v>450.0</v>
       </c>
-      <c r="E146" s="15">
+      <c r="E146" s="13">
         <v>4.0</v>
       </c>
       <c r="F146" s="1"/>
@@ -3738,10 +3738,10 @@
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
-      <c r="D147" s="13">
+      <c r="D147" s="11">
         <v>450.0</v>
       </c>
-      <c r="E147" s="15">
+      <c r="E147" s="13">
         <v>4.0</v>
       </c>
       <c r="F147" s="1"/>
@@ -3752,10 +3752,10 @@
       </c>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
-      <c r="D148" s="13">
+      <c r="D148" s="11">
         <v>450.0</v>
       </c>
-      <c r="E148" s="15">
+      <c r="E148" s="13">
         <v>4.0</v>
       </c>
       <c r="F148" s="1"/>
@@ -3766,10 +3766,10 @@
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
-      <c r="D149" s="13">
+      <c r="D149" s="11">
         <v>500.0</v>
       </c>
-      <c r="E149" s="15">
+      <c r="E149" s="13">
         <v>5.0</v>
       </c>
       <c r="F149" s="1"/>
@@ -3780,10 +3780,10 @@
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
-      <c r="D150" s="13">
+      <c r="D150" s="11">
         <v>800.0</v>
       </c>
-      <c r="E150" s="15">
+      <c r="E150" s="13">
         <v>8.0</v>
       </c>
       <c r="F150" s="1"/>
@@ -3794,10 +3794,10 @@
       </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
-      <c r="D151" s="13">
+      <c r="D151" s="11">
         <v>850.0</v>
       </c>
-      <c r="E151" s="15">
+      <c r="E151" s="13">
         <v>8.0</v>
       </c>
       <c r="F151" s="1"/>
@@ -3808,10 +3808,10 @@
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
-      <c r="D152" s="13">
+      <c r="D152" s="11">
         <v>500.0</v>
       </c>
-      <c r="E152" s="15">
+      <c r="E152" s="13">
         <v>5.0</v>
       </c>
       <c r="F152" s="1"/>
@@ -3822,10 +3822,10 @@
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
-      <c r="D153" s="13">
+      <c r="D153" s="11">
         <v>550.0</v>
       </c>
-      <c r="E153" s="15">
+      <c r="E153" s="13">
         <v>5.0</v>
       </c>
       <c r="F153" s="1"/>
@@ -3836,10 +3836,10 @@
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
-      <c r="D154" s="13">
+      <c r="D154" s="11">
         <v>450.0</v>
       </c>
-      <c r="E154" s="15">
+      <c r="E154" s="13">
         <v>4.0</v>
       </c>
       <c r="F154" s="1"/>
@@ -3850,10 +3850,10 @@
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
-      <c r="D155" s="13">
+      <c r="D155" s="11">
         <v>650.0</v>
       </c>
-      <c r="E155" s="15">
+      <c r="E155" s="13">
         <v>6.0</v>
       </c>
       <c r="F155" s="1"/>
@@ -3864,10 +3864,10 @@
       </c>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
-      <c r="D156" s="13">
+      <c r="D156" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E156" s="15">
+      <c r="E156" s="13">
         <v>10.0</v>
       </c>
       <c r="F156" s="1"/>
@@ -3878,10 +3878,10 @@
       </c>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
-      <c r="D157" s="13">
+      <c r="D157" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E157" s="15">
+      <c r="E157" s="13">
         <v>11.0</v>
       </c>
       <c r="F157" s="1"/>
@@ -3892,10 +3892,10 @@
       </c>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
-      <c r="D158" s="13">
+      <c r="D158" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E158" s="15">
+      <c r="E158" s="13">
         <v>11.0</v>
       </c>
       <c r="F158" s="1"/>
@@ -3906,10 +3906,10 @@
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
-      <c r="D159" s="13">
+      <c r="D159" s="11">
         <v>800.0</v>
       </c>
-      <c r="E159" s="15">
+      <c r="E159" s="13">
         <v>8.0</v>
       </c>
       <c r="F159" s="1"/>
@@ -3920,10 +3920,10 @@
       </c>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
-      <c r="D160" s="13">
+      <c r="D160" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E160" s="15">
+      <c r="E160" s="13">
         <v>12.0</v>
       </c>
       <c r="F160" s="1"/>
@@ -3934,10 +3934,10 @@
       </c>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
-      <c r="D161" s="13">
+      <c r="D161" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E161" s="15">
+      <c r="E161" s="13">
         <v>11.0</v>
       </c>
       <c r="F161" s="1"/>
@@ -3948,10 +3948,10 @@
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
-      <c r="D162" s="13">
+      <c r="D162" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E162" s="15">
+      <c r="E162" s="13">
         <v>11.0</v>
       </c>
       <c r="F162" s="1"/>
@@ -3962,10 +3962,10 @@
       </c>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
-      <c r="D163" s="13">
+      <c r="D163" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E163" s="15">
+      <c r="E163" s="13">
         <v>12.0</v>
       </c>
       <c r="F163" s="1"/>
@@ -3976,10 +3976,10 @@
       </c>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
-      <c r="D164" s="13">
+      <c r="D164" s="11">
         <v>550.0</v>
       </c>
-      <c r="E164" s="15">
+      <c r="E164" s="13">
         <v>5.0</v>
       </c>
       <c r="F164" s="1"/>
@@ -3990,10 +3990,10 @@
       </c>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
-      <c r="D165" s="13">
+      <c r="D165" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E165" s="15">
+      <c r="E165" s="13">
         <v>12.0</v>
       </c>
       <c r="F165" s="1"/>
@@ -4004,10 +4004,10 @@
       </c>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
-      <c r="D166" s="13">
+      <c r="D166" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E166" s="15">
+      <c r="E166" s="13">
         <v>11.0</v>
       </c>
       <c r="F166" s="1"/>
@@ -4018,10 +4018,10 @@
       </c>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
-      <c r="D167" s="13">
+      <c r="D167" s="11">
         <v>400.0</v>
       </c>
-      <c r="E167" s="15">
+      <c r="E167" s="13">
         <v>4.0</v>
       </c>
       <c r="F167" s="1"/>
@@ -4032,10 +4032,10 @@
       </c>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
-      <c r="D168" s="13">
+      <c r="D168" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E168" s="15">
+      <c r="E168" s="13">
         <v>12.0</v>
       </c>
       <c r="F168" s="1"/>
@@ -4046,10 +4046,10 @@
       </c>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
-      <c r="D169" s="13">
+      <c r="D169" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E169" s="15">
+      <c r="E169" s="13">
         <v>11.0</v>
       </c>
       <c r="F169" s="1"/>
@@ -4060,10 +4060,10 @@
       </c>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
-      <c r="D170" s="13">
+      <c r="D170" s="11">
         <v>500.0</v>
       </c>
-      <c r="E170" s="15">
+      <c r="E170" s="13">
         <v>5.0</v>
       </c>
       <c r="F170" s="1"/>
@@ -4074,10 +4074,10 @@
       </c>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
-      <c r="D171" s="13">
+      <c r="D171" s="11">
         <v>600.0</v>
       </c>
-      <c r="E171" s="15">
+      <c r="E171" s="13">
         <v>6.0</v>
       </c>
       <c r="F171" s="1"/>
@@ -4088,10 +4088,10 @@
       </c>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
-      <c r="D172" s="13">
+      <c r="D172" s="11">
         <v>900.0</v>
       </c>
-      <c r="E172" s="15">
+      <c r="E172" s="13">
         <v>9.0</v>
       </c>
       <c r="F172" s="1"/>
@@ -4102,10 +4102,10 @@
       </c>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
-      <c r="D173" s="13">
+      <c r="D173" s="11">
         <v>900.0</v>
       </c>
-      <c r="E173" s="15">
+      <c r="E173" s="13">
         <v>9.0</v>
       </c>
       <c r="F173" s="1"/>
@@ -4116,10 +4116,10 @@
       </c>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
-      <c r="D174" s="13">
+      <c r="D174" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E174" s="15">
+      <c r="E174" s="13">
         <v>11.0</v>
       </c>
       <c r="F174" s="1"/>
@@ -4130,10 +4130,10 @@
       </c>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
-      <c r="D175" s="13">
+      <c r="D175" s="11">
         <v>900.0</v>
       </c>
-      <c r="E175" s="15">
+      <c r="E175" s="13">
         <v>9.0</v>
       </c>
       <c r="F175" s="1"/>
@@ -4144,10 +4144,10 @@
       </c>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
-      <c r="D176" s="13">
+      <c r="D176" s="11">
         <v>550.0</v>
       </c>
-      <c r="E176" s="15">
+      <c r="E176" s="13">
         <v>5.0</v>
       </c>
       <c r="F176" s="1"/>
@@ -4158,10 +4158,10 @@
       </c>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
-      <c r="D177" s="13">
+      <c r="D177" s="11">
         <v>550.0</v>
       </c>
-      <c r="E177" s="15">
+      <c r="E177" s="13">
         <v>5.0</v>
       </c>
       <c r="F177" s="1"/>
@@ -4172,10 +4172,10 @@
       </c>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
-      <c r="D178" s="13">
+      <c r="D178" s="11">
         <v>800.0</v>
       </c>
-      <c r="E178" s="15">
+      <c r="E178" s="13">
         <v>8.0</v>
       </c>
       <c r="F178" s="1"/>
@@ -4186,10 +4186,10 @@
       </c>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
-      <c r="D179" s="13">
+      <c r="D179" s="11">
         <v>800.0</v>
       </c>
-      <c r="E179" s="15">
+      <c r="E179" s="13">
         <v>8.0</v>
       </c>
       <c r="F179" s="1"/>
@@ -4200,10 +4200,10 @@
       </c>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
-      <c r="D180" s="13">
+      <c r="D180" s="11">
         <v>950.0</v>
       </c>
-      <c r="E180" s="15">
+      <c r="E180" s="13">
         <v>9.0</v>
       </c>
       <c r="F180" s="1"/>
@@ -4214,10 +4214,10 @@
       </c>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
-      <c r="D181" s="13">
+      <c r="D181" s="11">
         <v>950.0</v>
       </c>
-      <c r="E181" s="15">
+      <c r="E181" s="13">
         <v>9.0</v>
       </c>
       <c r="F181" s="1"/>
@@ -4228,10 +4228,10 @@
       </c>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
-      <c r="D182" s="13">
+      <c r="D182" s="11">
         <v>150.0</v>
       </c>
-      <c r="E182" s="15">
+      <c r="E182" s="13">
         <v>1.0</v>
       </c>
       <c r="F182" s="1"/>
@@ -4242,10 +4242,10 @@
       </c>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
-      <c r="D183" s="13">
+      <c r="D183" s="11">
         <v>550.0</v>
       </c>
-      <c r="E183" s="15">
+      <c r="E183" s="13">
         <v>5.0</v>
       </c>
       <c r="F183" s="1"/>
@@ -4256,10 +4256,10 @@
       </c>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
-      <c r="D184" s="13">
+      <c r="D184" s="11">
         <v>600.0</v>
       </c>
-      <c r="E184" s="15">
+      <c r="E184" s="13">
         <v>6.0</v>
       </c>
       <c r="F184" s="1"/>
@@ -4270,10 +4270,10 @@
       </c>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
-      <c r="D185" s="13">
+      <c r="D185" s="11">
         <v>200.0</v>
       </c>
-      <c r="E185" s="15">
+      <c r="E185" s="13">
         <v>2.0</v>
       </c>
       <c r="F185" s="1"/>
@@ -4284,10 +4284,10 @@
       </c>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
-      <c r="D186" s="13">
+      <c r="D186" s="11">
         <v>600.0</v>
       </c>
-      <c r="E186" s="15">
+      <c r="E186" s="13">
         <v>6.0</v>
       </c>
       <c r="F186" s="1"/>
@@ -4298,10 +4298,10 @@
       </c>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
-      <c r="D187" s="13">
+      <c r="D187" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E187" s="15">
+      <c r="E187" s="13">
         <v>11.0</v>
       </c>
       <c r="F187" s="1"/>
@@ -4312,10 +4312,10 @@
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
-      <c r="D188" s="13">
+      <c r="D188" s="11">
         <v>900.0</v>
       </c>
-      <c r="E188" s="15">
+      <c r="E188" s="13">
         <v>9.0</v>
       </c>
       <c r="F188" s="1"/>
@@ -4326,10 +4326,10 @@
       </c>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
-      <c r="D189" s="13">
+      <c r="D189" s="11">
         <v>300.0</v>
       </c>
-      <c r="E189" s="15">
+      <c r="E189" s="13">
         <v>3.0</v>
       </c>
       <c r="F189" s="1"/>
@@ -4340,10 +4340,10 @@
       </c>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
-      <c r="D190" s="13">
+      <c r="D190" s="11">
         <v>550.0</v>
       </c>
-      <c r="E190" s="15">
+      <c r="E190" s="13">
         <v>5.0</v>
       </c>
       <c r="F190" s="1"/>
@@ -4354,10 +4354,10 @@
       </c>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
-      <c r="D191" s="13">
+      <c r="D191" s="11">
         <v>550.0</v>
       </c>
-      <c r="E191" s="15">
+      <c r="E191" s="13">
         <v>5.0</v>
       </c>
       <c r="F191" s="1"/>
@@ -4368,10 +4368,10 @@
       </c>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
-      <c r="D192" s="13">
+      <c r="D192" s="11">
         <v>550.0</v>
       </c>
-      <c r="E192" s="15">
+      <c r="E192" s="13">
         <v>5.0</v>
       </c>
       <c r="F192" s="1"/>
@@ -4382,10 +4382,10 @@
       </c>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
-      <c r="D193" s="13">
+      <c r="D193" s="11">
         <v>400.0</v>
       </c>
-      <c r="E193" s="15">
+      <c r="E193" s="13">
         <v>4.0</v>
       </c>
       <c r="F193" s="1"/>
@@ -4396,10 +4396,10 @@
       </c>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
-      <c r="D194" s="13">
+      <c r="D194" s="11">
         <v>500.0</v>
       </c>
-      <c r="E194" s="15">
+      <c r="E194" s="13">
         <v>5.0</v>
       </c>
       <c r="F194" s="1"/>
@@ -4410,10 +4410,10 @@
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
-      <c r="D195" s="13">
+      <c r="D195" s="11">
         <v>950.0</v>
       </c>
-      <c r="E195" s="15">
+      <c r="E195" s="13">
         <v>9.0</v>
       </c>
       <c r="F195" s="1"/>
@@ -4424,10 +4424,10 @@
       </c>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
-      <c r="D196" s="13">
+      <c r="D196" s="11">
         <v>500.0</v>
       </c>
-      <c r="E196" s="15">
+      <c r="E196" s="13">
         <v>5.0</v>
       </c>
       <c r="F196" s="1"/>
@@ -4438,10 +4438,10 @@
       </c>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
-      <c r="D197" s="13">
+      <c r="D197" s="11">
         <v>500.0</v>
       </c>
-      <c r="E197" s="15">
+      <c r="E197" s="13">
         <v>5.0</v>
       </c>
       <c r="F197" s="1"/>
@@ -4452,10 +4452,10 @@
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
-      <c r="D198" s="13">
+      <c r="D198" s="11">
         <v>350.0</v>
       </c>
-      <c r="E198" s="15">
+      <c r="E198" s="13">
         <v>3.0</v>
       </c>
       <c r="F198" s="1"/>
@@ -4466,10 +4466,10 @@
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
-      <c r="D199" s="13">
+      <c r="D199" s="11">
         <v>950.0</v>
       </c>
-      <c r="E199" s="15">
+      <c r="E199" s="13">
         <v>9.0</v>
       </c>
       <c r="F199" s="1"/>
@@ -4480,10 +4480,10 @@
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
-      <c r="D200" s="13">
+      <c r="D200" s="11">
         <v>150.0</v>
       </c>
-      <c r="E200" s="15">
+      <c r="E200" s="13">
         <v>1.0</v>
       </c>
       <c r="F200" s="1"/>
@@ -4494,10 +4494,10 @@
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
-      <c r="D201" s="13">
+      <c r="D201" s="11">
         <v>950.0</v>
       </c>
-      <c r="E201" s="15">
+      <c r="E201" s="13">
         <v>9.0</v>
       </c>
       <c r="F201" s="1"/>
@@ -4508,10 +4508,10 @@
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
-      <c r="D202" s="13">
+      <c r="D202" s="11">
         <v>150.0</v>
       </c>
-      <c r="E202" s="15">
+      <c r="E202" s="13">
         <v>1.0</v>
       </c>
       <c r="F202" s="1"/>
@@ -4522,10 +4522,10 @@
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
-      <c r="D203" s="13">
+      <c r="D203" s="11">
         <v>600.0</v>
       </c>
-      <c r="E203" s="15">
+      <c r="E203" s="13">
         <v>6.0</v>
       </c>
       <c r="F203" s="1"/>
@@ -4536,10 +4536,10 @@
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
-      <c r="D204" s="13">
+      <c r="D204" s="11">
         <v>550.0</v>
       </c>
-      <c r="E204" s="15">
+      <c r="E204" s="13">
         <v>5.0</v>
       </c>
       <c r="F204" s="1"/>
@@ -4550,10 +4550,10 @@
       </c>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
-      <c r="D205" s="13">
+      <c r="D205" s="11">
         <v>700.0</v>
       </c>
-      <c r="E205" s="15">
+      <c r="E205" s="13">
         <v>7.0</v>
       </c>
       <c r="F205" s="1"/>
@@ -4564,10 +4564,10 @@
       </c>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
-      <c r="D206" s="13">
+      <c r="D206" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E206" s="16">
+      <c r="E206" s="14">
         <v>10.0</v>
       </c>
       <c r="F206" s="1"/>
@@ -4578,10 +4578,10 @@
       </c>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
-      <c r="D207" s="13">
+      <c r="D207" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E207" s="14">
+      <c r="E207" s="12">
         <v>10.0</v>
       </c>
       <c r="F207" s="1"/>
@@ -4592,10 +4592,10 @@
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
-      <c r="D208" s="13">
+      <c r="D208" s="11">
         <v>500.0</v>
       </c>
-      <c r="E208" s="15">
+      <c r="E208" s="13">
         <v>5.0</v>
       </c>
       <c r="F208" s="1"/>
@@ -4606,10 +4606,10 @@
       </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
-      <c r="D209" s="13">
+      <c r="D209" s="11">
         <v>250.0</v>
       </c>
-      <c r="E209" s="15">
+      <c r="E209" s="13">
         <v>2.0</v>
       </c>
       <c r="F209" s="1"/>
@@ -4620,10 +4620,10 @@
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
-      <c r="D210" s="13">
+      <c r="D210" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E210" s="15">
+      <c r="E210" s="13">
         <v>10.0</v>
       </c>
       <c r="F210" s="1"/>
@@ -4634,10 +4634,10 @@
       </c>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
-      <c r="D211" s="13">
+      <c r="D211" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E211" s="15">
+      <c r="E211" s="13">
         <v>10.0</v>
       </c>
       <c r="F211" s="1"/>
@@ -4648,10 +4648,10 @@
       </c>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
-      <c r="D212" s="13">
+      <c r="D212" s="11">
         <v>1000.0</v>
       </c>
-      <c r="E212" s="15">
+      <c r="E212" s="13">
         <v>10.0</v>
       </c>
       <c r="F212" s="1"/>
@@ -4662,10 +4662,10 @@
       </c>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
-      <c r="D213" s="13">
+      <c r="D213" s="11">
         <v>500.0</v>
       </c>
-      <c r="E213" s="15">
+      <c r="E213" s="13">
         <v>5.0</v>
       </c>
       <c r="F213" s="1"/>
@@ -4679,7 +4679,7 @@
       <c r="D214" s="21">
         <v>900.0</v>
       </c>
-      <c r="E214" s="16">
+      <c r="E214" s="14">
         <v>9.0</v>
       </c>
       <c r="F214" s="1"/>
@@ -4690,10 +4690,10 @@
       </c>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
-      <c r="D215" s="13">
+      <c r="D215" s="11">
         <v>300.0</v>
       </c>
-      <c r="E215" s="15">
+      <c r="E215" s="13">
         <v>3.0</v>
       </c>
       <c r="F215" s="1"/>
@@ -4704,10 +4704,10 @@
       </c>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
-      <c r="D216" s="13">
+      <c r="D216" s="11">
         <v>400.0</v>
       </c>
-      <c r="E216" s="15">
+      <c r="E216" s="13">
         <v>4.0</v>
       </c>
       <c r="F216" s="1"/>
@@ -4718,10 +4718,10 @@
       </c>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
-      <c r="D217" s="13">
+      <c r="D217" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E217" s="15">
+      <c r="E217" s="13">
         <v>12.0</v>
       </c>
       <c r="F217" s="1"/>
@@ -4732,10 +4732,10 @@
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
-      <c r="D218" s="13">
+      <c r="D218" s="11">
         <v>450.0</v>
       </c>
-      <c r="E218" s="15">
+      <c r="E218" s="13">
         <v>4.0</v>
       </c>
       <c r="F218" s="1"/>
@@ -4746,10 +4746,10 @@
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
-      <c r="D219" s="13">
+      <c r="D219" s="11">
         <v>250.0</v>
       </c>
-      <c r="E219" s="15">
+      <c r="E219" s="13">
         <v>2.0</v>
       </c>
       <c r="F219" s="1"/>
@@ -4760,10 +4760,10 @@
       </c>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
-      <c r="D220" s="13">
+      <c r="D220" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E220" s="15">
+      <c r="E220" s="13">
         <v>12.0</v>
       </c>
       <c r="F220" s="1"/>
@@ -4774,10 +4774,10 @@
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
-      <c r="D221" s="13">
+      <c r="D221" s="11">
         <v>900.0</v>
       </c>
-      <c r="E221" s="15">
+      <c r="E221" s="13">
         <v>9.0</v>
       </c>
       <c r="F221" s="1"/>
@@ -4788,10 +4788,10 @@
       </c>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
-      <c r="D222" s="13">
+      <c r="D222" s="11">
         <v>700.0</v>
       </c>
-      <c r="E222" s="15">
+      <c r="E222" s="13">
         <v>7.0</v>
       </c>
       <c r="F222" s="1"/>
@@ -4812,10 +4812,10 @@
       </c>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
-      <c r="D224" s="13">
+      <c r="D224" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E224" s="15">
+      <c r="E224" s="13">
         <v>12.0</v>
       </c>
       <c r="F224" s="1"/>
@@ -4836,10 +4836,10 @@
       </c>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
-      <c r="D226" s="13">
+      <c r="D226" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E226" s="15">
+      <c r="E226" s="13">
         <v>12.0</v>
       </c>
       <c r="F226" s="1"/>
@@ -4850,10 +4850,10 @@
       </c>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
-      <c r="D227" s="13">
+      <c r="D227" s="11">
         <v>450.0</v>
       </c>
-      <c r="E227" s="15">
+      <c r="E227" s="13">
         <v>4.0</v>
       </c>
       <c r="F227" s="1"/>
@@ -4874,10 +4874,10 @@
       </c>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
-      <c r="D229" s="13">
+      <c r="D229" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E229" s="15">
+      <c r="E229" s="13">
         <v>12.0</v>
       </c>
       <c r="F229" s="1"/>
@@ -4888,10 +4888,10 @@
       </c>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
-      <c r="D230" s="13">
+      <c r="D230" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E230" s="15">
+      <c r="E230" s="13">
         <v>12.0</v>
       </c>
       <c r="F230" s="1"/>
@@ -4902,10 +4902,10 @@
       </c>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
-      <c r="D231" s="13">
+      <c r="D231" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E231" s="15">
+      <c r="E231" s="13">
         <v>12.0</v>
       </c>
       <c r="F231" s="1"/>
@@ -4916,10 +4916,10 @@
       </c>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
-      <c r="D232" s="13">
+      <c r="D232" s="11">
         <v>550.0</v>
       </c>
-      <c r="E232" s="15">
+      <c r="E232" s="13">
         <v>5.0</v>
       </c>
       <c r="F232" s="1"/>
@@ -4930,10 +4930,10 @@
       </c>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
-      <c r="D233" s="13">
+      <c r="D233" s="11">
         <v>900.0</v>
       </c>
-      <c r="E233" s="15">
+      <c r="E233" s="13">
         <v>9.0</v>
       </c>
       <c r="F233" s="1"/>
@@ -4944,10 +4944,10 @@
       </c>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
-      <c r="D234" s="13">
+      <c r="D234" s="11">
         <v>850.0</v>
       </c>
-      <c r="E234" s="15">
+      <c r="E234" s="13">
         <v>8.0</v>
       </c>
       <c r="F234" s="1"/>
@@ -4958,10 +4958,10 @@
       </c>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
-      <c r="D235" s="13">
+      <c r="D235" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E235" s="15">
+      <c r="E235" s="13">
         <v>11.0</v>
       </c>
       <c r="F235" s="1"/>
@@ -4972,10 +4972,10 @@
       </c>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
-      <c r="D236" s="13">
+      <c r="D236" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E236" s="15">
+      <c r="E236" s="13">
         <v>12.0</v>
       </c>
       <c r="F236" s="1"/>
@@ -4986,10 +4986,10 @@
       </c>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
-      <c r="D237" s="13">
+      <c r="D237" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E237" s="15">
+      <c r="E237" s="13">
         <v>12.0</v>
       </c>
       <c r="F237" s="1"/>
@@ -5000,10 +5000,10 @@
       </c>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
-      <c r="D238" s="13">
+      <c r="D238" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E238" s="15">
+      <c r="E238" s="13">
         <v>12.0</v>
       </c>
       <c r="F238" s="1"/>
@@ -5014,10 +5014,10 @@
       </c>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
-      <c r="D239" s="13">
+      <c r="D239" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E239" s="15">
+      <c r="E239" s="13">
         <v>12.0</v>
       </c>
       <c r="F239" s="1"/>
@@ -5028,10 +5028,10 @@
       </c>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
-      <c r="D240" s="13">
+      <c r="D240" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E240" s="15">
+      <c r="E240" s="13">
         <v>12.0</v>
       </c>
       <c r="F240" s="1"/>
@@ -5042,10 +5042,10 @@
       </c>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
-      <c r="D241" s="13">
+      <c r="D241" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E241" s="15">
+      <c r="E241" s="13">
         <v>12.0</v>
       </c>
       <c r="F241" s="1"/>
@@ -5056,10 +5056,10 @@
       </c>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
-      <c r="D242" s="13">
+      <c r="D242" s="11">
         <v>1250.0</v>
       </c>
-      <c r="E242" s="15">
+      <c r="E242" s="13">
         <v>12.0</v>
       </c>
       <c r="F242" s="1"/>
@@ -5070,10 +5070,10 @@
       </c>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
-      <c r="D243" s="13">
+      <c r="D243" s="11">
         <v>800.0</v>
       </c>
-      <c r="E243" s="15">
+      <c r="E243" s="13">
         <v>8.0</v>
       </c>
       <c r="F243" s="1"/>
@@ -5084,10 +5084,10 @@
       </c>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
-      <c r="D244" s="13">
+      <c r="D244" s="11">
         <v>1200.0</v>
       </c>
-      <c r="E244" s="15">
+      <c r="E244" s="13">
         <v>12.0</v>
       </c>
       <c r="F244" s="1"/>
@@ -5101,7 +5101,7 @@
       <c r="D245" s="21">
         <v>700.0</v>
       </c>
-      <c r="E245" s="16">
+      <c r="E245" s="14">
         <v>7.0</v>
       </c>
       <c r="F245" s="1"/>
@@ -5112,10 +5112,10 @@
       </c>
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
-      <c r="D246" s="13">
+      <c r="D246" s="11">
         <v>1100.0</v>
       </c>
-      <c r="E246" s="15">
+      <c r="E246" s="13">
         <v>11.0</v>
       </c>
       <c r="F246" s="1"/>
@@ -5175,16 +5175,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -5192,13 +5192,13 @@
         <v>8000.0</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -5206,13 +5206,13 @@
         <v>8000.0</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -5220,13 +5220,13 @@
         <v>8000.0</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -5234,13 +5234,13 @@
         <v>8000.0</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -5248,13 +5248,13 @@
         <v>8000.0</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5262,13 +5262,13 @@
         <v>8000.0</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="B8" s="1">
         <v>1.5632496E12</v>
@@ -5278,13 +5278,13 @@
         <v>8000.0</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="B9" s="1">
         <v>1.56204E12</v>
@@ -5294,13 +5294,13 @@
         <v>8000.0</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B10" s="1">
         <v>1.5658416E12</v>
@@ -5310,13 +5310,13 @@
         <v>8000.0</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="B11" s="1">
         <v>1.5667056E12</v>
@@ -5326,13 +5326,13 @@
         <v>8000.0</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="B12" s="1">
         <v>1.5649776E12</v>
@@ -5342,13 +5342,13 @@
         <v>8000.0</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -5356,13 +5356,13 @@
         <v>8000.0</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -5370,13 +5370,13 @@
         <v>8000.0</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -5384,13 +5384,13 @@
         <v>8000.0</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -5398,13 +5398,13 @@
         <v>8000.0</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -5412,13 +5412,13 @@
         <v>8000.0</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -5426,13 +5426,13 @@
         <v>8000.0</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -5440,13 +5440,13 @@
         <v>8000.0</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -5454,13 +5454,13 @@
         <v>8000.0</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -5468,13 +5468,13 @@
         <v>8000.0</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -5482,13 +5482,13 @@
         <v>8000.0</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -5496,13 +5496,13 @@
         <v>8000.0</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -5510,7 +5510,7 @@
         <v>8000.0</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="F24" s="1"/>
     </row>

</xml_diff>

<commit_message>
fix terms of service/privacypolicy buttons and settings helpcrow button
</commit_message>
<xml_diff>
--- a/Dictionaries/store.xlsx
+++ b/Dictionaries/store.xlsx
@@ -32,19 +32,43 @@
     <t>gold</t>
   </si>
   <si>
+    <t>silver1</t>
+  </si>
+  <si>
+    <t>silver2</t>
+  </si>
+  <si>
+    <t>consumable_alignmentBoosterSmaller</t>
+  </si>
+  <si>
     <t>bundle_abondiasBest</t>
   </si>
   <si>
+    <t>consumable_alignmentBoosterMedium</t>
+  </si>
+  <si>
     <t>bundle_sapphosChoice</t>
   </si>
   <si>
+    <t>consumable_alignmentBoosterGreater</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterSmaller</t>
+  </si>
+  <si>
+    <t>consumable_xpBoosterMedium</t>
+  </si>
+  <si>
     <t>bundle_hermeticCollection</t>
   </si>
   <si>
-    <t>silver1</t>
-  </si>
-  <si>
-    <t>silver2</t>
+    <t>consumable_xpBoosterGreater</t>
+  </si>
+  <si>
+    <t>consumable_invisible</t>
+  </si>
+  <si>
+    <t>consumable_truesight</t>
   </si>
   <si>
     <t>silver3</t>
@@ -65,88 +89,136 @@
     <t>shop_locked_wndg</t>
   </si>
   <si>
+    <t>cosmetic_f_S_HHO</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_HKO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_HLO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_SNOWQUEEN</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_BARGHEST</t>
   </si>
   <si>
     <t>shop_locked_barg</t>
   </si>
   <si>
+    <t>cosmetic_f_S_LILYOV</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_MIDSUMMER</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_CATSIDHE</t>
   </si>
   <si>
+    <t>cosmetic_f_S_THUNDERMOON</t>
+  </si>
+  <si>
     <t>shop_locked_sidh</t>
   </si>
   <si>
     <t>cosmetic_f_PF_GRINDYLOW</t>
   </si>
   <si>
+    <t>cosmetic_f_S_ECLIPSE</t>
+  </si>
+  <si>
     <t>shop_locked_grdlw</t>
   </si>
   <si>
     <t>cosmetic_f_PF_SENTINALOWL</t>
   </si>
   <si>
+    <t>cosmetic_f_S_CORNMOON</t>
+  </si>
+  <si>
     <t>shop_locked_owl</t>
   </si>
   <si>
+    <t>cosmetic_f_S_BRNNGWTCH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_CALYPSO</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_DWO</t>
   </si>
   <si>
+    <t>_</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_HDWO</t>
   </si>
   <si>
-    <t>consumable_alignmentBoosterSmaller</t>
-  </si>
-  <si>
-    <t>consumable_alignmentBoosterMedium</t>
-  </si>
-  <si>
-    <t>consumable_alignmentBoosterGreater</t>
-  </si>
-  <si>
-    <t>consumable_xpBoosterSmaller</t>
+    <t>cosmetic_m_S_HKO</t>
   </si>
   <si>
     <t>cosmetic_f_HE_HBH</t>
   </si>
   <si>
+    <t>cosmetic_m_S_HHO</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_HBO</t>
   </si>
   <si>
-    <t>consumable_xpBoosterMedium</t>
+    <t>cosmetic_m_S_HLO</t>
   </si>
   <si>
     <t>cosmetic_f_HE_HHO</t>
   </si>
   <si>
+    <t>cosmetic_m_S_JACKFROST</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_HNO</t>
   </si>
   <si>
+    <t>cosmetic_m_S_MIDSUMMER</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_CEH</t>
   </si>
   <si>
-    <t>consumable_xpBoosterGreater</t>
-  </si>
-  <si>
     <t>cosmetic_f_HE_CES</t>
   </si>
   <si>
+    <t>cosmetic_m_S_CORNMOON</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_FLOWER</t>
   </si>
   <si>
+    <t>cosmetic_m_S_CALYPSO</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_BDH</t>
   </si>
   <si>
     <t>shop_locked_rrc</t>
   </si>
   <si>
+    <t>cosmetic_m_S_FIREDANCER</t>
+  </si>
+  <si>
     <t>cosmetic_f_HA_DWO</t>
   </si>
   <si>
-    <t>consumable_invisible</t>
-  </si>
-  <si>
-    <t>consumable_truesight</t>
+    <t>cosmetic_m_S_BRNNGWTCH</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_ECLIPSE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_THUNDERMOON</t>
   </si>
   <si>
     <t>cosmetic_f_HA_FKFO</t>
@@ -278,147 +350,90 @@
     <t>cosmetic_f_L_KSO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HHO</t>
-  </si>
-  <si>
     <t>cosmetic_f_L_PPS</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>cosmetic_f_L_LS</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HKO</t>
-  </si>
-  <si>
     <t>cosmetic_f_L_SS</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HLO</t>
-  </si>
-  <si>
     <t>cosmetic_f_L_TIGHT</t>
   </si>
   <si>
     <t>cosmetic_f_L_HEAVYSKIRT</t>
   </si>
   <si>
-    <t>cosmetic_f_S_SNOWQUEEN</t>
-  </si>
-  <si>
     <t>cosmetic_f_L_SHORTS</t>
   </si>
   <si>
     <t>cosmetic_f_L_ROMPER</t>
   </si>
   <si>
-    <t>cosmetic_f_S_LILYOV</t>
-  </si>
-  <si>
     <t>cosmetic_f_L_LACELEG</t>
   </si>
   <si>
-    <t>cosmetic_f_S_MIDSUMMER</t>
-  </si>
-  <si>
     <t>cosmetic_f_F_BDWO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_THUNDERMOON</t>
-  </si>
-  <si>
     <t>cosmetic_f_F_SBDWO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_ECLIPSE</t>
-  </si>
-  <si>
     <t>cosmetic_f_F_SDWO</t>
   </si>
   <si>
     <t>cosmetic_f_F_KFO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_CORNMOON</t>
-  </si>
-  <si>
     <t>cosmetic_f_F_KSO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_BRNNGWTCH</t>
-  </si>
-  <si>
     <t>cosmetic_f_F_TIED</t>
   </si>
   <si>
-    <t>cosmetic_f_S_CALYPSO</t>
-  </si>
-  <si>
     <t>cosmetic_f_F_BOW</t>
   </si>
   <si>
     <t>cosmetic_f_F_FUR</t>
   </si>
   <si>
-    <t>_</t>
-  </si>
-  <si>
     <t>cosmetic_f_CR_DWO</t>
   </si>
   <si>
     <t>shop_locked_beta</t>
   </si>
   <si>
-    <t>cosmetic_m_S_HKO</t>
-  </si>
-  <si>
     <t>cosmetic_f_CR_DSO</t>
   </si>
   <si>
     <t>cosmetic_f_CR_DTO</t>
   </si>
   <si>
-    <t>cosmetic_m_S_HHO</t>
-  </si>
-  <si>
     <t>cosmetic_f_CR_PRIMAVERA</t>
   </si>
   <si>
     <t>cosmetic_f_CR_KIM</t>
   </si>
   <si>
-    <t>cosmetic_m_S_HLO</t>
-  </si>
-  <si>
     <t>shop_locked_top</t>
   </si>
   <si>
     <t>cosmetic_f_CR_SMMRSOL</t>
   </si>
   <si>
-    <t>cosmetic_m_S_JACKFROST</t>
-  </si>
-  <si>
     <t>cosmetic_f_CR_SHADOW</t>
   </si>
   <si>
     <t>shop_locked_shadow</t>
   </si>
   <si>
-    <t>cosmetic_m_S_MIDSUMMER</t>
-  </si>
-  <si>
     <t>cosmetic_f_CR_GRAY</t>
   </si>
   <si>
     <t>shop_locked_gray</t>
   </si>
   <si>
-    <t>cosmetic_m_S_CORNMOON</t>
-  </si>
-  <si>
     <t>cosmetic_f_CR_WHITE</t>
   </si>
   <si>
@@ -428,34 +443,19 @@
     <t>cosmetic_f_SF_HSF</t>
   </si>
   <si>
-    <t>cosmetic_m_S_CALYPSO</t>
-  </si>
-  <si>
     <t>cosmetic_f_SF_HSS</t>
   </si>
   <si>
-    <t>cosmetic_m_S_FIREDANCER</t>
-  </si>
-  <si>
     <t>cosmetic_f_SF_HST</t>
   </si>
   <si>
-    <t>cosmetic_m_S_BRNNGWTCH</t>
-  </si>
-  <si>
     <t>cosmetic_f_SF_GLSS</t>
   </si>
   <si>
-    <t>cosmetic_m_S_ECLIPSE</t>
-  </si>
-  <si>
     <t>cosmetic_f_SF_HOOPS</t>
   </si>
   <si>
     <t>cosmetic_f_SS_CROWSKULL</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_THUNDERMOON</t>
   </si>
   <si>
     <t>cosmetic_f_SS_HAT</t>
@@ -987,6 +987,15 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
@@ -1005,14 +1014,11 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -1028,12 +1034,6 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -1120,47 +1120,47 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="4">
+      <c r="D2" s="7">
         <v>300.0</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="6">
+      <c r="D3" s="9">
         <v>300.0</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="4">
+      <c r="D4" s="7">
         <v>300.0</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
@@ -1168,7 +1168,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="8"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
@@ -1176,7 +1176,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="8"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
@@ -1184,7 +1184,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1192,7 +1192,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="8"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1200,7 +1200,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1208,7 +1208,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1216,7 +1216,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="8"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1224,7 +1224,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1232,7 +1232,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1240,7 +1240,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1287,147 +1287,147 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="4">
+      <c r="D2" s="7">
         <v>100.0</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="4"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="6">
+      <c r="D3" s="9">
         <v>300.0</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="4">
+      <c r="D4" s="7">
         <v>500.0</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="6">
+      <c r="D5" s="9">
         <v>100.0</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="4">
+      <c r="D6" s="7">
         <v>300.0</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="6">
+      <c r="D7" s="9">
         <v>500.0</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="4">
+      <c r="D8" s="7">
         <v>200.0</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="16">
+      <c r="D9" s="11">
         <v>200.0</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="8"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1474,71 +1474,71 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="8"/>
+      <c r="E2" s="4"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="8"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="8"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="8"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="8"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1546,7 +1546,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="8"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1554,7 +1554,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1562,7 +1562,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1570,7 +1570,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="8"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1578,7 +1578,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1586,7 +1586,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1594,7 +1594,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1641,332 +1641,332 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="11">
+        <v>23</v>
+      </c>
+      <c r="D2" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="14">
         <v>10.0</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="11">
+        <v>30</v>
+      </c>
+      <c r="D3" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="15">
         <v>10.0</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="11">
+        <v>35</v>
+      </c>
+      <c r="D4" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="15">
         <v>10.0</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="11">
+        <v>38</v>
+      </c>
+      <c r="D5" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="15">
         <v>10.0</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="11">
+        <v>41</v>
+      </c>
+      <c r="D6" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="16">
         <v>10.0</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="11">
+      <c r="D7" s="13">
         <v>800.0</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="14">
         <v>8.0</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="11">
+      <c r="D8" s="13">
         <v>900.0</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="15">
         <v>9.0</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="11">
+      <c r="D9" s="13">
         <v>850.0</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="15">
         <v>8.0</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="11">
+      <c r="D10" s="13">
         <v>500.0</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="15">
         <v>5.0</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="11">
+      <c r="D11" s="13">
         <v>600.0</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="15">
         <v>6.0</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="11">
+      <c r="D12" s="13">
         <v>800.0</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="15">
         <v>8.0</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="11">
+      <c r="D13" s="13">
         <v>850.0</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="15">
         <v>8.0</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="11">
+      <c r="D14" s="13">
         <v>850.0</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="15">
         <v>8.0</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="11">
+      <c r="D15" s="13">
         <v>500.0</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="15">
         <v>5.0</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="11">
+        <v>62</v>
+      </c>
+      <c r="D16" s="13">
         <v>900.0</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="15">
         <v>9.0</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="15">
+      <c r="D17" s="17">
         <v>300.0</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="14">
         <v>3.0</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="11">
+      <c r="D18" s="13">
         <v>450.0</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="15">
         <v>4.0</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="11">
+      <c r="D19" s="13">
         <v>450.0</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="15">
         <v>4.0</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="11">
+      <c r="D20" s="13">
         <v>300.0</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="15">
         <v>3.0</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="11">
+      <c r="D21" s="13">
         <v>500.0</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="15">
         <v>5.0</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="11">
+      <c r="D22" s="13">
         <v>550.0</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="15">
         <v>5.0</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1980,956 +1980,956 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="11">
+      <c r="D24" s="13">
         <v>450.0</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="15">
         <v>4.0</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="11">
+      <c r="D25" s="13">
         <v>400.0</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="15">
         <v>4.0</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="11">
+      <c r="D26" s="13">
         <v>300.0</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="15">
         <v>3.0</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="11">
+      <c r="D27" s="13">
         <v>500.0</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="15">
         <v>5.0</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="11">
+      <c r="D28" s="13">
         <v>350.0</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="15">
         <v>3.0</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="11">
+      <c r="D29" s="13">
         <v>300.0</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="15">
         <v>3.0</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="11">
+      <c r="D30" s="13">
         <v>250.0</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="15">
         <v>2.0</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="11">
+      <c r="D31" s="13">
         <v>250.0</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="15">
         <v>2.0</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="11">
+      <c r="D32" s="13">
         <v>250.0</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="15">
         <v>2.0</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="11">
+      <c r="D33" s="13">
         <v>250.0</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="15">
         <v>2.0</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="11">
+      <c r="D34" s="13">
         <v>250.0</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="15">
         <v>2.0</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="11">
+      <c r="D35" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="15">
         <v>12.0</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="11">
+      <c r="D36" s="13">
         <v>950.0</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="15">
         <v>9.0</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="11">
+      <c r="D37" s="13">
         <v>950.0</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="15">
         <v>9.0</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="11">
+      <c r="D38" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="15">
         <v>12.0</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="11">
+      <c r="D39" s="13">
         <v>950.0</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="15">
         <v>9.0</v>
       </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="11">
+      <c r="D40" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="15">
         <v>12.0</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="11">
+      <c r="D41" s="13">
         <v>900.0</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="15">
         <v>9.0</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="11">
+      <c r="D42" s="13">
         <v>950.0</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="15">
         <v>9.0</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="11">
+      <c r="D43" s="13">
         <v>900.0</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="15">
         <v>9.0</v>
       </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="11">
+      <c r="D44" s="13">
         <v>950.0</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="15">
         <v>9.0</v>
       </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="11">
+      <c r="D45" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="15">
         <v>12.0</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="11">
+      <c r="D46" s="13">
         <v>900.0</v>
       </c>
-      <c r="E46" s="13">
+      <c r="E46" s="15">
         <v>9.0</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="11">
+      <c r="D47" s="13">
         <v>900.0</v>
       </c>
-      <c r="E47" s="13">
+      <c r="E47" s="15">
         <v>9.0</v>
       </c>
       <c r="F47" s="1"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="11">
+      <c r="D48" s="13">
         <v>900.0</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E48" s="15">
         <v>9.0</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="11">
+      <c r="D49" s="13">
         <v>150.0</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E49" s="15">
         <v>1.0</v>
       </c>
       <c r="F49" s="1"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="11">
+      <c r="D50" s="13">
         <v>150.0</v>
       </c>
-      <c r="E50" s="13">
+      <c r="E50" s="15">
         <v>1.0</v>
       </c>
       <c r="F50" s="1"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="11">
+      <c r="D51" s="13">
         <v>150.0</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E51" s="15">
         <v>1.0</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="11">
+      <c r="D52" s="13">
         <v>150.0</v>
       </c>
-      <c r="E52" s="13">
+      <c r="E52" s="15">
         <v>1.0</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="11">
+      <c r="D53" s="13">
         <v>300.0</v>
       </c>
-      <c r="E53" s="13">
+      <c r="E53" s="15">
         <v>3.0</v>
       </c>
       <c r="F53" s="1"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="11">
+      <c r="D54" s="13">
         <v>300.0</v>
       </c>
-      <c r="E54" s="13">
+      <c r="E54" s="15">
         <v>3.0</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="11">
+      <c r="D55" s="13">
         <v>150.0</v>
       </c>
-      <c r="E55" s="13">
+      <c r="E55" s="15">
         <v>1.0</v>
       </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="11">
+      <c r="D56" s="13">
         <v>150.0</v>
       </c>
-      <c r="E56" s="13">
+      <c r="E56" s="15">
         <v>1.0</v>
       </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="11">
+      <c r="D57" s="13">
         <v>150.0</v>
       </c>
-      <c r="E57" s="13">
+      <c r="E57" s="15">
         <v>1.0</v>
       </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="11">
+      <c r="D58" s="13">
         <v>550.0</v>
       </c>
-      <c r="E58" s="13">
+      <c r="E58" s="15">
         <v>5.0</v>
       </c>
       <c r="F58" s="1"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="11">
+      <c r="D59" s="13">
         <v>600.0</v>
       </c>
-      <c r="E59" s="13">
+      <c r="E59" s="15">
         <v>6.0</v>
       </c>
       <c r="F59" s="1"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="11">
+      <c r="D60" s="13">
         <v>550.0</v>
       </c>
-      <c r="E60" s="13">
+      <c r="E60" s="15">
         <v>5.0</v>
       </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="11">
+      <c r="D61" s="13">
         <v>600.0</v>
       </c>
-      <c r="E61" s="13">
+      <c r="E61" s="15">
         <v>6.0</v>
       </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="11">
+      <c r="D62" s="13">
         <v>600.0</v>
       </c>
-      <c r="E62" s="13">
+      <c r="E62" s="15">
         <v>6.0</v>
       </c>
       <c r="F62" s="1"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="11">
+      <c r="D63" s="13">
         <v>600.0</v>
       </c>
-      <c r="E63" s="13">
+      <c r="E63" s="15">
         <v>6.0</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="11">
+      <c r="D64" s="13">
         <v>500.0</v>
       </c>
-      <c r="E64" s="13">
+      <c r="E64" s="15">
         <v>5.0</v>
       </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="11">
+      <c r="D65" s="13">
         <v>600.0</v>
       </c>
-      <c r="E65" s="13">
+      <c r="E65" s="15">
         <v>6.0</v>
       </c>
       <c r="F65" s="1"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="11">
+      <c r="D66" s="13">
         <v>550.0</v>
       </c>
-      <c r="E66" s="13">
+      <c r="E66" s="15">
         <v>5.0</v>
       </c>
       <c r="F66" s="1"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="11">
+      <c r="D67" s="13">
         <v>550.0</v>
       </c>
-      <c r="E67" s="13">
+      <c r="E67" s="15">
         <v>5.0</v>
       </c>
       <c r="F67" s="1"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="11">
+      <c r="D68" s="13">
         <v>600.0</v>
       </c>
-      <c r="E68" s="13">
+      <c r="E68" s="15">
         <v>6.0</v>
       </c>
       <c r="F68" s="1"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="11">
+      <c r="D69" s="13">
         <v>450.0</v>
       </c>
-      <c r="E69" s="13">
+      <c r="E69" s="15">
         <v>4.0</v>
       </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="11">
+      <c r="D70" s="13">
         <v>450.0</v>
       </c>
-      <c r="E70" s="13">
+      <c r="E70" s="15">
         <v>4.0</v>
       </c>
       <c r="F70" s="1"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="11">
+      <c r="D71" s="13">
         <v>400.0</v>
       </c>
-      <c r="E71" s="13">
+      <c r="E71" s="15">
         <v>4.0</v>
       </c>
       <c r="F71" s="1"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="11">
+      <c r="D72" s="13">
         <v>450.0</v>
       </c>
-      <c r="E72" s="13">
+      <c r="E72" s="15">
         <v>4.0</v>
       </c>
       <c r="F72" s="1"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="11">
+      <c r="D73" s="13">
         <v>450.0</v>
       </c>
-      <c r="E73" s="13">
+      <c r="E73" s="15">
         <v>4.0</v>
       </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="11">
+      <c r="D74" s="13">
         <v>450.0</v>
       </c>
-      <c r="E74" s="13">
+      <c r="E74" s="15">
         <v>4.0</v>
       </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="11">
+      <c r="D75" s="13">
         <v>450.0</v>
       </c>
-      <c r="E75" s="13">
+      <c r="E75" s="15">
         <v>4.0</v>
       </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="11">
+      <c r="D76" s="13">
         <v>450.0</v>
       </c>
-      <c r="E76" s="13">
+      <c r="E76" s="15">
         <v>4.0</v>
       </c>
       <c r="F76" s="1"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D77" s="1"/>
-      <c r="E77" s="8"/>
+      <c r="E77" s="4"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D78" s="1"/>
-      <c r="E78" s="8"/>
+      <c r="E78" s="4"/>
       <c r="F78" s="1"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D79" s="1"/>
-      <c r="E79" s="8"/>
+      <c r="E79" s="4"/>
       <c r="F79" s="1"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="11">
+      <c r="D80" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E80" s="13">
+      <c r="E80" s="15">
         <v>12.0</v>
       </c>
       <c r="F80" s="1"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B81" s="1">
         <v>1.5646176E12</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D81" s="11">
+        <v>133</v>
+      </c>
+      <c r="D81" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E81" s="13">
+      <c r="E81" s="15">
         <v>12.0</v>
       </c>
       <c r="F81" s="1"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="11">
+      <c r="D82" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E82" s="13">
+      <c r="E82" s="15">
         <v>12.0</v>
       </c>
       <c r="F82" s="1"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D83" s="11">
+        <v>136</v>
+      </c>
+      <c r="D83" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E83" s="13">
+      <c r="E83" s="15">
         <v>12.0</v>
       </c>
       <c r="F83" s="1"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D84" s="11">
+        <v>138</v>
+      </c>
+      <c r="D84" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E84" s="13">
+      <c r="E84" s="15">
         <v>12.0</v>
       </c>
       <c r="F84" s="1"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D85" s="11">
+        <v>140</v>
+      </c>
+      <c r="D85" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E85" s="13">
+      <c r="E85" s="15">
         <v>12.0</v>
       </c>
       <c r="F85" s="1"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="11">
+      <c r="D86" s="13">
         <v>800.0</v>
       </c>
-      <c r="E86" s="13">
+      <c r="E86" s="15">
         <v>8.0</v>
       </c>
       <c r="F86" s="1"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="11">
+      <c r="D87" s="13">
         <v>800.0</v>
       </c>
-      <c r="E87" s="13">
+      <c r="E87" s="15">
         <v>8.0</v>
       </c>
       <c r="F87" s="1"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="11">
+      <c r="D88" s="13">
         <v>800.0</v>
       </c>
-      <c r="E88" s="13">
+      <c r="E88" s="15">
         <v>8.0</v>
       </c>
       <c r="F88" s="1"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="11">
+      <c r="D89" s="13">
         <v>600.0</v>
       </c>
-      <c r="E89" s="13">
+      <c r="E89" s="15">
         <v>6.0</v>
       </c>
       <c r="F89" s="1"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="11">
+      <c r="D90" s="13">
         <v>600.0</v>
       </c>
-      <c r="E90" s="13">
+      <c r="E90" s="15">
         <v>6.0</v>
       </c>
       <c r="F90" s="1"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="11">
+      <c r="D91" s="13">
         <v>850.0</v>
       </c>
-      <c r="E91" s="13">
+      <c r="E91" s="15">
         <v>8.0</v>
       </c>
       <c r="F91" s="1"/>
@@ -2940,10 +2940,10 @@
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="11">
+      <c r="D92" s="13">
         <v>550.0</v>
       </c>
-      <c r="E92" s="13">
+      <c r="E92" s="15">
         <v>5.0</v>
       </c>
       <c r="F92" s="1"/>
@@ -2954,10 +2954,10 @@
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="11">
+      <c r="D93" s="13">
         <v>850.0</v>
       </c>
-      <c r="E93" s="13">
+      <c r="E93" s="15">
         <v>8.0</v>
       </c>
       <c r="F93" s="1"/>
@@ -2968,10 +2968,10 @@
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="11">
+      <c r="D94" s="13">
         <v>650.0</v>
       </c>
-      <c r="E94" s="13">
+      <c r="E94" s="15">
         <v>6.0</v>
       </c>
       <c r="F94" s="1"/>
@@ -2982,10 +2982,10 @@
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="11">
+      <c r="D95" s="13">
         <v>550.0</v>
       </c>
-      <c r="E95" s="13">
+      <c r="E95" s="15">
         <v>5.0</v>
       </c>
       <c r="F95" s="1"/>
@@ -2996,10 +2996,10 @@
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="11">
+      <c r="D96" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E96" s="13">
+      <c r="E96" s="15">
         <v>12.0</v>
       </c>
       <c r="F96" s="1"/>
@@ -3010,10 +3010,10 @@
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="11">
+      <c r="D97" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E97" s="13">
+      <c r="E97" s="15">
         <v>10.0</v>
       </c>
       <c r="F97" s="1"/>
@@ -3024,10 +3024,10 @@
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="11">
+      <c r="D98" s="13">
         <v>500.0</v>
       </c>
-      <c r="E98" s="13">
+      <c r="E98" s="15">
         <v>5.0</v>
       </c>
       <c r="F98" s="1"/>
@@ -3038,10 +3038,10 @@
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="11">
+      <c r="D99" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E99" s="13">
+      <c r="E99" s="15">
         <v>12.0</v>
       </c>
       <c r="F99" s="1"/>
@@ -3052,10 +3052,10 @@
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="11">
+      <c r="D100" s="13">
         <v>700.0</v>
       </c>
-      <c r="E100" s="13">
+      <c r="E100" s="15">
         <v>7.0</v>
       </c>
       <c r="F100" s="1"/>
@@ -3066,10 +3066,10 @@
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
-      <c r="D101" s="11">
+      <c r="D101" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E101" s="13">
+      <c r="E101" s="15">
         <v>12.0</v>
       </c>
       <c r="F101" s="1"/>
@@ -3080,10 +3080,10 @@
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
-      <c r="D102" s="11">
+      <c r="D102" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E102" s="13">
+      <c r="E102" s="15">
         <v>12.0</v>
       </c>
       <c r="F102" s="1"/>
@@ -3094,10 +3094,10 @@
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
-      <c r="D103" s="11">
+      <c r="D103" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E103" s="13">
+      <c r="E103" s="15">
         <v>12.0</v>
       </c>
       <c r="F103" s="1"/>
@@ -3108,10 +3108,10 @@
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
-      <c r="D104" s="11">
+      <c r="D104" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E104" s="13">
+      <c r="E104" s="15">
         <v>12.0</v>
       </c>
       <c r="F104" s="1"/>
@@ -3122,10 +3122,10 @@
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
-      <c r="D105" s="11">
+      <c r="D105" s="13">
         <v>900.0</v>
       </c>
-      <c r="E105" s="13">
+      <c r="E105" s="15">
         <v>9.0</v>
       </c>
       <c r="F105" s="1"/>
@@ -3136,10 +3136,10 @@
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
-      <c r="D106" s="11">
+      <c r="D106" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E106" s="13">
+      <c r="E106" s="15">
         <v>11.0</v>
       </c>
       <c r="F106" s="1"/>
@@ -3150,10 +3150,10 @@
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
-      <c r="D107" s="11">
+      <c r="D107" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E107" s="13">
+      <c r="E107" s="15">
         <v>12.0</v>
       </c>
       <c r="F107" s="1"/>
@@ -3164,10 +3164,10 @@
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
-      <c r="D108" s="11">
+      <c r="D108" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E108" s="13">
+      <c r="E108" s="15">
         <v>11.0</v>
       </c>
       <c r="F108" s="1"/>
@@ -3178,10 +3178,10 @@
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
-      <c r="D109" s="11">
+      <c r="D109" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E109" s="13">
+      <c r="E109" s="15">
         <v>12.0</v>
       </c>
       <c r="F109" s="1"/>
@@ -3192,10 +3192,10 @@
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
-      <c r="D110" s="11">
+      <c r="D110" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E110" s="13">
+      <c r="E110" s="15">
         <v>12.0</v>
       </c>
       <c r="F110" s="1"/>
@@ -3206,10 +3206,10 @@
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
-      <c r="D111" s="11">
+      <c r="D111" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E111" s="13">
+      <c r="E111" s="15">
         <v>11.0</v>
       </c>
       <c r="F111" s="1"/>
@@ -3220,10 +3220,10 @@
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
-      <c r="D112" s="11">
+      <c r="D112" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E112" s="13">
+      <c r="E112" s="15">
         <v>11.0</v>
       </c>
       <c r="F112" s="1"/>
@@ -3234,10 +3234,10 @@
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
-      <c r="D113" s="11">
+      <c r="D113" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E113" s="13">
+      <c r="E113" s="15">
         <v>11.0</v>
       </c>
       <c r="F113" s="1"/>
@@ -3248,10 +3248,10 @@
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
-      <c r="D114" s="11">
+      <c r="D114" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E114" s="13">
+      <c r="E114" s="15">
         <v>11.0</v>
       </c>
       <c r="F114" s="1"/>
@@ -3262,10 +3262,10 @@
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
-      <c r="D115" s="11">
+      <c r="D115" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E115" s="13">
+      <c r="E115" s="15">
         <v>12.0</v>
       </c>
       <c r="F115" s="1"/>
@@ -3280,10 +3280,10 @@
       <c r="C116" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D116" s="15">
+      <c r="D116" s="17">
         <v>550.0</v>
       </c>
-      <c r="E116" s="12">
+      <c r="E116" s="14">
         <v>5.0</v>
       </c>
       <c r="F116" s="1"/>
@@ -3298,10 +3298,10 @@
       <c r="C117" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D117" s="11">
+      <c r="D117" s="13">
         <v>700.0</v>
       </c>
-      <c r="E117" s="13">
+      <c r="E117" s="15">
         <v>7.0</v>
       </c>
       <c r="F117" s="1"/>
@@ -3316,10 +3316,10 @@
       <c r="C118" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D118" s="11">
+      <c r="D118" s="13">
         <v>800.0</v>
       </c>
-      <c r="E118" s="13">
+      <c r="E118" s="15">
         <v>8.0</v>
       </c>
       <c r="F118" s="1"/>
@@ -3334,10 +3334,10 @@
       <c r="C119" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D119" s="11">
+      <c r="D119" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E119" s="13">
+      <c r="E119" s="15">
         <v>12.0</v>
       </c>
       <c r="F119" s="1"/>
@@ -3352,10 +3352,10 @@
       <c r="C120" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D120" s="11">
+      <c r="D120" s="13">
         <v>700.0</v>
       </c>
-      <c r="E120" s="13">
+      <c r="E120" s="15">
         <v>7.0</v>
       </c>
       <c r="F120" s="1"/>
@@ -3370,10 +3370,10 @@
       <c r="C121" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D121" s="15">
+      <c r="D121" s="17">
         <v>1100.0</v>
       </c>
-      <c r="E121" s="12">
+      <c r="E121" s="14">
         <v>11.0</v>
       </c>
       <c r="F121" s="1"/>
@@ -3388,10 +3388,10 @@
       <c r="C122" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D122" s="11">
+      <c r="D122" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E122" s="13">
+      <c r="E122" s="15">
         <v>11.0</v>
       </c>
       <c r="F122" s="1"/>
@@ -3406,10 +3406,10 @@
       <c r="C123" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D123" s="11">
+      <c r="D123" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E123" s="13">
+      <c r="E123" s="15">
         <v>12.0</v>
       </c>
       <c r="F123" s="1"/>
@@ -3424,22 +3424,22 @@
       <c r="C124" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D124" s="11">
+      <c r="D124" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E124" s="13">
+      <c r="E124" s="15">
         <v>12.0</v>
       </c>
       <c r="F124" s="1"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
-      <c r="E125" s="8"/>
+      <c r="E125" s="4"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126">
@@ -3448,10 +3448,10 @@
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
-      <c r="D126" s="11">
+      <c r="D126" s="13">
         <v>850.0</v>
       </c>
-      <c r="E126" s="13">
+      <c r="E126" s="15">
         <v>8.0</v>
       </c>
       <c r="F126" s="1"/>
@@ -3462,10 +3462,10 @@
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
-      <c r="D127" s="11">
+      <c r="D127" s="13">
         <v>450.0</v>
       </c>
-      <c r="E127" s="13">
+      <c r="E127" s="15">
         <v>4.0</v>
       </c>
       <c r="F127" s="1"/>
@@ -3476,10 +3476,10 @@
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
-      <c r="D128" s="11">
+      <c r="D128" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E128" s="13">
+      <c r="E128" s="15">
         <v>12.0</v>
       </c>
       <c r="F128" s="1"/>
@@ -3490,10 +3490,10 @@
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
-      <c r="D129" s="11">
+      <c r="D129" s="13">
         <v>450.0</v>
       </c>
-      <c r="E129" s="13">
+      <c r="E129" s="15">
         <v>4.0</v>
       </c>
       <c r="F129" s="1"/>
@@ -3504,10 +3504,10 @@
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
-      <c r="D130" s="11">
+      <c r="D130" s="13">
         <v>800.0</v>
       </c>
-      <c r="E130" s="13">
+      <c r="E130" s="15">
         <v>8.0</v>
       </c>
       <c r="F130" s="1"/>
@@ -3518,10 +3518,10 @@
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
-      <c r="D131" s="11">
+      <c r="D131" s="13">
         <v>500.0</v>
       </c>
-      <c r="E131" s="13">
+      <c r="E131" s="15">
         <v>5.0</v>
       </c>
       <c r="F131" s="1"/>
@@ -3532,10 +3532,10 @@
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
-      <c r="D132" s="11">
+      <c r="D132" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E132" s="13">
+      <c r="E132" s="15">
         <v>12.0</v>
       </c>
       <c r="F132" s="1"/>
@@ -3546,10 +3546,10 @@
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
-      <c r="D133" s="11">
+      <c r="D133" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E133" s="13">
+      <c r="E133" s="15">
         <v>11.0</v>
       </c>
       <c r="F133" s="1"/>
@@ -3560,10 +3560,10 @@
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
-      <c r="D134" s="11">
+      <c r="D134" s="13">
         <v>850.0</v>
       </c>
-      <c r="E134" s="13">
+      <c r="E134" s="15">
         <v>8.0</v>
       </c>
       <c r="F134" s="1"/>
@@ -3575,7 +3575,7 @@
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
-      <c r="E135" s="8"/>
+      <c r="E135" s="4"/>
       <c r="F135" s="1"/>
     </row>
     <row r="136">
@@ -3584,10 +3584,10 @@
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
-      <c r="D136" s="11">
+      <c r="D136" s="13">
         <v>900.0</v>
       </c>
-      <c r="E136" s="13">
+      <c r="E136" s="15">
         <v>9.0</v>
       </c>
       <c r="F136" s="1"/>
@@ -3598,10 +3598,10 @@
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
-      <c r="D137" s="11">
+      <c r="D137" s="13">
         <v>300.0</v>
       </c>
-      <c r="E137" s="13">
+      <c r="E137" s="15">
         <v>3.0</v>
       </c>
       <c r="F137" s="1"/>
@@ -3612,10 +3612,10 @@
       </c>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
-      <c r="D138" s="11">
+      <c r="D138" s="13">
         <v>300.0</v>
       </c>
-      <c r="E138" s="13">
+      <c r="E138" s="15">
         <v>3.0</v>
       </c>
       <c r="F138" s="1"/>
@@ -3626,10 +3626,10 @@
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
-      <c r="D139" s="11">
+      <c r="D139" s="13">
         <v>850.0</v>
       </c>
-      <c r="E139" s="13">
+      <c r="E139" s="15">
         <v>8.0</v>
       </c>
       <c r="F139" s="1"/>
@@ -3640,10 +3640,10 @@
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
-      <c r="D140" s="11">
+      <c r="D140" s="13">
         <v>450.0</v>
       </c>
-      <c r="E140" s="13">
+      <c r="E140" s="15">
         <v>4.0</v>
       </c>
       <c r="F140" s="1"/>
@@ -3654,10 +3654,10 @@
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
-      <c r="D141" s="11">
+      <c r="D141" s="13">
         <v>250.0</v>
       </c>
-      <c r="E141" s="13">
+      <c r="E141" s="15">
         <v>2.0</v>
       </c>
       <c r="F141" s="1"/>
@@ -3668,10 +3668,10 @@
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
-      <c r="D142" s="11">
+      <c r="D142" s="13">
         <v>150.0</v>
       </c>
-      <c r="E142" s="13">
+      <c r="E142" s="15">
         <v>1.0</v>
       </c>
       <c r="F142" s="1"/>
@@ -3682,10 +3682,10 @@
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
-      <c r="D143" s="11">
+      <c r="D143" s="13">
         <v>150.0</v>
       </c>
-      <c r="E143" s="13">
+      <c r="E143" s="15">
         <v>1.0</v>
       </c>
       <c r="F143" s="1"/>
@@ -3696,10 +3696,10 @@
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
-      <c r="D144" s="11">
+      <c r="D144" s="13">
         <v>150.0</v>
       </c>
-      <c r="E144" s="13">
+      <c r="E144" s="15">
         <v>1.0</v>
       </c>
       <c r="F144" s="1"/>
@@ -3710,10 +3710,10 @@
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
-      <c r="D145" s="11">
+      <c r="D145" s="13">
         <v>150.0</v>
       </c>
-      <c r="E145" s="13">
+      <c r="E145" s="15">
         <v>1.0</v>
       </c>
       <c r="F145" s="1"/>
@@ -3724,10 +3724,10 @@
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
-      <c r="D146" s="11">
+      <c r="D146" s="13">
         <v>450.0</v>
       </c>
-      <c r="E146" s="13">
+      <c r="E146" s="15">
         <v>4.0</v>
       </c>
       <c r="F146" s="1"/>
@@ -3738,10 +3738,10 @@
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
-      <c r="D147" s="11">
+      <c r="D147" s="13">
         <v>450.0</v>
       </c>
-      <c r="E147" s="13">
+      <c r="E147" s="15">
         <v>4.0</v>
       </c>
       <c r="F147" s="1"/>
@@ -3752,10 +3752,10 @@
       </c>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
-      <c r="D148" s="11">
+      <c r="D148" s="13">
         <v>450.0</v>
       </c>
-      <c r="E148" s="13">
+      <c r="E148" s="15">
         <v>4.0</v>
       </c>
       <c r="F148" s="1"/>
@@ -3766,10 +3766,10 @@
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
-      <c r="D149" s="11">
+      <c r="D149" s="13">
         <v>500.0</v>
       </c>
-      <c r="E149" s="13">
+      <c r="E149" s="15">
         <v>5.0</v>
       </c>
       <c r="F149" s="1"/>
@@ -3780,10 +3780,10 @@
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
-      <c r="D150" s="11">
+      <c r="D150" s="13">
         <v>800.0</v>
       </c>
-      <c r="E150" s="13">
+      <c r="E150" s="15">
         <v>8.0</v>
       </c>
       <c r="F150" s="1"/>
@@ -3794,10 +3794,10 @@
       </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
-      <c r="D151" s="11">
+      <c r="D151" s="13">
         <v>850.0</v>
       </c>
-      <c r="E151" s="13">
+      <c r="E151" s="15">
         <v>8.0</v>
       </c>
       <c r="F151" s="1"/>
@@ -3808,10 +3808,10 @@
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
-      <c r="D152" s="11">
+      <c r="D152" s="13">
         <v>500.0</v>
       </c>
-      <c r="E152" s="13">
+      <c r="E152" s="15">
         <v>5.0</v>
       </c>
       <c r="F152" s="1"/>
@@ -3822,10 +3822,10 @@
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
-      <c r="D153" s="11">
+      <c r="D153" s="13">
         <v>550.0</v>
       </c>
-      <c r="E153" s="13">
+      <c r="E153" s="15">
         <v>5.0</v>
       </c>
       <c r="F153" s="1"/>
@@ -3836,10 +3836,10 @@
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
-      <c r="D154" s="11">
+      <c r="D154" s="13">
         <v>450.0</v>
       </c>
-      <c r="E154" s="13">
+      <c r="E154" s="15">
         <v>4.0</v>
       </c>
       <c r="F154" s="1"/>
@@ -3850,10 +3850,10 @@
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
-      <c r="D155" s="11">
+      <c r="D155" s="13">
         <v>650.0</v>
       </c>
-      <c r="E155" s="13">
+      <c r="E155" s="15">
         <v>6.0</v>
       </c>
       <c r="F155" s="1"/>
@@ -3864,10 +3864,10 @@
       </c>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
-      <c r="D156" s="11">
+      <c r="D156" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E156" s="13">
+      <c r="E156" s="15">
         <v>10.0</v>
       </c>
       <c r="F156" s="1"/>
@@ -3878,10 +3878,10 @@
       </c>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
-      <c r="D157" s="11">
+      <c r="D157" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E157" s="13">
+      <c r="E157" s="15">
         <v>11.0</v>
       </c>
       <c r="F157" s="1"/>
@@ -3892,10 +3892,10 @@
       </c>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
-      <c r="D158" s="11">
+      <c r="D158" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E158" s="13">
+      <c r="E158" s="15">
         <v>11.0</v>
       </c>
       <c r="F158" s="1"/>
@@ -3906,10 +3906,10 @@
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
-      <c r="D159" s="11">
+      <c r="D159" s="13">
         <v>800.0</v>
       </c>
-      <c r="E159" s="13">
+      <c r="E159" s="15">
         <v>8.0</v>
       </c>
       <c r="F159" s="1"/>
@@ -3920,10 +3920,10 @@
       </c>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
-      <c r="D160" s="11">
+      <c r="D160" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E160" s="13">
+      <c r="E160" s="15">
         <v>12.0</v>
       </c>
       <c r="F160" s="1"/>
@@ -3934,10 +3934,10 @@
       </c>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
-      <c r="D161" s="11">
+      <c r="D161" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E161" s="13">
+      <c r="E161" s="15">
         <v>11.0</v>
       </c>
       <c r="F161" s="1"/>
@@ -3948,10 +3948,10 @@
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
-      <c r="D162" s="11">
+      <c r="D162" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E162" s="13">
+      <c r="E162" s="15">
         <v>11.0</v>
       </c>
       <c r="F162" s="1"/>
@@ -3962,10 +3962,10 @@
       </c>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
-      <c r="D163" s="11">
+      <c r="D163" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E163" s="13">
+      <c r="E163" s="15">
         <v>12.0</v>
       </c>
       <c r="F163" s="1"/>
@@ -3976,10 +3976,10 @@
       </c>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
-      <c r="D164" s="11">
+      <c r="D164" s="13">
         <v>550.0</v>
       </c>
-      <c r="E164" s="13">
+      <c r="E164" s="15">
         <v>5.0</v>
       </c>
       <c r="F164" s="1"/>
@@ -3990,10 +3990,10 @@
       </c>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
-      <c r="D165" s="11">
+      <c r="D165" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E165" s="13">
+      <c r="E165" s="15">
         <v>12.0</v>
       </c>
       <c r="F165" s="1"/>
@@ -4004,10 +4004,10 @@
       </c>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
-      <c r="D166" s="11">
+      <c r="D166" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E166" s="13">
+      <c r="E166" s="15">
         <v>11.0</v>
       </c>
       <c r="F166" s="1"/>
@@ -4018,10 +4018,10 @@
       </c>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
-      <c r="D167" s="11">
+      <c r="D167" s="13">
         <v>400.0</v>
       </c>
-      <c r="E167" s="13">
+      <c r="E167" s="15">
         <v>4.0</v>
       </c>
       <c r="F167" s="1"/>
@@ -4032,10 +4032,10 @@
       </c>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
-      <c r="D168" s="11">
+      <c r="D168" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E168" s="13">
+      <c r="E168" s="15">
         <v>12.0</v>
       </c>
       <c r="F168" s="1"/>
@@ -4046,10 +4046,10 @@
       </c>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
-      <c r="D169" s="11">
+      <c r="D169" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E169" s="13">
+      <c r="E169" s="15">
         <v>11.0</v>
       </c>
       <c r="F169" s="1"/>
@@ -4060,10 +4060,10 @@
       </c>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
-      <c r="D170" s="11">
+      <c r="D170" s="13">
         <v>500.0</v>
       </c>
-      <c r="E170" s="13">
+      <c r="E170" s="15">
         <v>5.0</v>
       </c>
       <c r="F170" s="1"/>
@@ -4074,10 +4074,10 @@
       </c>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
-      <c r="D171" s="11">
+      <c r="D171" s="13">
         <v>600.0</v>
       </c>
-      <c r="E171" s="13">
+      <c r="E171" s="15">
         <v>6.0</v>
       </c>
       <c r="F171" s="1"/>
@@ -4088,10 +4088,10 @@
       </c>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
-      <c r="D172" s="11">
+      <c r="D172" s="13">
         <v>900.0</v>
       </c>
-      <c r="E172" s="13">
+      <c r="E172" s="15">
         <v>9.0</v>
       </c>
       <c r="F172" s="1"/>
@@ -4102,10 +4102,10 @@
       </c>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
-      <c r="D173" s="11">
+      <c r="D173" s="13">
         <v>900.0</v>
       </c>
-      <c r="E173" s="13">
+      <c r="E173" s="15">
         <v>9.0</v>
       </c>
       <c r="F173" s="1"/>
@@ -4116,10 +4116,10 @@
       </c>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
-      <c r="D174" s="11">
+      <c r="D174" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E174" s="13">
+      <c r="E174" s="15">
         <v>11.0</v>
       </c>
       <c r="F174" s="1"/>
@@ -4130,10 +4130,10 @@
       </c>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
-      <c r="D175" s="11">
+      <c r="D175" s="13">
         <v>900.0</v>
       </c>
-      <c r="E175" s="13">
+      <c r="E175" s="15">
         <v>9.0</v>
       </c>
       <c r="F175" s="1"/>
@@ -4144,10 +4144,10 @@
       </c>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
-      <c r="D176" s="11">
+      <c r="D176" s="13">
         <v>550.0</v>
       </c>
-      <c r="E176" s="13">
+      <c r="E176" s="15">
         <v>5.0</v>
       </c>
       <c r="F176" s="1"/>
@@ -4158,10 +4158,10 @@
       </c>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
-      <c r="D177" s="11">
+      <c r="D177" s="13">
         <v>550.0</v>
       </c>
-      <c r="E177" s="13">
+      <c r="E177" s="15">
         <v>5.0</v>
       </c>
       <c r="F177" s="1"/>
@@ -4172,10 +4172,10 @@
       </c>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
-      <c r="D178" s="11">
+      <c r="D178" s="13">
         <v>800.0</v>
       </c>
-      <c r="E178" s="13">
+      <c r="E178" s="15">
         <v>8.0</v>
       </c>
       <c r="F178" s="1"/>
@@ -4186,10 +4186,10 @@
       </c>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
-      <c r="D179" s="11">
+      <c r="D179" s="13">
         <v>800.0</v>
       </c>
-      <c r="E179" s="13">
+      <c r="E179" s="15">
         <v>8.0</v>
       </c>
       <c r="F179" s="1"/>
@@ -4200,10 +4200,10 @@
       </c>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
-      <c r="D180" s="11">
+      <c r="D180" s="13">
         <v>950.0</v>
       </c>
-      <c r="E180" s="13">
+      <c r="E180" s="15">
         <v>9.0</v>
       </c>
       <c r="F180" s="1"/>
@@ -4214,10 +4214,10 @@
       </c>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
-      <c r="D181" s="11">
+      <c r="D181" s="13">
         <v>950.0</v>
       </c>
-      <c r="E181" s="13">
+      <c r="E181" s="15">
         <v>9.0</v>
       </c>
       <c r="F181" s="1"/>
@@ -4228,10 +4228,10 @@
       </c>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
-      <c r="D182" s="11">
+      <c r="D182" s="13">
         <v>150.0</v>
       </c>
-      <c r="E182" s="13">
+      <c r="E182" s="15">
         <v>1.0</v>
       </c>
       <c r="F182" s="1"/>
@@ -4242,10 +4242,10 @@
       </c>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
-      <c r="D183" s="11">
+      <c r="D183" s="13">
         <v>550.0</v>
       </c>
-      <c r="E183" s="13">
+      <c r="E183" s="15">
         <v>5.0</v>
       </c>
       <c r="F183" s="1"/>
@@ -4256,10 +4256,10 @@
       </c>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
-      <c r="D184" s="11">
+      <c r="D184" s="13">
         <v>600.0</v>
       </c>
-      <c r="E184" s="13">
+      <c r="E184" s="15">
         <v>6.0</v>
       </c>
       <c r="F184" s="1"/>
@@ -4270,10 +4270,10 @@
       </c>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
-      <c r="D185" s="11">
+      <c r="D185" s="13">
         <v>200.0</v>
       </c>
-      <c r="E185" s="13">
+      <c r="E185" s="15">
         <v>2.0</v>
       </c>
       <c r="F185" s="1"/>
@@ -4284,10 +4284,10 @@
       </c>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
-      <c r="D186" s="11">
+      <c r="D186" s="13">
         <v>600.0</v>
       </c>
-      <c r="E186" s="13">
+      <c r="E186" s="15">
         <v>6.0</v>
       </c>
       <c r="F186" s="1"/>
@@ -4298,10 +4298,10 @@
       </c>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
-      <c r="D187" s="11">
+      <c r="D187" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E187" s="13">
+      <c r="E187" s="15">
         <v>11.0</v>
       </c>
       <c r="F187" s="1"/>
@@ -4312,10 +4312,10 @@
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
-      <c r="D188" s="11">
+      <c r="D188" s="13">
         <v>900.0</v>
       </c>
-      <c r="E188" s="13">
+      <c r="E188" s="15">
         <v>9.0</v>
       </c>
       <c r="F188" s="1"/>
@@ -4326,10 +4326,10 @@
       </c>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
-      <c r="D189" s="11">
+      <c r="D189" s="13">
         <v>300.0</v>
       </c>
-      <c r="E189" s="13">
+      <c r="E189" s="15">
         <v>3.0</v>
       </c>
       <c r="F189" s="1"/>
@@ -4340,10 +4340,10 @@
       </c>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
-      <c r="D190" s="11">
+      <c r="D190" s="13">
         <v>550.0</v>
       </c>
-      <c r="E190" s="13">
+      <c r="E190" s="15">
         <v>5.0</v>
       </c>
       <c r="F190" s="1"/>
@@ -4354,10 +4354,10 @@
       </c>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
-      <c r="D191" s="11">
+      <c r="D191" s="13">
         <v>550.0</v>
       </c>
-      <c r="E191" s="13">
+      <c r="E191" s="15">
         <v>5.0</v>
       </c>
       <c r="F191" s="1"/>
@@ -4368,10 +4368,10 @@
       </c>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
-      <c r="D192" s="11">
+      <c r="D192" s="13">
         <v>550.0</v>
       </c>
-      <c r="E192" s="13">
+      <c r="E192" s="15">
         <v>5.0</v>
       </c>
       <c r="F192" s="1"/>
@@ -4382,10 +4382,10 @@
       </c>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
-      <c r="D193" s="11">
+      <c r="D193" s="13">
         <v>400.0</v>
       </c>
-      <c r="E193" s="13">
+      <c r="E193" s="15">
         <v>4.0</v>
       </c>
       <c r="F193" s="1"/>
@@ -4396,10 +4396,10 @@
       </c>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
-      <c r="D194" s="11">
+      <c r="D194" s="13">
         <v>500.0</v>
       </c>
-      <c r="E194" s="13">
+      <c r="E194" s="15">
         <v>5.0</v>
       </c>
       <c r="F194" s="1"/>
@@ -4410,10 +4410,10 @@
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
-      <c r="D195" s="11">
+      <c r="D195" s="13">
         <v>950.0</v>
       </c>
-      <c r="E195" s="13">
+      <c r="E195" s="15">
         <v>9.0</v>
       </c>
       <c r="F195" s="1"/>
@@ -4424,10 +4424,10 @@
       </c>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
-      <c r="D196" s="11">
+      <c r="D196" s="13">
         <v>500.0</v>
       </c>
-      <c r="E196" s="13">
+      <c r="E196" s="15">
         <v>5.0</v>
       </c>
       <c r="F196" s="1"/>
@@ -4438,10 +4438,10 @@
       </c>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
-      <c r="D197" s="11">
+      <c r="D197" s="13">
         <v>500.0</v>
       </c>
-      <c r="E197" s="13">
+      <c r="E197" s="15">
         <v>5.0</v>
       </c>
       <c r="F197" s="1"/>
@@ -4452,10 +4452,10 @@
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
-      <c r="D198" s="11">
+      <c r="D198" s="13">
         <v>350.0</v>
       </c>
-      <c r="E198" s="13">
+      <c r="E198" s="15">
         <v>3.0</v>
       </c>
       <c r="F198" s="1"/>
@@ -4466,10 +4466,10 @@
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
-      <c r="D199" s="11">
+      <c r="D199" s="13">
         <v>950.0</v>
       </c>
-      <c r="E199" s="13">
+      <c r="E199" s="15">
         <v>9.0</v>
       </c>
       <c r="F199" s="1"/>
@@ -4480,10 +4480,10 @@
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
-      <c r="D200" s="11">
+      <c r="D200" s="13">
         <v>150.0</v>
       </c>
-      <c r="E200" s="13">
+      <c r="E200" s="15">
         <v>1.0</v>
       </c>
       <c r="F200" s="1"/>
@@ -4494,10 +4494,10 @@
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
-      <c r="D201" s="11">
+      <c r="D201" s="13">
         <v>950.0</v>
       </c>
-      <c r="E201" s="13">
+      <c r="E201" s="15">
         <v>9.0</v>
       </c>
       <c r="F201" s="1"/>
@@ -4508,10 +4508,10 @@
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
-      <c r="D202" s="11">
+      <c r="D202" s="13">
         <v>150.0</v>
       </c>
-      <c r="E202" s="13">
+      <c r="E202" s="15">
         <v>1.0</v>
       </c>
       <c r="F202" s="1"/>
@@ -4522,10 +4522,10 @@
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
-      <c r="D203" s="11">
+      <c r="D203" s="13">
         <v>600.0</v>
       </c>
-      <c r="E203" s="13">
+      <c r="E203" s="15">
         <v>6.0</v>
       </c>
       <c r="F203" s="1"/>
@@ -4536,10 +4536,10 @@
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
-      <c r="D204" s="11">
+      <c r="D204" s="13">
         <v>550.0</v>
       </c>
-      <c r="E204" s="13">
+      <c r="E204" s="15">
         <v>5.0</v>
       </c>
       <c r="F204" s="1"/>
@@ -4550,10 +4550,10 @@
       </c>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
-      <c r="D205" s="11">
+      <c r="D205" s="13">
         <v>700.0</v>
       </c>
-      <c r="E205" s="13">
+      <c r="E205" s="15">
         <v>7.0</v>
       </c>
       <c r="F205" s="1"/>
@@ -4564,10 +4564,10 @@
       </c>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
-      <c r="D206" s="11">
+      <c r="D206" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E206" s="14">
+      <c r="E206" s="16">
         <v>10.0</v>
       </c>
       <c r="F206" s="1"/>
@@ -4578,10 +4578,10 @@
       </c>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
-      <c r="D207" s="11">
+      <c r="D207" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E207" s="12">
+      <c r="E207" s="14">
         <v>10.0</v>
       </c>
       <c r="F207" s="1"/>
@@ -4592,10 +4592,10 @@
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
-      <c r="D208" s="11">
+      <c r="D208" s="13">
         <v>500.0</v>
       </c>
-      <c r="E208" s="13">
+      <c r="E208" s="15">
         <v>5.0</v>
       </c>
       <c r="F208" s="1"/>
@@ -4606,10 +4606,10 @@
       </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
-      <c r="D209" s="11">
+      <c r="D209" s="13">
         <v>250.0</v>
       </c>
-      <c r="E209" s="13">
+      <c r="E209" s="15">
         <v>2.0</v>
       </c>
       <c r="F209" s="1"/>
@@ -4620,10 +4620,10 @@
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
-      <c r="D210" s="11">
+      <c r="D210" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E210" s="13">
+      <c r="E210" s="15">
         <v>10.0</v>
       </c>
       <c r="F210" s="1"/>
@@ -4634,10 +4634,10 @@
       </c>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
-      <c r="D211" s="11">
+      <c r="D211" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E211" s="13">
+      <c r="E211" s="15">
         <v>10.0</v>
       </c>
       <c r="F211" s="1"/>
@@ -4648,10 +4648,10 @@
       </c>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
-      <c r="D212" s="11">
+      <c r="D212" s="13">
         <v>1000.0</v>
       </c>
-      <c r="E212" s="13">
+      <c r="E212" s="15">
         <v>10.0</v>
       </c>
       <c r="F212" s="1"/>
@@ -4662,10 +4662,10 @@
       </c>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
-      <c r="D213" s="11">
+      <c r="D213" s="13">
         <v>500.0</v>
       </c>
-      <c r="E213" s="13">
+      <c r="E213" s="15">
         <v>5.0</v>
       </c>
       <c r="F213" s="1"/>
@@ -4679,7 +4679,7 @@
       <c r="D214" s="21">
         <v>900.0</v>
       </c>
-      <c r="E214" s="14">
+      <c r="E214" s="16">
         <v>9.0</v>
       </c>
       <c r="F214" s="1"/>
@@ -4690,10 +4690,10 @@
       </c>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
-      <c r="D215" s="11">
+      <c r="D215" s="13">
         <v>300.0</v>
       </c>
-      <c r="E215" s="13">
+      <c r="E215" s="15">
         <v>3.0</v>
       </c>
       <c r="F215" s="1"/>
@@ -4704,10 +4704,10 @@
       </c>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
-      <c r="D216" s="11">
+      <c r="D216" s="13">
         <v>400.0</v>
       </c>
-      <c r="E216" s="13">
+      <c r="E216" s="15">
         <v>4.0</v>
       </c>
       <c r="F216" s="1"/>
@@ -4718,10 +4718,10 @@
       </c>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
-      <c r="D217" s="11">
+      <c r="D217" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E217" s="13">
+      <c r="E217" s="15">
         <v>12.0</v>
       </c>
       <c r="F217" s="1"/>
@@ -4732,10 +4732,10 @@
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
-      <c r="D218" s="11">
+      <c r="D218" s="13">
         <v>450.0</v>
       </c>
-      <c r="E218" s="13">
+      <c r="E218" s="15">
         <v>4.0</v>
       </c>
       <c r="F218" s="1"/>
@@ -4746,10 +4746,10 @@
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
-      <c r="D219" s="11">
+      <c r="D219" s="13">
         <v>250.0</v>
       </c>
-      <c r="E219" s="13">
+      <c r="E219" s="15">
         <v>2.0</v>
       </c>
       <c r="F219" s="1"/>
@@ -4760,10 +4760,10 @@
       </c>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
-      <c r="D220" s="11">
+      <c r="D220" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E220" s="13">
+      <c r="E220" s="15">
         <v>12.0</v>
       </c>
       <c r="F220" s="1"/>
@@ -4774,10 +4774,10 @@
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
-      <c r="D221" s="11">
+      <c r="D221" s="13">
         <v>900.0</v>
       </c>
-      <c r="E221" s="13">
+      <c r="E221" s="15">
         <v>9.0</v>
       </c>
       <c r="F221" s="1"/>
@@ -4788,10 +4788,10 @@
       </c>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
-      <c r="D222" s="11">
+      <c r="D222" s="13">
         <v>700.0</v>
       </c>
-      <c r="E222" s="13">
+      <c r="E222" s="15">
         <v>7.0</v>
       </c>
       <c r="F222" s="1"/>
@@ -4803,7 +4803,7 @@
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
-      <c r="E223" s="8"/>
+      <c r="E223" s="4"/>
       <c r="F223" s="1"/>
     </row>
     <row r="224">
@@ -4812,10 +4812,10 @@
       </c>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
-      <c r="D224" s="11">
+      <c r="D224" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E224" s="13">
+      <c r="E224" s="15">
         <v>12.0</v>
       </c>
       <c r="F224" s="1"/>
@@ -4827,7 +4827,7 @@
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
-      <c r="E225" s="8"/>
+      <c r="E225" s="4"/>
       <c r="F225" s="1"/>
     </row>
     <row r="226">
@@ -4836,10 +4836,10 @@
       </c>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
-      <c r="D226" s="11">
+      <c r="D226" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E226" s="13">
+      <c r="E226" s="15">
         <v>12.0</v>
       </c>
       <c r="F226" s="1"/>
@@ -4850,10 +4850,10 @@
       </c>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
-      <c r="D227" s="11">
+      <c r="D227" s="13">
         <v>450.0</v>
       </c>
-      <c r="E227" s="13">
+      <c r="E227" s="15">
         <v>4.0</v>
       </c>
       <c r="F227" s="1"/>
@@ -4865,7 +4865,7 @@
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
-      <c r="E228" s="8"/>
+      <c r="E228" s="4"/>
       <c r="F228" s="1"/>
     </row>
     <row r="229">
@@ -4874,10 +4874,10 @@
       </c>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
-      <c r="D229" s="11">
+      <c r="D229" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E229" s="13">
+      <c r="E229" s="15">
         <v>12.0</v>
       </c>
       <c r="F229" s="1"/>
@@ -4888,10 +4888,10 @@
       </c>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
-      <c r="D230" s="11">
+      <c r="D230" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E230" s="13">
+      <c r="E230" s="15">
         <v>12.0</v>
       </c>
       <c r="F230" s="1"/>
@@ -4902,10 +4902,10 @@
       </c>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
-      <c r="D231" s="11">
+      <c r="D231" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E231" s="13">
+      <c r="E231" s="15">
         <v>12.0</v>
       </c>
       <c r="F231" s="1"/>
@@ -4916,10 +4916,10 @@
       </c>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
-      <c r="D232" s="11">
+      <c r="D232" s="13">
         <v>550.0</v>
       </c>
-      <c r="E232" s="13">
+      <c r="E232" s="15">
         <v>5.0</v>
       </c>
       <c r="F232" s="1"/>
@@ -4930,10 +4930,10 @@
       </c>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
-      <c r="D233" s="11">
+      <c r="D233" s="13">
         <v>900.0</v>
       </c>
-      <c r="E233" s="13">
+      <c r="E233" s="15">
         <v>9.0</v>
       </c>
       <c r="F233" s="1"/>
@@ -4944,10 +4944,10 @@
       </c>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
-      <c r="D234" s="11">
+      <c r="D234" s="13">
         <v>850.0</v>
       </c>
-      <c r="E234" s="13">
+      <c r="E234" s="15">
         <v>8.0</v>
       </c>
       <c r="F234" s="1"/>
@@ -4958,10 +4958,10 @@
       </c>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
-      <c r="D235" s="11">
+      <c r="D235" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E235" s="13">
+      <c r="E235" s="15">
         <v>11.0</v>
       </c>
       <c r="F235" s="1"/>
@@ -4972,10 +4972,10 @@
       </c>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
-      <c r="D236" s="11">
+      <c r="D236" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E236" s="13">
+      <c r="E236" s="15">
         <v>12.0</v>
       </c>
       <c r="F236" s="1"/>
@@ -4986,10 +4986,10 @@
       </c>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
-      <c r="D237" s="11">
+      <c r="D237" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E237" s="13">
+      <c r="E237" s="15">
         <v>12.0</v>
       </c>
       <c r="F237" s="1"/>
@@ -5000,10 +5000,10 @@
       </c>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
-      <c r="D238" s="11">
+      <c r="D238" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E238" s="13">
+      <c r="E238" s="15">
         <v>12.0</v>
       </c>
       <c r="F238" s="1"/>
@@ -5014,10 +5014,10 @@
       </c>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
-      <c r="D239" s="11">
+      <c r="D239" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E239" s="13">
+      <c r="E239" s="15">
         <v>12.0</v>
       </c>
       <c r="F239" s="1"/>
@@ -5028,10 +5028,10 @@
       </c>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
-      <c r="D240" s="11">
+      <c r="D240" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E240" s="13">
+      <c r="E240" s="15">
         <v>12.0</v>
       </c>
       <c r="F240" s="1"/>
@@ -5042,10 +5042,10 @@
       </c>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
-      <c r="D241" s="11">
+      <c r="D241" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E241" s="13">
+      <c r="E241" s="15">
         <v>12.0</v>
       </c>
       <c r="F241" s="1"/>
@@ -5056,10 +5056,10 @@
       </c>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
-      <c r="D242" s="11">
+      <c r="D242" s="13">
         <v>1250.0</v>
       </c>
-      <c r="E242" s="13">
+      <c r="E242" s="15">
         <v>12.0</v>
       </c>
       <c r="F242" s="1"/>
@@ -5070,10 +5070,10 @@
       </c>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
-      <c r="D243" s="11">
+      <c r="D243" s="13">
         <v>800.0</v>
       </c>
-      <c r="E243" s="13">
+      <c r="E243" s="15">
         <v>8.0</v>
       </c>
       <c r="F243" s="1"/>
@@ -5084,10 +5084,10 @@
       </c>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
-      <c r="D244" s="11">
+      <c r="D244" s="13">
         <v>1200.0</v>
       </c>
-      <c r="E244" s="13">
+      <c r="E244" s="15">
         <v>12.0</v>
       </c>
       <c r="F244" s="1"/>
@@ -5101,7 +5101,7 @@
       <c r="D245" s="21">
         <v>700.0</v>
       </c>
-      <c r="E245" s="14">
+      <c r="E245" s="16">
         <v>7.0</v>
       </c>
       <c r="F245" s="1"/>
@@ -5112,10 +5112,10 @@
       </c>
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
-      <c r="D246" s="11">
+      <c r="D246" s="13">
         <v>1100.0</v>
       </c>
-      <c r="E246" s="13">
+      <c r="E246" s="15">
         <v>11.0</v>
       </c>
       <c r="F246" s="1"/>
@@ -5125,7 +5125,7 @@
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
-      <c r="E247" s="8"/>
+      <c r="E247" s="4"/>
       <c r="F247" s="1"/>
     </row>
     <row r="248">
@@ -5133,7 +5133,7 @@
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
-      <c r="E248" s="8"/>
+      <c r="E248" s="4"/>
       <c r="F248" s="1"/>
     </row>
   </sheetData>
@@ -5175,100 +5175,100 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>89</v>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>89</v>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>96</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>89</v>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>89</v>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>89</v>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1">
         <v>1.5632496E12</v>
@@ -5277,14 +5277,14 @@
       <c r="D8" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>89</v>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1">
         <v>1.56204E12</v>
@@ -5293,14 +5293,14 @@
       <c r="D9" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>89</v>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
         <v>1.5658416E12</v>
@@ -5309,14 +5309,14 @@
       <c r="D10" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>89</v>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>110</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1">
         <v>1.5667056E12</v>
@@ -5325,14 +5325,14 @@
       <c r="D11" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>89</v>
+      <c r="E11" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1">
         <v>1.5649776E12</v>
@@ -5341,176 +5341,176 @@
       <c r="D12" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>89</v>
+      <c r="E12" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>89</v>
+      <c r="E13" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>89</v>
+      <c r="E14" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>89</v>
+      <c r="E15" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>124</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>89</v>
+      <c r="E16" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>127</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>89</v>
+      <c r="E17" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>89</v>
+      <c r="E18" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>89</v>
+      <c r="E19" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>89</v>
+      <c r="E20" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>89</v>
+      <c r="E21" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>89</v>
+      <c r="E22" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>143</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>89</v>
+      <c r="E23" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>146</v>
+        <v>67</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>89</v>
+      <c r="E24" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -5519,7 +5519,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="8"/>
+      <c r="E25" s="4"/>
       <c r="F25" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add localization to moon ui's "Spell Efficiency"
</commit_message>
<xml_diff>
--- a/Dictionaries/store.xlsx
+++ b/Dictionaries/store.xlsx
@@ -32,21 +32,39 @@
     <t>gold</t>
   </si>
   <si>
+    <t>bundle_abondiasBest</t>
+  </si>
+  <si>
+    <t>silver1</t>
+  </si>
+  <si>
+    <t>bundle_sapphosChoice</t>
+  </si>
+  <si>
+    <t>silver2</t>
+  </si>
+  <si>
+    <t>silver3</t>
+  </si>
+  <si>
+    <t>silver4</t>
+  </si>
+  <si>
+    <t>silver5</t>
+  </si>
+  <si>
+    <t>silver6</t>
+  </si>
+  <si>
+    <t>bundle_hermeticCollection</t>
+  </si>
+  <si>
     <t>consumable_alignmentBoosterSmaller</t>
   </si>
   <si>
-    <t>silver1</t>
-  </si>
-  <si>
-    <t>bundle_abondiasBest</t>
-  </si>
-  <si>
     <t>consumable_alignmentBoosterMedium</t>
   </si>
   <si>
-    <t>bundle_sapphosChoice</t>
-  </si>
-  <si>
     <t>consumable_alignmentBoosterGreater</t>
   </si>
   <si>
@@ -56,51 +74,93 @@
     <t>consumable_xpBoosterMedium</t>
   </si>
   <si>
-    <t>silver2</t>
-  </si>
-  <si>
-    <t>bundle_hermeticCollection</t>
-  </si>
-  <si>
     <t>consumable_xpBoosterGreater</t>
   </si>
   <si>
-    <t>silver3</t>
-  </si>
-  <si>
-    <t>silver4</t>
-  </si>
-  <si>
-    <t>silver5</t>
-  </si>
-  <si>
-    <t>silver6</t>
-  </si>
-  <si>
     <t>cosmetic_f_PF_WENDIGO</t>
   </si>
   <si>
+    <t>shop_locked_wndg</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_BARGHEST</t>
+  </si>
+  <si>
+    <t>shop_locked_barg</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_CATSIDHE</t>
+  </si>
+  <si>
+    <t>shop_locked_sidh</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_GRINDYLOW</t>
+  </si>
+  <si>
+    <t>shop_locked_grdlw</t>
+  </si>
+  <si>
+    <t>cosmetic_f_PF_SENTINALOWL</t>
+  </si>
+  <si>
+    <t>shop_locked_owl</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_DWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HDWO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HBH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_HBO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_HHO</t>
   </si>
   <si>
-    <t>shop_locked_wndg</t>
+    <t>cosmetic_f_HE_HHO</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
+    <t>cosmetic_f_HE_HNO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_HKO</t>
   </si>
   <si>
+    <t>cosmetic_f_HE_CEH</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_HLO</t>
   </si>
   <si>
+    <t>cosmetic_f_HE_CES</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HE_FLOWER</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_SNOWQUEEN</t>
   </si>
   <si>
+    <t>cosmetic_f_HE_BDH</t>
+  </si>
+  <si>
+    <t>shop_locked_rrc</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_LILYOV</t>
   </si>
   <si>
+    <t>cosmetic_f_HA_DWO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_MIDSUMMER</t>
   </si>
   <si>
@@ -113,135 +173,75 @@
     <t>cosmetic_f_S_CORNMOON</t>
   </si>
   <si>
+    <t>cosmetic_f_HA_FKFO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_BRNNGWTCH</t>
   </si>
   <si>
+    <t>cosmetic_f_HA_KSO</t>
+  </si>
+  <si>
     <t>cosmetic_f_S_CALYPSO</t>
   </si>
   <si>
-    <t>cosmetic_f_PF_BARGHEST</t>
-  </si>
-  <si>
-    <t>shop_locked_barg</t>
+    <t>cosmetic_f_HA_CGH</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_PNY</t>
   </si>
   <si>
     <t>_</t>
   </si>
   <si>
+    <t>cosmetic_f_HA_SNWDRP</t>
+  </si>
+  <si>
     <t>cosmetic_m_S_HKO</t>
   </si>
   <si>
-    <t>cosmetic_f_PF_CATSIDHE</t>
-  </si>
-  <si>
-    <t>shop_locked_sidh</t>
+    <t>cosmetic_f_HA_BUN</t>
   </si>
   <si>
     <t>cosmetic_m_S_HHO</t>
   </si>
   <si>
-    <t>cosmetic_f_PF_GRINDYLOW</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_HLO</t>
   </si>
   <si>
-    <t>shop_locked_grdlw</t>
-  </si>
-  <si>
-    <t>cosmetic_f_PF_SENTINALOWL</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_JACKFROST</t>
   </si>
   <si>
-    <t>shop_locked_owl</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_MIDSUMMER</t>
   </si>
   <si>
     <t>cosmetic_m_S_CORNMOON</t>
   </si>
   <si>
-    <t>cosmetic_f_HE_DWO</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_CALYPSO</t>
   </si>
   <si>
-    <t>cosmetic_f_HE_HDWO</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_FIREDANCER</t>
   </si>
   <si>
-    <t>cosmetic_f_HE_HBH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_HBO</t>
-  </si>
-  <si>
     <t>cosmetic_m_S_BRNNGWTCH</t>
   </si>
   <si>
-    <t>cosmetic_f_HE_HHO</t>
+    <t>cosmetic_f_HA_BRD</t>
+  </si>
+  <si>
+    <t>cosmetic_f_HA_SPK</t>
   </si>
   <si>
     <t>cosmetic_m_S_ECLIPSE</t>
   </si>
   <si>
-    <t>cosmetic_f_HE_HNO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_CEH</t>
+    <t>cosmetic_f_HA_BZZ</t>
   </si>
   <si>
     <t>cosmetic_m_S_THUNDERMOON</t>
   </si>
   <si>
-    <t>cosmetic_f_HE_CES</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_FLOWER</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HE_BDH</t>
-  </si>
-  <si>
-    <t>shop_locked_rrc</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_FKFO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_KSO</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_CGH</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_PNY</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_SNWDRP</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_BUN</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_BRD</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_SPK</t>
-  </si>
-  <si>
-    <t>cosmetic_f_HA_BZZ</t>
-  </si>
-  <si>
     <t>cosmetic_f_HA_CURL</t>
   </si>
   <si>
@@ -581,7 +581,7 @@
     <t>cosmetic_m_HE_HBH</t>
   </si>
   <si>
-    <t>cosmetic_m_HE_GLSS</t>
+    <t>_cosmetic_m_HE_GLSS</t>
   </si>
   <si>
     <t>cosmetic_m_HE_HDWO</t>
@@ -845,22 +845,22 @@
     <t>cosmetic_m_SS_PYRAMIDS</t>
   </si>
   <si>
-    <t>cosmetic_m_CL_DWO</t>
+    <t>_cosmetic_m_CL_DWO</t>
   </si>
   <si>
     <t>cosmetic_m_CL_SMMRSOL</t>
   </si>
   <si>
-    <t>cosmetic_m_CL_DTO</t>
-  </si>
-  <si>
-    <t>cosmetic_m_CL_GRAY</t>
+    <t>_cosmetic_m_CL_DTO</t>
+  </si>
+  <si>
+    <t>_cosmetic_m_CL_GRAY</t>
   </si>
   <si>
     <t>cosmetic_m_F_STRAPPEDSHOES</t>
   </si>
   <si>
-    <t>cosmetic_m_CL_DSO</t>
+    <t>_cosmetic_m_CL_DSO</t>
   </si>
   <si>
     <t>cosmetic_m_CL_PRIMAVERA</t>
@@ -981,26 +981,26 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="top"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1114,28 +1114,28 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>300.0</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1147,14 +1147,14 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>300.0</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
@@ -1162,7 +1162,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
@@ -1170,7 +1170,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
@@ -1178,7 +1178,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1186,7 +1186,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1194,7 +1194,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1202,7 +1202,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1210,7 +1210,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1218,7 +1218,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1226,7 +1226,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1234,7 +1234,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1281,7 +1281,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -1290,82 +1290,82 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>100.0</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="9">
         <v>300.0</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>500.0</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="9">
         <v>100.0</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>300.0</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="9">
         <v>500.0</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1373,7 +1373,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1381,15 +1381,15 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1397,15 +1397,15 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1413,7 +1413,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1460,7 +1460,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -1474,57 +1474,57 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1532,7 +1532,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1540,7 +1540,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1548,7 +1548,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1556,7 +1556,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1564,7 +1564,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1572,7 +1572,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1580,7 +1580,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1627,7 +1627,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -1642,7 +1642,7 @@
         <v>1.56168E12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="13">
         <v>1000.0</v>
@@ -1654,13 +1654,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D3" s="13">
         <v>1000.0</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D4" s="13">
         <v>1000.0</v>
@@ -1690,13 +1690,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D5" s="13">
         <v>1000.0</v>
@@ -1708,13 +1708,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D6" s="13">
         <v>1000.0</v>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1852,11 +1852,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="D16" s="13">
         <v>900.0</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2715,7 +2715,7 @@
         <v>126</v>
       </c>
       <c r="D77" s="1"/>
-      <c r="E77" s="7"/>
+      <c r="E77" s="8"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78">
@@ -2727,7 +2727,7 @@
         <v>126</v>
       </c>
       <c r="D78" s="1"/>
-      <c r="E78" s="7"/>
+      <c r="E78" s="8"/>
       <c r="F78" s="1"/>
     </row>
     <row r="79">
@@ -2739,7 +2739,7 @@
         <v>126</v>
       </c>
       <c r="D79" s="1"/>
-      <c r="E79" s="7"/>
+      <c r="E79" s="8"/>
       <c r="F79" s="1"/>
     </row>
     <row r="80">
@@ -3420,12 +3420,12 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
-      <c r="E125" s="7"/>
+      <c r="E125" s="8"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126">
@@ -3561,7 +3561,7 @@
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
-      <c r="E135" s="7"/>
+      <c r="E135" s="8"/>
       <c r="F135" s="1"/>
     </row>
     <row r="136">
@@ -4789,7 +4789,7 @@
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
-      <c r="E223" s="7"/>
+      <c r="E223" s="8"/>
       <c r="F223" s="1"/>
     </row>
     <row r="224">
@@ -4813,7 +4813,7 @@
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
-      <c r="E225" s="7"/>
+      <c r="E225" s="8"/>
       <c r="F225" s="1"/>
     </row>
     <row r="226">
@@ -4851,7 +4851,7 @@
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
-      <c r="E228" s="7"/>
+      <c r="E228" s="8"/>
       <c r="F228" s="1"/>
     </row>
     <row r="229">
@@ -5111,7 +5111,7 @@
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
-      <c r="E247" s="7"/>
+      <c r="E247" s="8"/>
       <c r="F247" s="1"/>
     </row>
     <row r="248">
@@ -5119,7 +5119,7 @@
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
-      <c r="E248" s="7"/>
+      <c r="E248" s="8"/>
       <c r="F248" s="1"/>
     </row>
   </sheetData>
@@ -5161,7 +5161,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -5170,91 +5170,91 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>23</v>
+      <c r="E2" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>23</v>
+      <c r="E3" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>23</v>
+      <c r="E4" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>23</v>
+      <c r="E5" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>23</v>
+      <c r="E6" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>23</v>
+      <c r="E7" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1">
         <v>1.5632496E12</v>
@@ -5263,14 +5263,14 @@
       <c r="D8" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>23</v>
+      <c r="E8" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1">
         <v>1.56204E12</v>
@@ -5279,14 +5279,14 @@
       <c r="D9" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>23</v>
+      <c r="E9" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1">
         <v>1.5658416E12</v>
@@ -5295,14 +5295,14 @@
       <c r="D10" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>23</v>
+      <c r="E10" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1">
         <v>1.5667056E12</v>
@@ -5311,14 +5311,14 @@
       <c r="D11" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>23</v>
+      <c r="E11" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1">
         <v>1.5649776E12</v>
@@ -5327,176 +5327,176 @@
       <c r="D12" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>23</v>
+      <c r="E12" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>23</v>
+      <c r="E13" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>23</v>
+      <c r="E14" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>23</v>
+      <c r="E15" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>23</v>
+      <c r="E16" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>23</v>
+      <c r="E17" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>23</v>
+      <c r="E18" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>23</v>
+      <c r="E19" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>23</v>
+      <c r="E20" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>23</v>
+      <c r="E21" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>23</v>
+      <c r="E22" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>23</v>
+      <c r="E23" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>23</v>
+      <c r="E24" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -5505,7 +5505,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="7"/>
+      <c r="E25" s="8"/>
       <c r="F25" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix UISPiritInfo not showing details when response arrived befores scene was loaded
</commit_message>
<xml_diff>
--- a/Dictionaries/store.xlsx
+++ b/Dictionaries/store.xlsx
@@ -53,12 +53,12 @@
     <t>silver5</t>
   </si>
   <si>
+    <t>bundle_hermeticCollection</t>
+  </si>
+  <si>
     <t>silver6</t>
   </si>
   <si>
-    <t>bundle_hermeticCollection</t>
-  </si>
-  <si>
     <t>consumable_alignmentBoosterSmaller</t>
   </si>
   <si>
@@ -83,163 +83,163 @@
     <t>shop_locked_wndg</t>
   </si>
   <si>
+    <t>cosmetic_f_S_HHO</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_HKO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_HLO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_SNOWQUEEN</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_LILYOV</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_MIDSUMMER</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_BARGHEST</t>
   </si>
   <si>
     <t>shop_locked_barg</t>
   </si>
   <si>
+    <t>cosmetic_f_S_THUNDERMOON</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_ECLIPSE</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_CATSIDHE</t>
   </si>
   <si>
+    <t>cosmetic_f_S_CORNMOON</t>
+  </si>
+  <si>
     <t>shop_locked_sidh</t>
   </si>
   <si>
     <t>cosmetic_f_PF_GRINDYLOW</t>
   </si>
   <si>
+    <t>cosmetic_f_S_BRNNGWTCH</t>
+  </si>
+  <si>
     <t>shop_locked_grdlw</t>
   </si>
   <si>
+    <t>cosmetic_f_S_CALYPSO</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_SENTINALOWL</t>
   </si>
   <si>
     <t>shop_locked_owl</t>
   </si>
   <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_HKO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_HHO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_HLO</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_DWO</t>
   </si>
   <si>
+    <t>cosmetic_m_S_JACKFROST</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_HDWO</t>
   </si>
   <si>
+    <t>cosmetic_m_S_MIDSUMMER</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_HBH</t>
   </si>
   <si>
     <t>cosmetic_f_HE_HBO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HHO</t>
+    <t>cosmetic_m_S_CORNMOON</t>
   </si>
   <si>
     <t>cosmetic_f_HE_HHO</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>cosmetic_f_HE_HNO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HKO</t>
+    <t>cosmetic_m_S_CALYPSO</t>
   </si>
   <si>
     <t>cosmetic_f_HE_CEH</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HLO</t>
-  </si>
-  <si>
     <t>cosmetic_f_HE_CES</t>
   </si>
   <si>
+    <t>cosmetic_m_S_FIREDANCER</t>
+  </si>
+  <si>
     <t>cosmetic_f_HE_FLOWER</t>
   </si>
   <si>
-    <t>cosmetic_f_S_SNOWQUEEN</t>
-  </si>
-  <si>
     <t>cosmetic_f_HE_BDH</t>
   </si>
   <si>
     <t>shop_locked_rrc</t>
   </si>
   <si>
-    <t>cosmetic_f_S_LILYOV</t>
+    <t>cosmetic_m_S_BRNNGWTCH</t>
   </si>
   <si>
     <t>cosmetic_f_HA_DWO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_MIDSUMMER</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_THUNDERMOON</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_ECLIPSE</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_CORNMOON</t>
+    <t>cosmetic_m_S_ECLIPSE</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_THUNDERMOON</t>
   </si>
   <si>
     <t>cosmetic_f_HA_FKFO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_BRNNGWTCH</t>
-  </si>
-  <si>
     <t>cosmetic_f_HA_KSO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_CALYPSO</t>
-  </si>
-  <si>
     <t>cosmetic_f_HA_CGH</t>
   </si>
   <si>
     <t>cosmetic_f_HA_PNY</t>
   </si>
   <si>
-    <t>_</t>
-  </si>
-  <si>
     <t>cosmetic_f_HA_SNWDRP</t>
   </si>
   <si>
-    <t>cosmetic_m_S_HKO</t>
-  </si>
-  <si>
     <t>cosmetic_f_HA_BUN</t>
   </si>
   <si>
-    <t>cosmetic_m_S_HHO</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_HLO</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_JACKFROST</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_MIDSUMMER</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_CORNMOON</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_CALYPSO</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_FIREDANCER</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_BRNNGWTCH</t>
-  </si>
-  <si>
     <t>cosmetic_f_HA_BRD</t>
   </si>
   <si>
     <t>cosmetic_f_HA_SPK</t>
   </si>
   <si>
-    <t>cosmetic_m_S_ECLIPSE</t>
-  </si>
-  <si>
     <t>cosmetic_f_HA_BZZ</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_THUNDERMOON</t>
   </si>
   <si>
     <t>cosmetic_f_HA_CURL</t>
@@ -981,20 +981,20 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1114,10 +1114,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>300.0</v>
       </c>
       <c r="E2" s="7"/>
@@ -1147,11 +1147,11 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>300.0</v>
       </c>
       <c r="E4" s="7"/>
@@ -1281,10 +1281,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>100.0</v>
       </c>
       <c r="E2" s="8"/>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>500.0</v>
       </c>
       <c r="E4" s="8"/>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>300.0</v>
       </c>
       <c r="E6" s="8"/>
@@ -1364,7 +1364,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
@@ -1388,7 +1388,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="8"/>
       <c r="F11" s="1"/>
     </row>
@@ -1404,7 +1404,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="8"/>
       <c r="F13" s="1"/>
     </row>
@@ -1460,10 +1460,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1627,10 +1627,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1654,13 +1654,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D3" s="13">
         <v>1000.0</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D4" s="13">
         <v>1000.0</v>
@@ -1690,13 +1690,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D5" s="13">
         <v>1000.0</v>
@@ -1708,13 +1708,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D6" s="13">
         <v>1000.0</v>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1852,11 +1852,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D16" s="13">
         <v>900.0</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -5161,16 +5161,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -5178,13 +5178,13 @@
         <v>8000.0</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -5192,13 +5192,13 @@
         <v>8000.0</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -5206,13 +5206,13 @@
         <v>8000.0</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -5220,13 +5220,13 @@
         <v>8000.0</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -5234,13 +5234,13 @@
         <v>8000.0</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -5248,13 +5248,13 @@
         <v>8000.0</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1">
         <v>1.5632496E12</v>
@@ -5264,13 +5264,13 @@
         <v>8000.0</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1">
         <v>1.56204E12</v>
@@ -5280,13 +5280,13 @@
         <v>8000.0</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1">
         <v>1.5658416E12</v>
@@ -5296,13 +5296,13 @@
         <v>8000.0</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1">
         <v>1.5667056E12</v>
@@ -5312,13 +5312,13 @@
         <v>8000.0</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1">
         <v>1.5649776E12</v>
@@ -5328,13 +5328,13 @@
         <v>8000.0</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -5342,13 +5342,13 @@
         <v>8000.0</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -5356,13 +5356,13 @@
         <v>8000.0</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -5370,13 +5370,13 @@
         <v>8000.0</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -5384,13 +5384,13 @@
         <v>8000.0</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -5398,13 +5398,13 @@
         <v>8000.0</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -5412,13 +5412,13 @@
         <v>8000.0</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -5426,13 +5426,13 @@
         <v>8000.0</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -5440,13 +5440,13 @@
         <v>8000.0</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -5454,13 +5454,13 @@
         <v>8000.0</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -5468,13 +5468,13 @@
         <v>8000.0</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -5482,13 +5482,13 @@
         <v>8000.0</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -5496,7 +5496,7 @@
         <v>8000.0</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F24" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update StatusEffect's status handling
</commit_message>
<xml_diff>
--- a/Dictionaries/store.xlsx
+++ b/Dictionaries/store.xlsx
@@ -35,6 +35,9 @@
     <t>silver1</t>
   </si>
   <si>
+    <t>bundle_abondiasBest</t>
+  </si>
+  <si>
     <t>silver2</t>
   </si>
   <si>
@@ -44,24 +47,24 @@
     <t>silver4</t>
   </si>
   <si>
+    <t>bundle_sapphosChoice</t>
+  </si>
+  <si>
     <t>silver5</t>
   </si>
   <si>
     <t>silver6</t>
   </si>
   <si>
+    <t>bundle_hermeticCollection</t>
+  </si>
+  <si>
     <t>consumable_alignmentBoosterSmaller</t>
   </si>
   <si>
-    <t>bundle_abondiasBest</t>
-  </si>
-  <si>
     <t>consumable_alignmentBoosterMedium</t>
   </si>
   <si>
-    <t>bundle_sapphosChoice</t>
-  </si>
-  <si>
     <t>consumable_alignmentBoosterGreater</t>
   </si>
   <si>
@@ -71,91 +74,103 @@
     <t>consumable_xpBoosterMedium</t>
   </si>
   <si>
-    <t>bundle_hermeticCollection</t>
-  </si>
-  <si>
     <t>consumable_xpBoosterGreater</t>
   </si>
   <si>
     <t>cosmetic_f_PF_WENDIGO</t>
   </si>
   <si>
+    <t>cosmetic_f_S_HHO</t>
+  </si>
+  <si>
     <t>shop_locked_wndg</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HHO</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
     <t>cosmetic_f_S_HKO</t>
   </si>
   <si>
+    <t>cosmetic_f_S_HLO</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_SNOWQUEEN</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_LILYOV</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_MIDSUMMER</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_THUNDERMOON</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_ECLIPSE</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_BARGHEST</t>
   </si>
   <si>
-    <t>cosmetic_f_S_HLO</t>
-  </si>
-  <si>
     <t>shop_locked_barg</t>
   </si>
   <si>
-    <t>cosmetic_f_S_SNOWQUEEN</t>
+    <t>cosmetic_f_S_CORNMOON</t>
+  </si>
+  <si>
+    <t>cosmetic_f_S_BRNNGWTCH</t>
   </si>
   <si>
     <t>cosmetic_f_PF_CATSIDHE</t>
   </si>
   <si>
-    <t>cosmetic_f_S_LILYOV</t>
-  </si>
-  <si>
     <t>shop_locked_sidh</t>
   </si>
   <si>
+    <t>cosmetic_f_S_CALYPSO</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_GRINDYLOW</t>
   </si>
   <si>
-    <t>cosmetic_f_S_MIDSUMMER</t>
-  </si>
-  <si>
     <t>shop_locked_grdlw</t>
   </si>
   <si>
+    <t>_</t>
+  </si>
+  <si>
     <t>cosmetic_f_PF_SENTINALOWL</t>
   </si>
   <si>
-    <t>cosmetic_f_S_THUNDERMOON</t>
-  </si>
-  <si>
     <t>shop_locked_owl</t>
   </si>
   <si>
-    <t>cosmetic_f_S_ECLIPSE</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_CORNMOON</t>
-  </si>
-  <si>
-    <t>cosmetic_f_S_BRNNGWTCH</t>
+    <t>cosmetic_m_S_HKO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_HHO</t>
+  </si>
+  <si>
+    <t>cosmetic_m_S_HLO</t>
   </si>
   <si>
     <t>cosmetic_f_HE_DWO</t>
   </si>
   <si>
-    <t>cosmetic_f_S_CALYPSO</t>
+    <t>cosmetic_m_S_JACKFROST</t>
   </si>
   <si>
     <t>cosmetic_f_HE_HDWO</t>
   </si>
   <si>
-    <t>_</t>
+    <t>cosmetic_m_S_MIDSUMMER</t>
   </si>
   <si>
     <t>cosmetic_f_HE_HBH</t>
   </si>
   <si>
-    <t>cosmetic_m_S_HKO</t>
+    <t>cosmetic_m_S_CORNMOON</t>
   </si>
   <si>
     <t>cosmetic_f_HE_HBO</t>
@@ -164,31 +179,31 @@
     <t>cosmetic_f_HE_HHO</t>
   </si>
   <si>
-    <t>cosmetic_m_S_HHO</t>
+    <t>cosmetic_m_S_CALYPSO</t>
   </si>
   <si>
     <t>cosmetic_f_HE_HNO</t>
   </si>
   <si>
-    <t>cosmetic_m_S_HLO</t>
+    <t>cosmetic_m_S_FIREDANCER</t>
   </si>
   <si>
     <t>cosmetic_f_HE_CEH</t>
   </si>
   <si>
-    <t>cosmetic_m_S_JACKFROST</t>
+    <t>cosmetic_m_S_BRNNGWTCH</t>
   </si>
   <si>
     <t>cosmetic_f_HE_CES</t>
   </si>
   <si>
-    <t>cosmetic_m_S_MIDSUMMER</t>
+    <t>cosmetic_m_S_ECLIPSE</t>
   </si>
   <si>
     <t>cosmetic_f_HE_FLOWER</t>
   </si>
   <si>
-    <t>cosmetic_m_S_CORNMOON</t>
+    <t>cosmetic_m_S_THUNDERMOON</t>
   </si>
   <si>
     <t>cosmetic_f_HE_BDH</t>
@@ -197,22 +212,7 @@
     <t>shop_locked_rrc</t>
   </si>
   <si>
-    <t>cosmetic_m_S_CALYPSO</t>
-  </si>
-  <si>
     <t>cosmetic_f_HA_DWO</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_FIREDANCER</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_BRNNGWTCH</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_ECLIPSE</t>
-  </si>
-  <si>
-    <t>cosmetic_m_S_THUNDERMOON</t>
   </si>
   <si>
     <t>cosmetic_f_HA_FKFO</t>
@@ -981,20 +981,20 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1114,16 +1114,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1162,7 +1162,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
@@ -1170,7 +1170,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
@@ -1178,7 +1178,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1186,7 +1186,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1194,7 +1194,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1202,7 +1202,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1210,7 +1210,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1218,7 +1218,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1226,7 +1226,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1234,7 +1234,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1281,71 +1281,71 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="7">
         <v>100.0</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="9">
         <v>300.0</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="7">
         <v>500.0</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="9">
         <v>100.0</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="7">
         <v>300.0</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
@@ -1357,7 +1357,7 @@
       <c r="D7" s="9">
         <v>500.0</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1365,7 +1365,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1373,7 +1373,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1381,15 +1381,15 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1397,15 +1397,15 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1413,7 +1413,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1460,10 +1460,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1474,57 +1474,57 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -1532,7 +1532,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -1540,7 +1540,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -1548,7 +1548,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
@@ -1556,7 +1556,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
@@ -1564,7 +1564,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -1572,7 +1572,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -1580,7 +1580,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="1"/>
     </row>
   </sheetData>
@@ -1627,10 +1627,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
         <v>1.56168E12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="13">
         <v>1000.0</v>
@@ -1654,13 +1654,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D3" s="13">
         <v>1000.0</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D4" s="13">
         <v>1000.0</v>
@@ -1690,13 +1690,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D5" s="13">
         <v>1000.0</v>
@@ -1708,13 +1708,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
         <v>1.56168E12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D6" s="13">
         <v>1000.0</v>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1852,11 +1852,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D16" s="13">
         <v>900.0</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2715,7 +2715,7 @@
         <v>126</v>
       </c>
       <c r="D77" s="1"/>
-      <c r="E77" s="4"/>
+      <c r="E77" s="6"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78">
@@ -2727,7 +2727,7 @@
         <v>126</v>
       </c>
       <c r="D78" s="1"/>
-      <c r="E78" s="4"/>
+      <c r="E78" s="6"/>
       <c r="F78" s="1"/>
     </row>
     <row r="79">
@@ -2739,7 +2739,7 @@
         <v>126</v>
       </c>
       <c r="D79" s="1"/>
-      <c r="E79" s="4"/>
+      <c r="E79" s="6"/>
       <c r="F79" s="1"/>
     </row>
     <row r="80">
@@ -3420,12 +3420,12 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
-      <c r="E125" s="4"/>
+      <c r="E125" s="6"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126">
@@ -3561,7 +3561,7 @@
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
-      <c r="E135" s="4"/>
+      <c r="E135" s="6"/>
       <c r="F135" s="1"/>
     </row>
     <row r="136">
@@ -4549,7 +4549,7 @@
         <v>259</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D206" s="13">
         <v>1000.0</v>
@@ -4564,7 +4564,7 @@
         <v>260</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D207" s="13">
         <v>1000.0</v>
@@ -4605,7 +4605,7 @@
         <v>263</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D210" s="13">
         <v>1000.0</v>
@@ -4620,7 +4620,7 @@
         <v>264</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D211" s="13">
         <v>1000.0</v>
@@ -4635,7 +4635,7 @@
         <v>265</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D212" s="13">
         <v>1000.0</v>
@@ -4790,7 +4790,7 @@
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
-      <c r="E223" s="4"/>
+      <c r="E223" s="6"/>
       <c r="F223" s="1"/>
     </row>
     <row r="224">
@@ -4814,7 +4814,7 @@
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
-      <c r="E225" s="4"/>
+      <c r="E225" s="6"/>
       <c r="F225" s="1"/>
     </row>
     <row r="226">
@@ -4852,7 +4852,7 @@
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
-      <c r="E228" s="4"/>
+      <c r="E228" s="6"/>
       <c r="F228" s="1"/>
     </row>
     <row r="229">
@@ -5114,7 +5114,7 @@
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
-      <c r="E247" s="4"/>
+      <c r="E247" s="6"/>
       <c r="F247" s="1"/>
     </row>
     <row r="248">
@@ -5122,7 +5122,7 @@
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
-      <c r="E248" s="4"/>
+      <c r="E248" s="6"/>
       <c r="F248" s="1"/>
     </row>
   </sheetData>
@@ -5164,23 +5164,23 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="1"/>
@@ -5194,70 +5194,70 @@
       <c r="D3" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
         <v>1.5632496E12</v>
@@ -5266,14 +5266,14 @@
       <c r="D8" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>1.56204E12</v>
@@ -5282,14 +5282,14 @@
       <c r="D9" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1">
         <v>1.5658416E12</v>
@@ -5298,14 +5298,14 @@
       <c r="D10" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1">
         <v>1.5667056E12</v>
@@ -5314,14 +5314,14 @@
       <c r="D11" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1">
         <v>1.5649776E12</v>
@@ -5330,175 +5330,175 @@
       <c r="D12" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
         <v>8000.0</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F24" s="1"/>
@@ -5508,7 +5508,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="6"/>
       <c r="F25" s="1"/>
     </row>
   </sheetData>

</xml_diff>